<commit_message>
updated vector list, collection done
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -142,7 +142,7 @@
   </si>
   <si>
     <t>From management interfaces 
-(api's &amp; webinterfaces, cloud &amp; k8s)</t>
+(api's &amp; webinterfaces of cloud &amp; k8s)</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added screenshot dump + notes risk assessment session MPO
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vector Overview" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="120">
   <si>
     <t>Attack Vectors Overview</t>
   </si>
@@ -159,15 +159,6 @@
     <t>out of scope</t>
   </si>
   <si>
-    <t>cloud admin (1)</t>
-  </si>
-  <si>
-    <t>read access (4)</t>
-  </si>
-  <si>
-    <t>any (5)</t>
-  </si>
-  <si>
     <t>Quellen:</t>
   </si>
   <si>
@@ -181,12 +172,6 @@
   </si>
   <si>
     <t>Resulting Risk</t>
-  </si>
-  <si>
-    <t>cluster/system user (3)</t>
-  </si>
-  <si>
-    <t>cluster/system admin (2)</t>
   </si>
   <si>
     <t>1 (cloud)
@@ -350,6 +335,78 @@
   </si>
   <si>
     <t xml:space="preserve"> @LGR?</t>
+  </si>
+  <si>
+    <t>modify this container</t>
+  </si>
+  <si>
+    <t>modify running container</t>
+  </si>
+  <si>
+    <t>modify (other) running container</t>
+  </si>
+  <si>
+    <t>gather secrets, passwords, tokens, keys, …</t>
+  </si>
+  <si>
+    <t>gather source code</t>
+  </si>
+  <si>
+    <t>gather setup-information (HW/SW, versions, dockerfiles, config), mail-adresses, usernames, …</t>
+  </si>
+  <si>
+    <t>unauthenticated (4)</t>
+  </si>
+  <si>
+    <t>read only (3)</t>
+  </si>
+  <si>
+    <t>cluster/system user (2)</t>
+  </si>
+  <si>
+    <t>cluster/system admin (1)</t>
+  </si>
+  <si>
+    <t>cloud/infrastructure admin (0)</t>
+  </si>
+  <si>
+    <t>Access to dashboard</t>
+  </si>
+  <si>
+    <t>Read access</t>
+  </si>
+  <si>
+    <t>User access</t>
+  </si>
+  <si>
+    <t>Admin access???</t>
+  </si>
+  <si>
+    <t>Critical (4)</t>
+  </si>
+  <si>
+    <t>EW</t>
+  </si>
+  <si>
+    <t>Imp</t>
+  </si>
+  <si>
+    <t>detect</t>
+  </si>
+  <si>
+    <t>expl</t>
+  </si>
+  <si>
+    <t>vantage</t>
+  </si>
+  <si>
+    <t>access level</t>
+  </si>
+  <si>
+    <t>comprise user</t>
+  </si>
+  <si>
+    <t>compromise admin</t>
   </si>
 </sst>
 </file>
@@ -646,7 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -792,6 +849,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1082,7 +1145,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,6 +1168,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
@@ -1417,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L66"/>
+  <dimension ref="A2:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1509,7 @@
     <col min="2" max="2" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.5703125" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -1437,28 +1517,28 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H2" s="60" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1502,7 +1582,7 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="62" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D5" s="64">
         <v>3</v>
@@ -1520,24 +1600,24 @@
     </row>
     <row r="6" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="62" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E6" s="65" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F6" s="55" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="L6" s="51">
         <v>5</v>
@@ -1549,13 +1629,13 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="62" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E7" s="65" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F7" s="55" t="e">
         <f t="shared" si="0"/>
@@ -1569,12 +1649,14 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="23">
+        <v>4</v>
+      </c>
       <c r="C8" s="63" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E8" s="23">
         <v>3</v>
@@ -1584,7 +1666,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L8" s="51">
         <v>1</v>
@@ -1595,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
@@ -1604,7 +1686,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="65" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F9" s="55" t="e">
         <f t="shared" si="0"/>
@@ -1619,7 +1701,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C10" s="10">
         <v>3</v>
@@ -1673,104 +1755,85 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="B14" s="23">
-        <v>3</v>
-      </c>
-      <c r="C14" s="10">
-        <v>3</v>
-      </c>
-      <c r="D14" s="10">
-        <v>3</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="55" t="e">
-        <f t="shared" ref="F14" si="1">ROUND(((L14+C14+D14)/3*E14), 2)</f>
-        <v>#VALUE!</v>
+        <v>2</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="66">
+        <v>3</v>
+      </c>
+      <c r="F14" s="55">
+        <f t="shared" ref="F14:F16" si="1">ROUND(((L14+C14+D14)/3*E14), 2)</f>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L14" s="51"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="57"/>
-      <c r="L15" s="52"/>
+      <c r="A15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="23">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="66">
+        <v>3</v>
+      </c>
+      <c r="F15" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="51"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="57"/>
+      <c r="L17" s="52"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="10">
-        <v>3</v>
-      </c>
-      <c r="D16" s="64">
-        <v>2</v>
-      </c>
-      <c r="E16" s="23">
-        <v>3</v>
-      </c>
-      <c r="F16" s="55">
-        <f t="shared" ref="F16:F20" si="2">ROUND(((L16+C16+D16)/3*E16), 2)</f>
+      <c r="B18" s="23"/>
+      <c r="C18" s="10">
+        <v>3</v>
+      </c>
+      <c r="D18" s="64">
+        <v>2</v>
+      </c>
+      <c r="E18" s="23">
+        <v>3</v>
+      </c>
+      <c r="F18" s="55">
+        <f t="shared" ref="F18:F22" si="2">ROUND(((L18+C18+D18)/3*E18), 2)</f>
         <v>10</v>
-      </c>
-      <c r="L16" s="51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="64">
-        <v>2</v>
-      </c>
-      <c r="E17" s="23">
-        <v>3</v>
-      </c>
-      <c r="F17" s="55" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L17" s="51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="55" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" t="s">
-        <v>78</v>
       </c>
       <c r="L18" s="51">
         <v>5</v>
@@ -1778,16 +1841,18 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="D19" s="64">
+        <v>2</v>
+      </c>
+      <c r="E19" s="23">
+        <v>3</v>
+      </c>
       <c r="F19" s="55" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
@@ -1797,182 +1862,180 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
+      <c r="A20" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B20" s="23"/>
-      <c r="C20" s="63" t="s">
-        <v>92</v>
+      <c r="C20" s="62" t="s">
+        <v>89</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="23">
-        <v>3</v>
+        <v>94</v>
+      </c>
+      <c r="E20" s="65" t="s">
+        <v>86</v>
       </c>
       <c r="F20" s="55" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L20" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L21" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="23">
+        <v>3</v>
+      </c>
+      <c r="F22" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="51">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="58"/>
-      <c r="L21" s="50"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B23" s="47"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="58"/>
+      <c r="L23" s="50"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="58"/>
-      <c r="L22" s="50"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B24" s="47"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="58"/>
+      <c r="L24" s="50"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="10">
-        <v>3</v>
-      </c>
-      <c r="D23" s="10">
-        <v>3</v>
-      </c>
-      <c r="E23" s="65">
+      <c r="B25" s="23"/>
+      <c r="C25" s="10">
+        <v>3</v>
+      </c>
+      <c r="D25" s="10">
+        <v>3</v>
+      </c>
+      <c r="E25" s="65">
         <v>1</v>
       </c>
-      <c r="F23" s="55">
-        <f t="shared" ref="F23:F24" si="3">ROUND(((L23+C23+D23)/3*E23), 2)</f>
-        <v>2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L23" s="51"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="F25" s="55">
+        <f t="shared" ref="F25:F26" si="3">ROUND(((L25+C25+D25)/3*E25), 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="L25" s="51"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="55" t="e">
+      <c r="B26" s="23"/>
+      <c r="C26" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="23"/>
+      <c r="F26" s="55" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H24" t="s">
-        <v>77</v>
-      </c>
-      <c r="L24" s="51"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="H26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" s="51"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="58"/>
-      <c r="L25" s="50"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="57"/>
-      <c r="L26" s="52"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="58"/>
+      <c r="L27" s="50"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="57"/>
+      <c r="L28" s="52"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="10">
-        <v>3</v>
-      </c>
-      <c r="D27" s="10">
-        <v>2</v>
-      </c>
-      <c r="E27" s="23">
-        <v>3</v>
-      </c>
-      <c r="F27" s="55">
-        <f t="shared" ref="F27:F37" si="4">ROUND(((L27+C27+D27)/3*E27), 2)</f>
+      <c r="B29" s="23"/>
+      <c r="C29" s="10">
+        <v>3</v>
+      </c>
+      <c r="D29" s="10">
+        <v>2</v>
+      </c>
+      <c r="E29" s="23">
+        <v>3</v>
+      </c>
+      <c r="F29" s="55">
+        <f t="shared" ref="F29:F40" si="4">ROUND(((L29+C29+D29)/3*E29), 2)</f>
         <v>8</v>
-      </c>
-      <c r="L27" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="10">
-        <v>2</v>
-      </c>
-      <c r="E28" s="23">
-        <v>3</v>
-      </c>
-      <c r="F28" s="55" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L28" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="63" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="55" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H29" t="s">
-        <v>78</v>
       </c>
       <c r="L29" s="51">
         <v>3</v>
@@ -1980,16 +2043,18 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="D30" s="10">
+        <v>2</v>
+      </c>
+      <c r="E30" s="23">
+        <v>3</v>
+      </c>
       <c r="F30" s="55" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
@@ -1998,26 +2063,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B31" s="23"/>
-      <c r="C31" s="63" t="s">
-        <v>92</v>
+      <c r="C31" s="62" t="s">
+        <v>89</v>
       </c>
       <c r="D31" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="23">
-        <v>3</v>
+        <v>91</v>
+      </c>
+      <c r="E31" s="65" t="s">
+        <v>86</v>
       </c>
       <c r="F31" s="55" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="H31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L31" s="51">
         <v>3</v>
@@ -2025,108 +2090,109 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="10">
-        <v>2</v>
-      </c>
-      <c r="E32" s="23">
-        <v>3</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D32" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="23"/>
       <c r="F32" s="55" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H32" t="s">
-        <v>80</v>
-      </c>
       <c r="L32" s="51">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="23">
+        <v>3</v>
+      </c>
+      <c r="F33" s="55" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="10">
+        <v>2</v>
+      </c>
+      <c r="E34" s="23">
+        <v>3</v>
+      </c>
+      <c r="F34" s="55" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H34" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="10">
+      <c r="B35" s="23"/>
+      <c r="C35" s="10">
         <v>1</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D35" s="10">
         <v>1</v>
       </c>
-      <c r="E33" s="23">
-        <v>3</v>
-      </c>
-      <c r="F33" s="55">
+      <c r="E35" s="23">
+        <v>3</v>
+      </c>
+      <c r="F35" s="55">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="L33" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="10">
-        <v>2</v>
-      </c>
-      <c r="E34" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="55" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L34" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="10">
-        <v>3</v>
-      </c>
-      <c r="D35" s="10">
-        <v>2</v>
-      </c>
-      <c r="E35" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="55" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="L35" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B36" s="23"/>
-      <c r="C36" s="10">
-        <v>3</v>
+      <c r="C36" s="62" t="s">
+        <v>92</v>
       </c>
       <c r="D36" s="10">
         <v>2</v>
       </c>
       <c r="E36" s="65" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F36" s="55" t="e">
         <f t="shared" si="4"/>
@@ -2138,51 +2204,71 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B37" s="23"/>
-      <c r="C37" s="10">
-        <v>3</v>
-      </c>
-      <c r="D37" s="10">
-        <v>2</v>
+      <c r="C37" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="62" t="s">
+        <v>89</v>
       </c>
       <c r="E37" s="65" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F37" s="55" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L37" s="51">
-        <v>3</v>
-      </c>
+      <c r="L37" s="51"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="58"/>
-      <c r="L38" s="50"/>
+      <c r="A38" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="10">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10">
+        <v>2</v>
+      </c>
+      <c r="E38" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="55" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L38" s="51">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="58"/>
-      <c r="L39" s="50"/>
+      <c r="A39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="10">
+        <v>3</v>
+      </c>
+      <c r="D39" s="10">
+        <v>2</v>
+      </c>
+      <c r="E39" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="55" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L39" s="51">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="10">
@@ -2192,179 +2278,157 @@
         <v>2</v>
       </c>
       <c r="E40" s="65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F40" s="55" t="e">
-        <f t="shared" ref="F40:F43" si="5">ROUND(((L40+C40+D40)/3*E40), 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H40" t="s">
-        <v>76</v>
-      </c>
-      <c r="L40" s="51"/>
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L40" s="51">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41" s="55" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H41" t="s">
-        <v>77</v>
-      </c>
-      <c r="L41" s="51"/>
+      <c r="A41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="47"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="58"/>
+      <c r="L41" s="50"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="10">
-        <v>1</v>
-      </c>
-      <c r="E42" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" s="55" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H42" t="s">
-        <v>87</v>
-      </c>
-      <c r="L42" s="51">
-        <v>3</v>
-      </c>
+      <c r="A42" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="47"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="58"/>
+      <c r="L42" s="50"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="10">
         <v>3</v>
       </c>
-      <c r="D43" s="62" t="s">
-        <v>98</v>
+      <c r="D43" s="10">
+        <v>2</v>
       </c>
       <c r="E43" s="65" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F43" s="55" t="e">
+        <f t="shared" ref="F43:F46" si="5">ROUND(((L43+C43+D43)/3*E43), 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H43" t="s">
+        <v>71</v>
+      </c>
+      <c r="L43" s="51"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="55" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H43" t="s">
-        <v>88</v>
-      </c>
-      <c r="L43" s="51"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="44"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="58"/>
-      <c r="L44" s="50"/>
+      <c r="H44" t="s">
+        <v>72</v>
+      </c>
+      <c r="L44" s="51"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="57"/>
-      <c r="L45" s="52"/>
+      <c r="A45" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="10">
+        <v>1</v>
+      </c>
+      <c r="E45" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="55" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H45" t="s">
+        <v>82</v>
+      </c>
+      <c r="L45" s="51">
+        <v>3</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B46" s="23"/>
       <c r="C46" s="10">
         <v>3</v>
       </c>
-      <c r="D46" s="10">
-        <v>1</v>
+      <c r="D46" s="62" t="s">
+        <v>93</v>
       </c>
       <c r="E46" s="65" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F46" s="55" t="e">
-        <f t="shared" ref="F46:F54" si="6">ROUND(((L46+C46+D46)/3*E46), 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L46" s="51">
-        <v>2</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H46" t="s">
+        <v>83</v>
+      </c>
+      <c r="L46" s="51"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="10">
-        <v>3</v>
-      </c>
-      <c r="D47" s="10">
-        <v>1</v>
-      </c>
-      <c r="E47" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F47" s="55" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L47" s="51">
-        <v>3</v>
-      </c>
+      <c r="A47" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="44"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="58"/>
+      <c r="L47" s="50"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="10">
-        <v>1</v>
-      </c>
-      <c r="E48" s="23">
-        <v>3</v>
-      </c>
-      <c r="F48" s="55" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L48" s="51">
-        <v>2</v>
-      </c>
+      <c r="A48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="45"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="57"/>
+      <c r="L48" s="52"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B49" s="23"/>
       <c r="C49" s="10">
@@ -2373,23 +2437,20 @@
       <c r="D49" s="10">
         <v>1</v>
       </c>
-      <c r="E49" s="23">
-        <v>1</v>
-      </c>
-      <c r="F49" s="55">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="H49" t="s">
-        <v>82</v>
+      <c r="E49" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="55" t="e">
+        <f t="shared" ref="F49:F57" si="6">ROUND(((L49+C49+D49)/3*E49), 2)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="L49" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>24</v>
+      <c r="A50" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B50" s="23"/>
       <c r="C50" s="10">
@@ -2399,32 +2460,29 @@
         <v>1</v>
       </c>
       <c r="E50" s="65" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F50" s="55" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H50" t="s">
-        <v>85</v>
-      </c>
       <c r="L50" s="51">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B51" s="23"/>
-      <c r="C51" s="10">
-        <v>3</v>
+      <c r="C51" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="D51" s="10">
         <v>1</v>
       </c>
-      <c r="E51" s="65" t="s">
-        <v>94</v>
+      <c r="E51" s="23">
+        <v>3</v>
       </c>
       <c r="F51" s="55" t="e">
         <f t="shared" si="6"/>
@@ -2436,52 +2494,57 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B52" s="23"/>
-      <c r="C52" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="F52" s="55" t="e">
+      <c r="C52" s="10">
+        <v>3</v>
+      </c>
+      <c r="D52" s="10">
+        <v>1</v>
+      </c>
+      <c r="E52" s="23">
+        <v>1</v>
+      </c>
+      <c r="F52" s="55">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
       <c r="H52" t="s">
         <v>77</v>
       </c>
-      <c r="L52" s="51"/>
+      <c r="L52" s="51">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B53" s="23"/>
-      <c r="C53" s="62" t="s">
-        <v>98</v>
+      <c r="C53" s="10">
+        <v>3</v>
       </c>
       <c r="D53" s="10">
         <v>1</v>
       </c>
       <c r="E53" s="65" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F53" s="55" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
+      <c r="H53" t="s">
+        <v>80</v>
+      </c>
       <c r="L53" s="51">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B54" s="23"/>
       <c r="C54" s="10">
@@ -2490,201 +2553,194 @@
       <c r="D54" s="10">
         <v>1</v>
       </c>
-      <c r="E54" s="23">
-        <v>3</v>
-      </c>
-      <c r="F54" s="55">
+      <c r="E54" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" s="55" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L54" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" s="55" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H55" t="s">
+        <v>72</v>
+      </c>
+      <c r="L55" s="51"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="10">
+        <v>1</v>
+      </c>
+      <c r="E56" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="55" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L56" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" s="23"/>
+      <c r="C57" s="10">
+        <v>3</v>
+      </c>
+      <c r="D57" s="10">
+        <v>1</v>
+      </c>
+      <c r="E57" s="23">
+        <v>3</v>
+      </c>
+      <c r="F57" s="55">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="H54" t="s">
-        <v>83</v>
-      </c>
-      <c r="L54" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="H57" t="s">
+        <v>78</v>
+      </c>
+      <c r="L57" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="47"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="58"/>
-      <c r="L55" s="50"/>
-    </row>
-    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="B58" s="47"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="58"/>
+      <c r="L58" s="50"/>
+    </row>
+    <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="57"/>
-      <c r="L56" s="52"/>
-    </row>
-    <row r="57" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="B59" s="45"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="57"/>
+      <c r="L59" s="52"/>
+    </row>
+    <row r="60" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D57" s="63" t="s">
+      <c r="B60" s="23"/>
+      <c r="C60" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="E57" s="23">
-        <v>3</v>
-      </c>
-      <c r="F57" s="55" t="e">
-        <f t="shared" ref="F57:F65" si="7">ROUND(((L57+C57+D57)/3*E57), 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H57" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="L57" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="D60" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60" s="23">
+        <v>3</v>
+      </c>
+      <c r="F60" s="55" t="e">
+        <f t="shared" ref="F60:F68" si="7">ROUND(((L60+C60+D60)/3*E60), 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H60" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="L60" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="10">
-        <v>3</v>
-      </c>
-      <c r="D58" s="10">
-        <v>2</v>
-      </c>
-      <c r="E58" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F58" s="55" t="e">
+      <c r="B61" s="23"/>
+      <c r="C61" s="10">
+        <v>3</v>
+      </c>
+      <c r="D61" s="10">
+        <v>2</v>
+      </c>
+      <c r="E61" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61" s="55" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H58" t="s">
-        <v>84</v>
-      </c>
-      <c r="L58" s="51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="H61" t="s">
+        <v>79</v>
+      </c>
+      <c r="L61" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="10">
-        <v>3</v>
-      </c>
-      <c r="D59" s="10">
-        <v>2</v>
-      </c>
-      <c r="E59" s="23">
-        <v>3</v>
-      </c>
-      <c r="F59" s="55">
+      <c r="B62" s="23"/>
+      <c r="C62" s="10">
+        <v>3</v>
+      </c>
+      <c r="D62" s="10">
+        <v>2</v>
+      </c>
+      <c r="E62" s="23">
+        <v>3</v>
+      </c>
+      <c r="F62" s="55">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="L59" s="51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="10">
-        <v>2</v>
-      </c>
-      <c r="E60" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="F60" s="55" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H60" t="s">
-        <v>82</v>
-      </c>
-      <c r="L60" s="51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="23">
-        <v>3</v>
-      </c>
-      <c r="C61" s="10">
-        <v>3</v>
-      </c>
-      <c r="D61" s="10">
-        <v>2</v>
-      </c>
-      <c r="E61" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F61" s="55" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H61" t="s">
-        <v>81</v>
-      </c>
-      <c r="L61" s="51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="10">
-        <v>3</v>
-      </c>
-      <c r="D62" s="10">
-        <v>3</v>
-      </c>
-      <c r="E62" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="F62" s="55" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="L62" s="51">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D63" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" s="65" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="D63" s="10">
+        <v>2</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>89</v>
       </c>
       <c r="F63" s="55" t="e">
         <f t="shared" si="7"/>
@@ -2693,65 +2749,195 @@
       <c r="H63" t="s">
         <v>77</v>
       </c>
-      <c r="L63" s="51"/>
+      <c r="L63" s="51">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="63" t="s">
-        <v>100</v>
+        <v>26</v>
+      </c>
+      <c r="B64" s="23">
+        <v>3</v>
+      </c>
+      <c r="C64" s="10">
+        <v>3</v>
       </c>
       <c r="D64" s="10">
         <v>2</v>
       </c>
       <c r="E64" s="65" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F64" s="55" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
+      <c r="H64" t="s">
+        <v>76</v>
+      </c>
       <c r="L64" s="51">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B65" s="23"/>
-      <c r="C65" s="62" t="s">
-        <v>97</v>
+      <c r="C65" s="10">
+        <v>3</v>
       </c>
       <c r="D65" s="10">
-        <v>1</v>
-      </c>
-      <c r="E65" s="23">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="E65" s="65" t="s">
+        <v>89</v>
       </c>
       <c r="F65" s="55" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H65" t="s">
-        <v>84</v>
-      </c>
       <c r="L65" s="51">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E66" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="F66" s="55" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H66" t="s">
+        <v>72</v>
+      </c>
+      <c r="L66" s="51"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="23"/>
+      <c r="C67" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D67" s="10">
+        <v>2</v>
+      </c>
+      <c r="E67" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="F67" s="55" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L67" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="23"/>
+      <c r="C68" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" s="10">
+        <v>1</v>
+      </c>
+      <c r="E68" s="23">
+        <v>3</v>
+      </c>
+      <c r="F68" s="55" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H68" t="s">
+        <v>79</v>
+      </c>
+      <c r="L68" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="44"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="59"/>
-      <c r="L66" s="53"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="59"/>
+      <c r="L69" s="53"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>107</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>108</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2761,10 +2947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,169 +2963,270 @@
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
       <c r="H2" s="41" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>37</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="E4" s="26"/>
       <c r="H4" s="21" t="s">
         <v>38</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>58</v>
+      <c r="B5" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>54</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E5" s="26"/>
       <c r="H5" s="22"/>
       <c r="I5" s="35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="26"/>
       <c r="H6" s="22"/>
       <c r="I6" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="26"/>
+        <v>60</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="C7" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" s="26"/>
       <c r="H7" s="22"/>
       <c r="I7" s="35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B8" s="27"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="26"/>
+      <c r="C8" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>47</v>
+      </c>
       <c r="E8" s="26"/>
       <c r="H8" s="36"/>
       <c r="I8" s="37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="24" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="26"/>
       <c r="E9" s="28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="27"/>
       <c r="E10" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f>(G13+H13+I13+J13)/4</f>
+        <v>2.75</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <f>L13*K13</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f>(G14+H14+I14+J14)/4</f>
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <f>L14*K14</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added simplified risk estimation to sheet
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vector Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Vector Details" sheetId="3" r:id="rId2"/>
-    <sheet name="Risk assessment formula" sheetId="2" r:id="rId3"/>
+    <sheet name="Vectors simple" sheetId="4" r:id="rId2"/>
+    <sheet name="Vector Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ISFOXAutomaticLabelingDisabled" hidden="1">TRUE</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="158">
   <si>
     <t>Attack Vectors Overview</t>
   </si>
@@ -168,9 +169,6 @@
     <t>Vector</t>
   </si>
   <si>
-    <t>Required Access Level</t>
-  </si>
-  <si>
     <t>Resulting Risk</t>
   </si>
   <si>
@@ -184,9 +182,6 @@
     <t>Exploitability</t>
   </si>
   <si>
-    <t>None (0)</t>
-  </si>
-  <si>
     <t>Low (1)</t>
   </si>
   <si>
@@ -208,40 +203,16 @@
     <t>Easy (3)</t>
   </si>
   <si>
-    <t>Excluded b/c part of 'Exploitability'!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prevalence </t>
   </si>
   <si>
-    <t>Very widespread (4)</t>
-  </si>
-  <si>
-    <t>Widespread (3)</t>
-  </si>
-  <si>
-    <t>Common (2)</t>
-  </si>
-  <si>
-    <t>Uncommon (1)</t>
-  </si>
-  <si>
-    <t>Application specific (0)</t>
-  </si>
-  <si>
     <t>Excluded (generic view)</t>
   </si>
   <si>
     <t>Risk</t>
   </si>
   <si>
-    <t xml:space="preserve">^Probability = (Prevalence + Detectability + Exploitability)/3 </t>
-  </si>
-  <si>
     <t>^Risk = ROUND(Probability * Impact)</t>
-  </si>
-  <si>
-    <t>Range: 0,00 - 3,33 (  0-1,33 Low; 1,66-2,33 Medium; 2,66-3,33  High )</t>
   </si>
   <si>
     <t>HvS-Interna</t>
@@ -407,6 +378,150 @@
   </si>
   <si>
     <t>compromise admin</t>
+  </si>
+  <si>
+    <t>None/Theoretical (0)</t>
+  </si>
+  <si>
+    <t>Vantage Point</t>
+  </si>
+  <si>
+    <t>Public www (4)</t>
+  </si>
+  <si>
+    <t>Container (2)</t>
+  </si>
+  <si>
+    <t>Company network (3)</t>
+  </si>
+  <si>
+    <t>Node/Mgmt Interface (1)</t>
+  </si>
+  <si>
+    <t>Physical Access (0)</t>
+  </si>
+  <si>
+    <t>Required Access Level (RAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^Probability = (RAL + Vantage + Detectability + Exploitability)/4 </t>
+  </si>
+  <si>
+    <t>Unpublished 0-Days = Theoretical</t>
+  </si>
+  <si>
+    <t>Multi-tenant pwning = Severe</t>
+  </si>
+  <si>
+    <t>Intermediate Step = Low</t>
+  </si>
+  <si>
+    <t>Single-Tenant pwning = Moderate</t>
+  </si>
+  <si>
+    <t>Range: 0,25 - 3,5 (  0,25-1,25 Low; 1,5-2,25 Medium; 2,5-3,5  High )</t>
+  </si>
+  <si>
+    <t>Rating: see below</t>
+  </si>
+  <si>
+    <t>Example stuff:</t>
+  </si>
+  <si>
+    <t>Vector risk assessment, simplified</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Resulting risk</t>
+  </si>
+  <si>
+    <t>Change configuration through dashboard</t>
+  </si>
+  <si>
+    <t>Reconaissance through dashboard</t>
+  </si>
+  <si>
+    <t>OpenShift Container Platform On-Premise</t>
+  </si>
+  <si>
+    <t>Azure Kubernetes Cluster Cloud-Hosted</t>
+  </si>
+  <si>
+    <t>Probability:</t>
+  </si>
+  <si>
+    <t>High (3)</t>
+  </si>
+  <si>
+    <t>Medium (2)</t>
+  </si>
+  <si>
+    <t>Read confidentials through dashboard</t>
+  </si>
+  <si>
+    <t>Multi-tenant pwning = Critical</t>
+  </si>
+  <si>
+    <t>Single-Tenant pwning = Severe</t>
+  </si>
+  <si>
+    <t>CIA violated = Moderate</t>
+  </si>
+  <si>
+    <t>Reconaissance through k8s-apiserver, kubelets</t>
+  </si>
+  <si>
+    <t>Read confidentials through k8s-apiserver, kubelets</t>
+  </si>
+  <si>
+    <t>Change configuration through k8s-apiserver, kubelets</t>
+  </si>
+  <si>
+    <t>Reconaissance through cloud provider mgmt console / API</t>
+  </si>
+  <si>
+    <t>Read confidentials through cloud provider mgmt console / API</t>
+  </si>
+  <si>
+    <t>Change configuration through cloud provider mgmt console / API</t>
+  </si>
+  <si>
+    <t>supply compromised k8s configuration</t>
+  </si>
+  <si>
+    <t>Compromise application components</t>
+  </si>
+  <si>
+    <t>Compromise other k8s control plane components</t>
+  </si>
+  <si>
+    <t>gain persistence in container</t>
+  </si>
+  <si>
+    <t>entry though known, unpatched vulnerabilities</t>
+  </si>
+  <si>
+    <t>Assumption: Default configs for everything!</t>
+  </si>
+  <si>
+    <t>Assumption: Tenants only divided by namespace, NOT cluster!</t>
+  </si>
+  <si>
+    <t>&lt;- impact lower on cluster split</t>
+  </si>
+  <si>
+    <t>gain persistence in k8s control plane</t>
+  </si>
+  <si>
+    <t>gain persistence in cloud mgmt</t>
+  </si>
+  <si>
+    <t>&lt;- diff -&gt;</t>
+  </si>
+  <si>
+    <t>&lt;- On-Prem impact lower on cluster split</t>
   </si>
 </sst>
 </file>
@@ -502,7 +617,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -698,12 +813,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -737,28 +863,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,19 +888,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -855,6 +959,59 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1145,7 +1302,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,8 +1338,8 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="67" t="s">
-        <v>89</v>
+      <c r="E4" s="57" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1497,10 +1654,952 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C2" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="76">
+        <f>B4*C4</f>
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="20">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
+      <c r="H4" s="76">
+        <f>F4*G4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="10">
+        <v>4</v>
+      </c>
+      <c r="D5" s="75">
+        <f t="shared" ref="D5:D24" si="0">B5*C5</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>4</v>
+      </c>
+      <c r="H5" s="75">
+        <f t="shared" ref="H5:H24" si="1">F5*G5</f>
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4</v>
+      </c>
+      <c r="D6" s="75">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4</v>
+      </c>
+      <c r="H6" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="56">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="75">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="56">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N7" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="O7" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="56">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10">
+        <v>4</v>
+      </c>
+      <c r="D8" s="75">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="56">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10">
+        <v>4</v>
+      </c>
+      <c r="H8" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="56">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10">
+        <v>4</v>
+      </c>
+      <c r="D9" s="75">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="56">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>4</v>
+      </c>
+      <c r="H9" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>153</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="75">
+        <f>B10*C10</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="10">
+        <v>4</v>
+      </c>
+      <c r="H10" s="75">
+        <f>F10*G10</f>
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>153</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="75">
+        <f>B11*C11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="56">
+        <v>2</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="75">
+        <f>F11*G11</f>
+        <v>2</v>
+      </c>
+      <c r="N11" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>4</v>
+      </c>
+      <c r="D12" s="75">
+        <f>B12*C12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="56">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>4</v>
+      </c>
+      <c r="H12" s="75">
+        <f>F12*G12</f>
+        <v>4</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>4</v>
+      </c>
+      <c r="D13" s="75">
+        <f>B13*C13</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F13" s="56">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
+        <v>4</v>
+      </c>
+      <c r="H13" s="75">
+        <f>F13*G13</f>
+        <v>4</v>
+      </c>
+      <c r="O13" s="65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="20">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2</v>
+      </c>
+      <c r="D14" s="75">
+        <f>B14*C14</f>
+        <v>6</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="20">
+        <v>3</v>
+      </c>
+      <c r="G14" s="77">
+        <v>2</v>
+      </c>
+      <c r="H14" s="75">
+        <f>F14*G14</f>
+        <v>6</v>
+      </c>
+      <c r="O14" s="22"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="10">
+        <v>4</v>
+      </c>
+      <c r="D15" s="75">
+        <f>B15*C15</f>
+        <v>10</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="77">
+        <v>4</v>
+      </c>
+      <c r="H15" s="75">
+        <f>F15*G15</f>
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>153</v>
+      </c>
+      <c r="O15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="20">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2</v>
+      </c>
+      <c r="D16" s="75">
+        <f>B16*C16</f>
+        <v>4</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="20">
+        <v>2</v>
+      </c>
+      <c r="G16" s="77">
+        <v>2</v>
+      </c>
+      <c r="H16" s="75">
+        <f>F16*G16</f>
+        <v>4</v>
+      </c>
+      <c r="O16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="56">
+        <v>2</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4</v>
+      </c>
+      <c r="D17" s="75">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="20">
+        <v>2</v>
+      </c>
+      <c r="G17" s="77">
+        <v>4</v>
+      </c>
+      <c r="H17" s="75">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>153</v>
+      </c>
+      <c r="O17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="20">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2</v>
+      </c>
+      <c r="D18" s="75">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="20">
+        <v>1</v>
+      </c>
+      <c r="G18" s="77">
+        <v>2</v>
+      </c>
+      <c r="H18" s="75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="20">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10">
+        <v>4</v>
+      </c>
+      <c r="D19" s="75">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="20">
+        <v>2</v>
+      </c>
+      <c r="G19" s="77">
+        <v>4</v>
+      </c>
+      <c r="H19" s="75">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>153</v>
+      </c>
+      <c r="O19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="56">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10">
+        <v>2</v>
+      </c>
+      <c r="D20" s="75">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="56">
+        <v>2</v>
+      </c>
+      <c r="G20" s="77">
+        <v>2</v>
+      </c>
+      <c r="H20" s="75">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="56">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
+      <c r="D21" s="75">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="56">
+        <v>2</v>
+      </c>
+      <c r="G21" s="77">
+        <v>1</v>
+      </c>
+      <c r="H21" s="75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="56">
+        <v>2</v>
+      </c>
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+      <c r="D22" s="75">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="56">
+        <v>2</v>
+      </c>
+      <c r="G22" s="77">
+        <v>1</v>
+      </c>
+      <c r="H22" s="75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="56">
+        <v>2</v>
+      </c>
+      <c r="C23" s="10">
+        <v>4</v>
+      </c>
+      <c r="D23" s="75">
+        <f t="shared" ref="D23" si="2">B23*C23</f>
+        <v>8</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="56">
+        <v>2</v>
+      </c>
+      <c r="G23" s="77">
+        <v>2</v>
+      </c>
+      <c r="H23" s="75">
+        <f t="shared" ref="H23" si="3">F23*G23</f>
+        <v>4</v>
+      </c>
+      <c r="J23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="56">
+        <v>2</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2</v>
+      </c>
+      <c r="D24" s="75">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="56">
+        <v>2</v>
+      </c>
+      <c r="G24" s="77">
+        <v>3</v>
+      </c>
+      <c r="H24" s="75">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="56">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2</v>
+      </c>
+      <c r="D25" s="75">
+        <f>B25*C25</f>
+        <v>2</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="56">
+        <v>1</v>
+      </c>
+      <c r="G25" s="77">
+        <v>2</v>
+      </c>
+      <c r="H25" s="75">
+        <f>F25*G25</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="56">
+        <v>2</v>
+      </c>
+      <c r="C26" s="10">
+        <v>4</v>
+      </c>
+      <c r="D26" s="75">
+        <f t="shared" ref="D26:D32" si="4">B26*C26</f>
+        <v>8</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" s="56">
+        <v>1</v>
+      </c>
+      <c r="G26" s="77">
+        <v>4</v>
+      </c>
+      <c r="H26" s="75">
+        <f>F26*G26</f>
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="56">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10">
+        <v>4</v>
+      </c>
+      <c r="D27" s="75">
+        <f t="shared" ref="D27" si="5">B27*C27</f>
+        <v>4</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="56">
+        <v>1</v>
+      </c>
+      <c r="G27" s="77">
+        <v>4</v>
+      </c>
+      <c r="H27" s="75">
+        <f t="shared" ref="H27" si="6">F27*G27</f>
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="56">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10">
+        <v>4</v>
+      </c>
+      <c r="D28" s="75">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="56">
+        <v>1</v>
+      </c>
+      <c r="G28" s="77">
+        <v>4</v>
+      </c>
+      <c r="H28" s="75">
+        <f>F28*G28</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="56">
+        <v>2</v>
+      </c>
+      <c r="C29" s="10">
+        <v>2</v>
+      </c>
+      <c r="D29" s="75">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="56">
+        <v>2</v>
+      </c>
+      <c r="G29" s="77">
+        <v>2</v>
+      </c>
+      <c r="H29" s="75">
+        <f>F29*G29</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="78">
+        <v>3</v>
+      </c>
+      <c r="C30" s="12">
+        <v>4</v>
+      </c>
+      <c r="D30" s="79">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F30" s="78">
+        <v>2</v>
+      </c>
+      <c r="G30" s="80">
+        <v>4</v>
+      </c>
+      <c r="H30" s="79">
+        <f>F30*G30</f>
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="74"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="74"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="74"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="74"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="73"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="74"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="73"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="74"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D4:D22 H4:H22 H24:H30 D24:D30">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23 D23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:A54"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,43 +2619,43 @@
         <v>41</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="60" t="s">
-        <v>70</v>
+        <v>42</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="54"/>
-      <c r="L3" s="50"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="44"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="20">
         <v>4</v>
       </c>
       <c r="C4" s="10">
@@ -1565,14 +2664,14 @@
       <c r="D4" s="10">
         <v>3</v>
       </c>
-      <c r="E4" s="23">
-        <v>3</v>
-      </c>
-      <c r="F4" s="55">
+      <c r="E4" s="20">
+        <v>3</v>
+      </c>
+      <c r="F4" s="45">
         <f>ROUND(((L4+C4+D4)/3*E4), 2)</f>
         <v>11</v>
       </c>
-      <c r="L4" s="51">
+      <c r="L4" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1580,46 +2679,46 @@
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="64">
-        <v>3</v>
-      </c>
-      <c r="E5" s="23">
-        <v>3</v>
-      </c>
-      <c r="F5" s="55" t="e">
+      <c r="B5" s="20"/>
+      <c r="C5" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="54">
+        <v>3</v>
+      </c>
+      <c r="E5" s="20">
+        <v>3</v>
+      </c>
+      <c r="F5" s="45" t="e">
         <f t="shared" ref="F5:F10" si="0">ROUND(((L5+C5+D5)/3*E5), 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L5" s="51">
+      <c r="L5" s="41">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="62" t="s">
-        <v>89</v>
+        <v>58</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="52" t="s">
+        <v>79</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="55" t="e">
+        <v>43</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" s="51">
+        <v>63</v>
+      </c>
+      <c r="L6" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1627,21 +2726,21 @@
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="55" t="e">
+      <c r="B7" s="20"/>
+      <c r="C7" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L7" s="51">
+      <c r="L7" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1649,26 +2748,26 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="23">
-        <v>4</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="23">
-        <v>3</v>
-      </c>
-      <c r="F8" s="55" t="e">
+      <c r="B8" s="20">
+        <v>4</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="20">
+        <v>3</v>
+      </c>
+      <c r="F8" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
-      </c>
-      <c r="L8" s="51">
+        <v>59</v>
+      </c>
+      <c r="L8" s="41">
         <v>1</v>
       </c>
     </row>
@@ -1676,23 +2775,23 @@
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="65" t="s">
-        <v>92</v>
+      <c r="B9" s="55" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
       </c>
-      <c r="D9" s="64">
-        <v>2</v>
-      </c>
-      <c r="E9" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="55" t="e">
+      <c r="D9" s="54">
+        <v>2</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L9" s="51">
+      <c r="L9" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1700,23 +2799,23 @@
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="65" t="s">
-        <v>93</v>
+      <c r="B10" s="55" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="10">
         <v>3</v>
       </c>
-      <c r="D10" s="64">
-        <v>2</v>
-      </c>
-      <c r="E10" s="23">
-        <v>3</v>
-      </c>
-      <c r="F10" s="55">
+      <c r="D10" s="54">
+        <v>2</v>
+      </c>
+      <c r="E10" s="20">
+        <v>3</v>
+      </c>
+      <c r="F10" s="45">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L10" s="51">
+      <c r="L10" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1724,118 +2823,118 @@
       <c r="A11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="56"/>
-      <c r="L11" s="50"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="46"/>
+      <c r="L11" s="40"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="56"/>
-      <c r="L12" s="50"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="46"/>
+      <c r="L12" s="40"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="56"/>
-      <c r="L13" s="50"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="46"/>
+      <c r="L13" s="40"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="23">
+        <v>89</v>
+      </c>
+      <c r="B14" s="20">
         <v>2</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="66">
-        <v>3</v>
-      </c>
-      <c r="F14" s="55">
+      <c r="E14" s="56">
+        <v>3</v>
+      </c>
+      <c r="F14" s="45">
         <f t="shared" ref="F14:F16" si="1">ROUND(((L14+C14+D14)/3*E14), 2)</f>
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
-      </c>
-      <c r="L14" s="51"/>
+        <v>61</v>
+      </c>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="23">
+        <v>90</v>
+      </c>
+      <c r="B15" s="20">
         <v>2</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="66">
-        <v>3</v>
-      </c>
-      <c r="F15" s="55">
+      <c r="E15" s="56">
+        <v>3</v>
+      </c>
+      <c r="F15" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15" s="51"/>
+      <c r="L15" s="41"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="23"/>
+        <v>91</v>
+      </c>
+      <c r="B16" s="20"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="55">
+      <c r="E16" s="56"/>
+      <c r="F16" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L16" s="51"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="57"/>
-      <c r="L17" s="52"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="47"/>
+      <c r="L17" s="42"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="10">
         <v>3</v>
       </c>
-      <c r="D18" s="64">
-        <v>2</v>
-      </c>
-      <c r="E18" s="23">
-        <v>3</v>
-      </c>
-      <c r="F18" s="55">
+      <c r="D18" s="54">
+        <v>2</v>
+      </c>
+      <c r="E18" s="20">
+        <v>3</v>
+      </c>
+      <c r="F18" s="45">
         <f t="shared" ref="F18:F22" si="2">ROUND(((L18+C18+D18)/3*E18), 2)</f>
         <v>10</v>
       </c>
-      <c r="L18" s="51">
+      <c r="L18" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1843,46 +2942,46 @@
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="64">
-        <v>2</v>
-      </c>
-      <c r="E19" s="23">
-        <v>3</v>
-      </c>
-      <c r="F19" s="55" t="e">
+      <c r="B19" s="20"/>
+      <c r="C19" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="54">
+        <v>2</v>
+      </c>
+      <c r="E19" s="20">
+        <v>3</v>
+      </c>
+      <c r="F19" s="45" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L19" s="51">
+      <c r="L19" s="41">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="55" t="e">
+        <v>58</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="45" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
-      </c>
-      <c r="L20" s="51">
+        <v>63</v>
+      </c>
+      <c r="L20" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1890,19 +2989,19 @@
       <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="55" t="e">
+      <c r="B21" s="20"/>
+      <c r="C21" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="45" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L21" s="51">
+      <c r="L21" s="41">
         <v>5</v>
       </c>
     </row>
@@ -1910,24 +3009,24 @@
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="23">
-        <v>3</v>
-      </c>
-      <c r="F22" s="55" t="e">
+      <c r="B22" s="20"/>
+      <c r="C22" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="20">
+        <v>3</v>
+      </c>
+      <c r="F22" s="45" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="51">
+        <v>59</v>
+      </c>
+      <c r="L22" s="41">
         <v>1</v>
       </c>
     </row>
@@ -1935,109 +3034,109 @@
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="47"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="58"/>
-      <c r="L23" s="50"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="48"/>
+      <c r="L23" s="40"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="47"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="58"/>
-      <c r="L24" s="50"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="48"/>
+      <c r="L24" s="40"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="10">
         <v>3</v>
       </c>
       <c r="D25" s="10">
         <v>3</v>
       </c>
-      <c r="E25" s="65">
-        <v>1</v>
-      </c>
-      <c r="F25" s="55">
+      <c r="E25" s="55">
+        <v>1</v>
+      </c>
+      <c r="F25" s="45">
         <f t="shared" ref="F25:F26" si="3">ROUND(((L25+C25+D25)/3*E25), 2)</f>
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>71</v>
-      </c>
-      <c r="L25" s="51"/>
+        <v>61</v>
+      </c>
+      <c r="L25" s="41"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="55" t="e">
+      <c r="B26" s="20"/>
+      <c r="C26" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26" s="45" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="H26" t="s">
-        <v>72</v>
-      </c>
-      <c r="L26" s="51"/>
+        <v>62</v>
+      </c>
+      <c r="L26" s="41"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="44"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="58"/>
-      <c r="L27" s="50"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="48"/>
+      <c r="L27" s="40"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="57"/>
-      <c r="L28" s="52"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="47"/>
+      <c r="L28" s="42"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="10">
         <v>3</v>
       </c>
       <c r="D29" s="10">
         <v>2</v>
       </c>
-      <c r="E29" s="23">
-        <v>3</v>
-      </c>
-      <c r="F29" s="55">
+      <c r="E29" s="20">
+        <v>3</v>
+      </c>
+      <c r="F29" s="45">
         <f t="shared" ref="F29:F40" si="4">ROUND(((L29+C29+D29)/3*E29), 2)</f>
         <v>8</v>
       </c>
-      <c r="L29" s="51">
+      <c r="L29" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2045,46 +3144,46 @@
       <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="62" t="s">
-        <v>88</v>
+      <c r="B30" s="20"/>
+      <c r="C30" s="52" t="s">
+        <v>78</v>
       </c>
       <c r="D30" s="10">
         <v>2</v>
       </c>
-      <c r="E30" s="23">
-        <v>3</v>
-      </c>
-      <c r="F30" s="55" t="e">
+      <c r="E30" s="20">
+        <v>3</v>
+      </c>
+      <c r="F30" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L30" s="51">
+      <c r="L30" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="55" t="e">
+        <v>58</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
-      </c>
-      <c r="L31" s="51">
+        <v>63</v>
+      </c>
+      <c r="L31" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2092,19 +3191,19 @@
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="55" t="e">
+      <c r="B32" s="20"/>
+      <c r="C32" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="20"/>
+      <c r="F32" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L32" s="51">
+      <c r="L32" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2112,49 +3211,49 @@
       <c r="A33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="23">
-        <v>3</v>
-      </c>
-      <c r="F33" s="55" t="e">
+      <c r="B33" s="20"/>
+      <c r="C33" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="20">
+        <v>3</v>
+      </c>
+      <c r="F33" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="H33" t="s">
-        <v>69</v>
-      </c>
-      <c r="L33" s="51">
+        <v>59</v>
+      </c>
+      <c r="L33" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="62" t="s">
-        <v>89</v>
+        <v>64</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="52" t="s">
+        <v>79</v>
       </c>
       <c r="D34" s="10">
         <v>2</v>
       </c>
-      <c r="E34" s="23">
-        <v>3</v>
-      </c>
-      <c r="F34" s="55" t="e">
+      <c r="E34" s="20">
+        <v>3</v>
+      </c>
+      <c r="F34" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
-      </c>
-      <c r="L34" s="51">
+        <v>65</v>
+      </c>
+      <c r="L34" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2162,21 +3261,21 @@
       <c r="A35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="23"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="10">
         <v>1</v>
       </c>
       <c r="D35" s="10">
         <v>1</v>
       </c>
-      <c r="E35" s="23">
-        <v>3</v>
-      </c>
-      <c r="F35" s="55">
+      <c r="E35" s="20">
+        <v>3</v>
+      </c>
+      <c r="F35" s="45">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="L35" s="51">
+      <c r="L35" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2184,63 +3283,63 @@
       <c r="A36" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="62" t="s">
-        <v>92</v>
+      <c r="B36" s="20"/>
+      <c r="C36" s="52" t="s">
+        <v>82</v>
       </c>
       <c r="D36" s="10">
         <v>2</v>
       </c>
-      <c r="E36" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="55" t="e">
+      <c r="E36" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L36" s="51">
+      <c r="L36" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E37" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F37" s="55" t="e">
+        <v>86</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L37" s="51"/>
+      <c r="L37" s="41"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="B38" s="20"/>
       <c r="C38" s="10">
         <v>3</v>
       </c>
       <c r="D38" s="10">
         <v>2</v>
       </c>
-      <c r="E38" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="55" t="e">
+      <c r="E38" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L38" s="51">
+      <c r="L38" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2248,21 +3347,21 @@
       <c r="A39" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="23"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="10">
         <v>3</v>
       </c>
       <c r="D39" s="10">
         <v>2</v>
       </c>
-      <c r="E39" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39" s="55" t="e">
+      <c r="E39" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L39" s="51">
+      <c r="L39" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2270,21 +3369,21 @@
       <c r="A40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="23"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="10">
         <v>3</v>
       </c>
       <c r="D40" s="10">
         <v>2</v>
       </c>
-      <c r="E40" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40" s="55" t="e">
+      <c r="E40" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L40" s="51">
+      <c r="L40" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2292,92 +3391,92 @@
       <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="47"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="58"/>
-      <c r="L41" s="50"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="48"/>
+      <c r="L41" s="40"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="47"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="58"/>
-      <c r="L42" s="50"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="48"/>
+      <c r="L42" s="40"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="23"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="10">
         <v>3</v>
       </c>
       <c r="D43" s="10">
         <v>2</v>
       </c>
-      <c r="E43" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F43" s="55" t="e">
+      <c r="E43" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="45" t="e">
         <f t="shared" ref="F43:F46" si="5">ROUND(((L43+C43+D43)/3*E43), 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="H43" t="s">
-        <v>71</v>
-      </c>
-      <c r="L43" s="51"/>
+        <v>61</v>
+      </c>
+      <c r="L43" s="41"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="55" t="e">
+      <c r="B44" s="20"/>
+      <c r="C44" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="45" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="H44" t="s">
-        <v>72</v>
-      </c>
-      <c r="L44" s="51"/>
+        <v>62</v>
+      </c>
+      <c r="L44" s="41"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="62" t="s">
-        <v>89</v>
+      <c r="B45" s="20"/>
+      <c r="C45" s="52" t="s">
+        <v>79</v>
       </c>
       <c r="D45" s="10">
         <v>1</v>
       </c>
-      <c r="E45" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="55" t="e">
+      <c r="E45" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="45" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="H45" t="s">
-        <v>82</v>
-      </c>
-      <c r="L45" s="51">
+        <v>72</v>
+      </c>
+      <c r="L45" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2385,88 +3484,88 @@
       <c r="A46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="10">
         <v>3</v>
       </c>
-      <c r="D46" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="55" t="e">
+      <c r="D46" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="45" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="H46" t="s">
-        <v>83</v>
-      </c>
-      <c r="L46" s="51"/>
+        <v>73</v>
+      </c>
+      <c r="L46" s="41"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="44"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="58"/>
-      <c r="L47" s="50"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="48"/>
+      <c r="L47" s="40"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="57"/>
-      <c r="L48" s="52"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="47"/>
+      <c r="L48" s="42"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="23"/>
+      <c r="B49" s="20"/>
       <c r="C49" s="10">
         <v>3</v>
       </c>
       <c r="D49" s="10">
         <v>1</v>
       </c>
-      <c r="E49" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F49" s="55" t="e">
+      <c r="E49" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" s="45" t="e">
         <f t="shared" ref="F49:F57" si="6">ROUND(((L49+C49+D49)/3*E49), 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L49" s="51">
+      <c r="L49" s="41">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="23"/>
+        <v>87</v>
+      </c>
+      <c r="B50" s="20"/>
       <c r="C50" s="10">
         <v>3</v>
       </c>
       <c r="D50" s="10">
         <v>1</v>
       </c>
-      <c r="E50" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F50" s="55" t="e">
+      <c r="E50" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="45" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L50" s="51">
+      <c r="L50" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2474,21 +3573,21 @@
       <c r="A51" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="20"/>
       <c r="C51" s="10" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D51" s="10">
         <v>1</v>
       </c>
-      <c r="E51" s="23">
-        <v>3</v>
-      </c>
-      <c r="F51" s="55" t="e">
+      <c r="E51" s="20">
+        <v>3</v>
+      </c>
+      <c r="F51" s="45" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L51" s="51">
+      <c r="L51" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2496,24 +3595,24 @@
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="20"/>
       <c r="C52" s="10">
         <v>3</v>
       </c>
       <c r="D52" s="10">
         <v>1</v>
       </c>
-      <c r="E52" s="23">
-        <v>1</v>
-      </c>
-      <c r="F52" s="55">
+      <c r="E52" s="20">
+        <v>1</v>
+      </c>
+      <c r="F52" s="45">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="H52" t="s">
-        <v>77</v>
-      </c>
-      <c r="L52" s="51">
+        <v>67</v>
+      </c>
+      <c r="L52" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2521,24 +3620,24 @@
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="23"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="10">
         <v>3</v>
       </c>
       <c r="D53" s="10">
         <v>1</v>
       </c>
-      <c r="E53" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F53" s="55" t="e">
+      <c r="E53" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F53" s="45" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H53" t="s">
-        <v>80</v>
-      </c>
-      <c r="L53" s="51">
+        <v>70</v>
+      </c>
+      <c r="L53" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2546,21 +3645,21 @@
       <c r="A54" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B54" s="23"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="10">
         <v>3</v>
       </c>
       <c r="D54" s="10">
         <v>1</v>
       </c>
-      <c r="E54" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F54" s="55" t="e">
+      <c r="E54" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="45" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L54" s="51">
+      <c r="L54" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2568,44 +3667,44 @@
       <c r="A55" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E55" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F55" s="55" t="e">
+      <c r="B55" s="20"/>
+      <c r="C55" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E55" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="45" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H55" t="s">
-        <v>72</v>
-      </c>
-      <c r="L55" s="51"/>
+        <v>62</v>
+      </c>
+      <c r="L55" s="41"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="62" t="s">
-        <v>93</v>
+      <c r="B56" s="20"/>
+      <c r="C56" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="D56" s="10">
         <v>1</v>
       </c>
-      <c r="E56" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F56" s="55" t="e">
+      <c r="E56" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56" s="45" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L56" s="51">
+      <c r="L56" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2613,24 +3712,24 @@
       <c r="A57" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="20"/>
       <c r="C57" s="10">
         <v>3</v>
       </c>
       <c r="D57" s="10">
         <v>1</v>
       </c>
-      <c r="E57" s="23">
-        <v>3</v>
-      </c>
-      <c r="F57" s="55">
+      <c r="E57" s="20">
+        <v>3</v>
+      </c>
+      <c r="F57" s="45">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="H57" t="s">
-        <v>78</v>
-      </c>
-      <c r="L57" s="51">
+        <v>68</v>
+      </c>
+      <c r="L57" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2638,46 +3737,46 @@
       <c r="A58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="47"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="58"/>
-      <c r="L58" s="50"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="48"/>
+      <c r="L58" s="40"/>
     </row>
     <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B59" s="45"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="57"/>
-      <c r="L59" s="52"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="47"/>
+      <c r="L59" s="42"/>
     </row>
     <row r="60" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="E60" s="23">
-        <v>3</v>
-      </c>
-      <c r="F60" s="55" t="e">
+      <c r="B60" s="20"/>
+      <c r="C60" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" s="20">
+        <v>3</v>
+      </c>
+      <c r="F60" s="45" t="e">
         <f t="shared" ref="F60:F68" si="7">ROUND(((L60+C60+D60)/3*E60), 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H60" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="L60" s="51">
+      <c r="H60" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="L60" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2685,24 +3784,24 @@
       <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B61" s="23"/>
+      <c r="B61" s="20"/>
       <c r="C61" s="10">
         <v>3</v>
       </c>
       <c r="D61" s="10">
         <v>2</v>
       </c>
-      <c r="E61" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" s="55" t="e">
+      <c r="E61" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="H61" t="s">
-        <v>79</v>
-      </c>
-      <c r="L61" s="51">
+        <v>69</v>
+      </c>
+      <c r="L61" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2710,21 +3809,21 @@
       <c r="A62" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="23"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="10">
         <v>3</v>
       </c>
       <c r="D62" s="10">
         <v>2</v>
       </c>
-      <c r="E62" s="23">
-        <v>3</v>
-      </c>
-      <c r="F62" s="55">
+      <c r="E62" s="20">
+        <v>3</v>
+      </c>
+      <c r="F62" s="45">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="L62" s="51">
+      <c r="L62" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2732,24 +3831,24 @@
       <c r="A63" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="62" t="s">
-        <v>89</v>
+      <c r="B63" s="20"/>
+      <c r="C63" s="52" t="s">
+        <v>79</v>
       </c>
       <c r="D63" s="10">
         <v>2</v>
       </c>
-      <c r="E63" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="F63" s="55" t="e">
+      <c r="E63" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F63" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="H63" t="s">
-        <v>77</v>
-      </c>
-      <c r="L63" s="51">
+        <v>67</v>
+      </c>
+      <c r="L63" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2757,7 +3856,7 @@
       <c r="A64" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B64" s="23">
+      <c r="B64" s="20">
         <v>3</v>
       </c>
       <c r="C64" s="10">
@@ -2766,17 +3865,17 @@
       <c r="D64" s="10">
         <v>2</v>
       </c>
-      <c r="E64" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F64" s="55" t="e">
+      <c r="E64" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="H64" t="s">
-        <v>76</v>
-      </c>
-      <c r="L64" s="51">
+        <v>66</v>
+      </c>
+      <c r="L64" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2784,21 +3883,21 @@
       <c r="A65" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="23"/>
+      <c r="B65" s="20"/>
       <c r="C65" s="10">
         <v>3</v>
       </c>
       <c r="D65" s="10">
         <v>3</v>
       </c>
-      <c r="E65" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F65" s="55" t="e">
+      <c r="E65" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F65" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L65" s="51">
+      <c r="L65" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2806,44 +3905,44 @@
       <c r="A66" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D66" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="E66" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F66" s="55" t="e">
+      <c r="B66" s="20"/>
+      <c r="C66" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="H66" t="s">
-        <v>72</v>
-      </c>
-      <c r="L66" s="51"/>
+        <v>62</v>
+      </c>
+      <c r="L66" s="41"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B67" s="23"/>
-      <c r="C67" s="63" t="s">
-        <v>95</v>
+      <c r="B67" s="20"/>
+      <c r="C67" s="53" t="s">
+        <v>85</v>
       </c>
       <c r="D67" s="10">
         <v>2</v>
       </c>
-      <c r="E67" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="F67" s="55" t="e">
+      <c r="E67" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L67" s="51">
+      <c r="L67" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2851,41 +3950,41 @@
       <c r="A68" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="23"/>
-      <c r="C68" s="62" t="s">
-        <v>92</v>
+      <c r="B68" s="20"/>
+      <c r="C68" s="52" t="s">
+        <v>82</v>
       </c>
       <c r="D68" s="10">
         <v>1</v>
       </c>
-      <c r="E68" s="23">
-        <v>3</v>
-      </c>
-      <c r="F68" s="55" t="e">
+      <c r="E68" s="20">
+        <v>3</v>
+      </c>
+      <c r="F68" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="H68" t="s">
-        <v>79</v>
-      </c>
-      <c r="L68" s="51">
+        <v>69</v>
+      </c>
+      <c r="L68" s="41">
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="49" t="s">
+      <c r="A69" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B69" s="44"/>
-      <c r="C69" s="48"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="44"/>
-      <c r="F69" s="59"/>
-      <c r="L69" s="53"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="49"/>
+      <c r="L69" s="43"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -2899,7 +3998,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -2913,7 +4012,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -2927,7 +4026,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -2945,287 +4044,307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="H2" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="39" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="H2" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="H3" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="21"/>
+      <c r="H4" s="64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="26"/>
-      <c r="H4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="35" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="26"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I12" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" t="s">
-        <v>112</v>
-      </c>
-      <c r="L12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
-      <c r="J13">
-        <v>3</v>
-      </c>
-      <c r="K13">
-        <f>(G13+H13+I13+J13)/4</f>
-        <v>2.75</v>
-      </c>
-      <c r="L13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <f>L13*K13</f>
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>119</v>
       </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
-      <c r="K14">
-        <f>(G14+H14+I14+J14)/4</f>
-        <v>2</v>
-      </c>
-      <c r="L14">
-        <v>4</v>
-      </c>
-      <c r="M14">
-        <f>L14*K14</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <f>(F21+G21+H21+I21)/4</f>
+        <v>2.75</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <f>K21*J21</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24">
-        <v>3</v>
-      </c>
-      <c r="J24">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <f>(F22+G22+H22+I22)/4</f>
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <f>K22*J22</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added detailed risk assess
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vector Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Vectors simple" sheetId="4" r:id="rId2"/>
-    <sheet name="Vector Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Vectors detailed" sheetId="5" r:id="rId3"/>
     <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
+    <sheet name="Vector Details_OLD" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ISFOXAutomaticLabelingDisabled" hidden="1">TRUE</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="166">
   <si>
     <t>Attack Vectors Overview</t>
   </si>
@@ -522,6 +523,30 @@
   </si>
   <si>
     <t>&lt;- On-Prem impact lower on cluster split</t>
+  </si>
+  <si>
+    <t>Vector risk assessment, detailed</t>
+  </si>
+  <si>
+    <t>RAL</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Assumption: Average "usual" (non container-specific) application security measures taken</t>
+  </si>
+  <si>
+    <t>Probability (+)</t>
+  </si>
+  <si>
+    <t>Resulting risk (+)</t>
+  </si>
+  <si>
+    <t>Note: Probability is multiplication of factors and not addition, since that proberly resembles reality! If its twice as difficult to exploit something, the probability should be half, not 1/4th or less. Also: if there's one zero, the resulting probability should come out as zero.</t>
+  </si>
+  <si>
+    <t>probability simple est.</t>
   </si>
 </sst>
 </file>
@@ -617,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -824,12 +849,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1013,10 +1047,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1037,7 +1104,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1305,7 +1372,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1656,11 +1723,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
@@ -1915,7 +1982,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="75">
-        <f>B10*C10</f>
+        <f t="shared" ref="D10:D16" si="2">B10*C10</f>
         <v>2</v>
       </c>
       <c r="E10" s="10"/>
@@ -1926,7 +1993,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="75">
-        <f>F10*G10</f>
+        <f t="shared" ref="H10:H16" si="3">F10*G10</f>
         <v>2</v>
       </c>
       <c r="J10" t="s">
@@ -1950,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="75">
-        <f>B11*C11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -1963,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="75">
-        <f>F11*G11</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N11" s="70" t="s">
@@ -1984,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="75">
-        <f>B12*C12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -1997,7 +2064,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="75">
-        <f>F12*G12</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="O12" s="21" t="s">
@@ -2015,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="75">
-        <f>B13*C13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -2028,7 +2095,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="75">
-        <f>F13*G13</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="O13" s="65" t="s">
@@ -2046,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="75">
-        <f>B14*C14</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E14" s="10"/>
@@ -2057,7 +2124,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="75">
-        <f>F14*G14</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="O14" s="22"/>
@@ -2073,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="75">
-        <f>B15*C15</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E15" s="10"/>
@@ -2084,7 +2151,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="75">
-        <f>F15*G15</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="J15" t="s">
@@ -2105,7 +2172,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="75">
-        <f>B16*C16</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E16" s="10"/>
@@ -2116,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="75">
-        <f>F16*G16</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="O16" t="s">
@@ -2305,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="75">
-        <f t="shared" ref="D23" si="2">B23*C23</f>
+        <f t="shared" ref="D23" si="4">B23*C23</f>
         <v>8</v>
       </c>
       <c r="E23" s="10" t="s">
@@ -2318,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="75">
-        <f t="shared" ref="H23" si="3">F23*G23</f>
+        <f t="shared" ref="H23" si="5">F23*G23</f>
         <v>4</v>
       </c>
       <c r="J23" t="s">
@@ -2390,7 +2457,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="75">
-        <f t="shared" ref="D26:D32" si="4">B26*C26</f>
+        <f t="shared" ref="D26:D30" si="6">B26*C26</f>
         <v>8</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -2421,7 +2488,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="75">
-        <f t="shared" ref="D27" si="5">B27*C27</f>
+        <f t="shared" ref="D27" si="7">B27*C27</f>
         <v>4</v>
       </c>
       <c r="E27" s="10"/>
@@ -2432,7 +2499,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="75">
-        <f t="shared" ref="H27" si="6">F27*G27</f>
+        <f t="shared" ref="H27" si="8">F27*G27</f>
         <v>4</v>
       </c>
       <c r="J27" t="s">
@@ -2450,7 +2517,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E28" s="10"/>
@@ -2476,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E29" s="10"/>
@@ -2502,7 +2569,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="E30" s="12" t="s">
@@ -2577,7 +2644,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23 D23">
+  <conditionalFormatting sqref="D23 H23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2596,13 +2663,2326 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+    <col min="18" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="D2" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="90" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="91" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="L3" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="M3" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="90" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q3" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="R3" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="84">
+        <v>1</v>
+      </c>
+      <c r="C4" s="81">
+        <v>1</v>
+      </c>
+      <c r="D4" s="81">
+        <v>3</v>
+      </c>
+      <c r="E4" s="81">
+        <v>2</v>
+      </c>
+      <c r="F4" s="82">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="81">
+        <f>ROUND(((B4*C4*D4*E4)/81*3), 1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="88">
+        <f>ROUND(((B4+C4+D4+E4)/4), 1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="86">
+        <f>G4*I4</f>
+        <v>0.2</v>
+      </c>
+      <c r="K4" s="86">
+        <f>H4*I4</f>
+        <v>1.8</v>
+      </c>
+      <c r="L4" s="84">
+        <v>1</v>
+      </c>
+      <c r="M4" s="81">
+        <v>1</v>
+      </c>
+      <c r="N4" s="81">
+        <v>3</v>
+      </c>
+      <c r="O4" s="81">
+        <v>2</v>
+      </c>
+      <c r="P4" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="88">
+        <f>ROUND(((L4*M4*N4*O4)/81*3), 1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="R4" s="10">
+        <v>1</v>
+      </c>
+      <c r="S4" s="86">
+        <f>Q4*R4</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="81">
+        <v>1</v>
+      </c>
+      <c r="D5" s="81">
+        <v>3</v>
+      </c>
+      <c r="E5" s="81">
+        <v>3</v>
+      </c>
+      <c r="F5" s="82">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="81">
+        <f>ROUND(((B5*C5*D5*E5)/81*3), 1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="81">
+        <f>ROUND(((B5+C5+D5+E5)/4), 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="10">
+        <v>4</v>
+      </c>
+      <c r="J5" s="86">
+        <f>G5*I5</f>
+        <v>1.2</v>
+      </c>
+      <c r="K5" s="86">
+        <f t="shared" ref="K5:K30" si="0">H5*I5</f>
+        <v>8</v>
+      </c>
+      <c r="L5" s="20">
+        <v>1</v>
+      </c>
+      <c r="M5" s="81">
+        <v>1</v>
+      </c>
+      <c r="N5" s="81">
+        <v>3</v>
+      </c>
+      <c r="O5" s="81">
+        <v>3</v>
+      </c>
+      <c r="P5" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="81">
+        <f>ROUND(((L5*M5*N5*O5)/81*3), 1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R5" s="10">
+        <v>4</v>
+      </c>
+      <c r="S5" s="86">
+        <f t="shared" ref="S5:S30" si="1">Q5*R5</f>
+        <v>1.2</v>
+      </c>
+      <c r="U5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="20">
+        <v>1</v>
+      </c>
+      <c r="C6" s="81">
+        <v>1</v>
+      </c>
+      <c r="D6" s="81">
+        <v>3</v>
+      </c>
+      <c r="E6" s="81">
+        <v>3</v>
+      </c>
+      <c r="F6" s="82">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="81">
+        <f>ROUND(((B6*C6*D6*E6)/81*3), 1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H6" s="81">
+        <f>ROUND(((B6+C6+D6+E6)/4), 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="10">
+        <v>4</v>
+      </c>
+      <c r="J6" s="86">
+        <f>G6*I6</f>
+        <v>1.2</v>
+      </c>
+      <c r="K6" s="86">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L6" s="20">
+        <v>1</v>
+      </c>
+      <c r="M6" s="81">
+        <v>1</v>
+      </c>
+      <c r="N6" s="81">
+        <v>3</v>
+      </c>
+      <c r="O6" s="81">
+        <v>3</v>
+      </c>
+      <c r="P6" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="81">
+        <f>ROUND(((L6*M6*N6*O6)/81*3), 1)</f>
+        <v>0.3</v>
+      </c>
+      <c r="R6" s="10">
+        <v>4</v>
+      </c>
+      <c r="S6" s="86">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="U6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="20">
+        <v>3</v>
+      </c>
+      <c r="C7" s="81">
+        <v>3</v>
+      </c>
+      <c r="D7" s="81">
+        <v>2</v>
+      </c>
+      <c r="E7" s="81">
+        <v>2</v>
+      </c>
+      <c r="F7" s="82">
+        <v>2</v>
+      </c>
+      <c r="G7" s="81">
+        <f>ROUND(((B7*C7*D7*E7)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H7" s="81">
+        <f>ROUND(((B7+C7+D7+E7)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="86">
+        <f>G7*I7</f>
+        <v>1.3</v>
+      </c>
+      <c r="K7" s="86">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L7" s="20">
+        <v>3</v>
+      </c>
+      <c r="M7" s="81">
+        <v>3</v>
+      </c>
+      <c r="N7" s="81">
+        <v>2</v>
+      </c>
+      <c r="O7" s="81">
+        <v>2</v>
+      </c>
+      <c r="P7" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="81">
+        <f>ROUND(((L7*M7*N7*O7)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R7" s="10">
+        <v>1</v>
+      </c>
+      <c r="S7" s="86">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="Y7" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z7" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="20">
+        <v>2</v>
+      </c>
+      <c r="C8" s="81">
+        <v>3</v>
+      </c>
+      <c r="D8" s="77">
+        <v>2</v>
+      </c>
+      <c r="E8" s="77">
+        <v>2</v>
+      </c>
+      <c r="F8" s="82">
+        <v>1</v>
+      </c>
+      <c r="G8" s="81">
+        <f>ROUND(((B8*C8*D8*E8)/81*3), 1)</f>
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="81">
+        <f>ROUND(((B8+C8+D8+E8)/4), 1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I8" s="10">
+        <v>4</v>
+      </c>
+      <c r="J8" s="86">
+        <f>G8*I8</f>
+        <v>3.6</v>
+      </c>
+      <c r="K8" s="86">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L8" s="20">
+        <v>2</v>
+      </c>
+      <c r="M8" s="81">
+        <v>3</v>
+      </c>
+      <c r="N8" s="77">
+        <v>2</v>
+      </c>
+      <c r="O8" s="77">
+        <v>2</v>
+      </c>
+      <c r="P8" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="81">
+        <f>ROUND(((L8*M8*N8*O8)/81*3), 1)</f>
+        <v>0.9</v>
+      </c>
+      <c r="R8" s="10">
+        <v>4</v>
+      </c>
+      <c r="S8" s="86">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="U8" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y8" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z8" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="81">
+        <v>1</v>
+      </c>
+      <c r="D9" s="77">
+        <v>2</v>
+      </c>
+      <c r="E9" s="77">
+        <v>2</v>
+      </c>
+      <c r="F9" s="82">
+        <v>1</v>
+      </c>
+      <c r="G9" s="81">
+        <f>ROUND(((B9*C9*D9*E9)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="81">
+        <f>ROUND(((B9+C9+D9+E9)/4), 1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="10">
+        <v>4</v>
+      </c>
+      <c r="J9" s="86">
+        <f>G9*I9</f>
+        <v>0.4</v>
+      </c>
+      <c r="K9" s="86">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L9" s="20">
+        <v>1</v>
+      </c>
+      <c r="M9" s="81">
+        <v>1</v>
+      </c>
+      <c r="N9" s="77">
+        <v>2</v>
+      </c>
+      <c r="O9" s="77">
+        <v>2</v>
+      </c>
+      <c r="P9" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="81">
+        <f>ROUND(((L9*M9*N9*O9)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="R9" s="10">
+        <v>4</v>
+      </c>
+      <c r="S9" s="86">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="U9" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z9" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="20">
+        <v>1</v>
+      </c>
+      <c r="C10" s="81">
+        <v>3</v>
+      </c>
+      <c r="D10" s="81">
+        <v>1</v>
+      </c>
+      <c r="E10" s="81">
+        <v>1</v>
+      </c>
+      <c r="F10" s="82">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="81">
+        <f>ROUND(((B10*C10*D10*E10)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="81">
+        <f>ROUND(((B10+C10+D10+E10)/4), 1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="10">
+        <v>4</v>
+      </c>
+      <c r="J10" s="86">
+        <f>G10*I10</f>
+        <v>0.4</v>
+      </c>
+      <c r="K10" s="86">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L10" s="20">
+        <v>1</v>
+      </c>
+      <c r="M10" s="81">
+        <v>3</v>
+      </c>
+      <c r="N10" s="81">
+        <v>1</v>
+      </c>
+      <c r="O10" s="81">
+        <v>1</v>
+      </c>
+      <c r="P10" s="82">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="81">
+        <f>ROUND(((L10*M10*N10*O10)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="R10" s="10">
+        <v>4</v>
+      </c>
+      <c r="S10" s="86">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="U10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z10" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" s="82">
+        <v>0</v>
+      </c>
+      <c r="G11" s="81">
+        <v>0</v>
+      </c>
+      <c r="H11" s="81">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <v>1</v>
+      </c>
+      <c r="J11" s="86">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="56">
+        <v>2</v>
+      </c>
+      <c r="M11" s="77">
+        <v>4</v>
+      </c>
+      <c r="N11" s="77">
+        <v>3</v>
+      </c>
+      <c r="O11" s="77">
+        <v>2</v>
+      </c>
+      <c r="P11" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="81">
+        <f>ROUND(((L11*M11*N11*O11)/81*3), 1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="R11" s="10">
+        <v>1</v>
+      </c>
+      <c r="S11" s="86">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="Y11" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="82">
+        <v>0</v>
+      </c>
+      <c r="G12" s="81">
+        <v>0</v>
+      </c>
+      <c r="H12" s="81">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>4</v>
+      </c>
+      <c r="J12" s="86">
+        <f>G12*I12</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="56">
+        <v>2</v>
+      </c>
+      <c r="M12" s="77">
+        <v>4</v>
+      </c>
+      <c r="N12" s="77">
+        <v>3</v>
+      </c>
+      <c r="O12" s="77">
+        <v>3</v>
+      </c>
+      <c r="P12" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="81">
+        <f>ROUND(((L12*M12*N12*O12)/81*3), 1)</f>
+        <v>2.7</v>
+      </c>
+      <c r="R12" s="10">
+        <v>4</v>
+      </c>
+      <c r="S12" s="86">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
+      <c r="Z12" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="82">
+        <v>0</v>
+      </c>
+      <c r="G13" s="81">
+        <v>0</v>
+      </c>
+      <c r="H13" s="81">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>4</v>
+      </c>
+      <c r="J13" s="86">
+        <f>G13*I13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="56">
+        <v>1</v>
+      </c>
+      <c r="M13" s="77">
+        <v>4</v>
+      </c>
+      <c r="N13" s="77">
+        <v>3</v>
+      </c>
+      <c r="O13" s="77">
+        <v>3</v>
+      </c>
+      <c r="P13" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="81">
+        <f>ROUND(((L13*M13*N13*O13)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R13" s="10">
+        <v>4</v>
+      </c>
+      <c r="S13" s="86">
+        <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+      <c r="Z13" s="65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="20">
+        <v>4</v>
+      </c>
+      <c r="C14" s="81">
+        <v>4</v>
+      </c>
+      <c r="D14" s="81">
+        <v>3</v>
+      </c>
+      <c r="E14" s="81">
+        <v>3</v>
+      </c>
+      <c r="F14" s="82">
+        <v>3</v>
+      </c>
+      <c r="G14" s="81">
+        <f>ROUND(((B14*C14*D14*E14)/81*3), 1)</f>
+        <v>5.3</v>
+      </c>
+      <c r="H14" s="81">
+        <f>ROUND(((B14+C14+D14+E14)/4), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="I14" s="10">
+        <v>2</v>
+      </c>
+      <c r="J14" s="86">
+        <f>G14*I14</f>
+        <v>10.6</v>
+      </c>
+      <c r="K14" s="86">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L14" s="20">
+        <v>4</v>
+      </c>
+      <c r="M14" s="81">
+        <v>4</v>
+      </c>
+      <c r="N14" s="81">
+        <v>3</v>
+      </c>
+      <c r="O14" s="81">
+        <v>3</v>
+      </c>
+      <c r="P14" s="82">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="81">
+        <f>ROUND(((L14*M14*N14*O14)/81*3), 1)</f>
+        <v>5.3</v>
+      </c>
+      <c r="R14" s="77">
+        <v>2</v>
+      </c>
+      <c r="S14" s="86">
+        <f t="shared" si="1"/>
+        <v>10.6</v>
+      </c>
+      <c r="Z14" s="22"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="20">
+        <v>4</v>
+      </c>
+      <c r="C15" s="81">
+        <v>4</v>
+      </c>
+      <c r="D15" s="81">
+        <v>3</v>
+      </c>
+      <c r="E15" s="81">
+        <v>2</v>
+      </c>
+      <c r="F15" s="82">
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="81">
+        <f>ROUND(((B15*C15*D15*E15)/81*3), 1)</f>
+        <v>3.6</v>
+      </c>
+      <c r="H15" s="81">
+        <f>ROUND(((B15+C15+D15+E15)/4), 1)</f>
+        <v>3.3</v>
+      </c>
+      <c r="I15" s="10">
+        <v>4</v>
+      </c>
+      <c r="J15" s="86">
+        <f>G15*I15</f>
+        <v>14.4</v>
+      </c>
+      <c r="K15" s="86">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+      <c r="L15" s="20">
+        <v>4</v>
+      </c>
+      <c r="M15" s="81">
+        <v>4</v>
+      </c>
+      <c r="N15" s="81">
+        <v>3</v>
+      </c>
+      <c r="O15" s="81">
+        <v>2</v>
+      </c>
+      <c r="P15" s="82">
+        <v>2.5</v>
+      </c>
+      <c r="Q15" s="81">
+        <f>ROUND(((L15*M15*N15*O15)/81*3), 1)</f>
+        <v>3.6</v>
+      </c>
+      <c r="R15" s="77">
+        <v>4</v>
+      </c>
+      <c r="S15" s="86">
+        <f t="shared" si="1"/>
+        <v>14.4</v>
+      </c>
+      <c r="U15" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="56">
+        <v>2</v>
+      </c>
+      <c r="C16" s="81">
+        <v>2</v>
+      </c>
+      <c r="D16" s="81">
+        <v>2</v>
+      </c>
+      <c r="E16" s="81">
+        <v>2</v>
+      </c>
+      <c r="F16" s="82">
+        <v>2</v>
+      </c>
+      <c r="G16" s="81">
+        <f>ROUND(((B16*C16*D16*E16)/81*3), 1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="H16" s="81">
+        <f>ROUND(((B16+C16+D16+E16)/4), 1)</f>
+        <v>2</v>
+      </c>
+      <c r="I16" s="10">
+        <v>2</v>
+      </c>
+      <c r="J16" s="86">
+        <f>G16*I16</f>
+        <v>1.2</v>
+      </c>
+      <c r="K16" s="86">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L16" s="56">
+        <v>2</v>
+      </c>
+      <c r="M16" s="81">
+        <v>2</v>
+      </c>
+      <c r="N16" s="81">
+        <v>2</v>
+      </c>
+      <c r="O16" s="81">
+        <v>2</v>
+      </c>
+      <c r="P16" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="81">
+        <f>ROUND(((L16*M16*N16*O16)/81*3), 1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="R16" s="77">
+        <v>2</v>
+      </c>
+      <c r="S16" s="86">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="20">
+        <v>3</v>
+      </c>
+      <c r="C17" s="77">
+        <v>2</v>
+      </c>
+      <c r="D17" s="77">
+        <v>3</v>
+      </c>
+      <c r="E17" s="77">
+        <v>2</v>
+      </c>
+      <c r="F17" s="82">
+        <v>2</v>
+      </c>
+      <c r="G17" s="81">
+        <f>ROUND(((B17*C17*D17*E17)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H17" s="81">
+        <f>ROUND(((B17+C17+D17+E17)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I17" s="10">
+        <v>4</v>
+      </c>
+      <c r="J17" s="86">
+        <f>G17*I17</f>
+        <v>5.2</v>
+      </c>
+      <c r="K17" s="86">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L17" s="20">
+        <v>3</v>
+      </c>
+      <c r="M17" s="77">
+        <v>2</v>
+      </c>
+      <c r="N17" s="77">
+        <v>3</v>
+      </c>
+      <c r="O17" s="77">
+        <v>2</v>
+      </c>
+      <c r="P17" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="81">
+        <f>ROUND(((L17*M17*N17*O17)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R17" s="77">
+        <v>4</v>
+      </c>
+      <c r="S17" s="86">
+        <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+      <c r="U17" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="20">
+        <v>2</v>
+      </c>
+      <c r="C18" s="81">
+        <v>1</v>
+      </c>
+      <c r="D18" s="81">
+        <v>2</v>
+      </c>
+      <c r="E18" s="81">
+        <v>1</v>
+      </c>
+      <c r="F18" s="82">
+        <v>1</v>
+      </c>
+      <c r="G18" s="81">
+        <f>ROUND(((B18*C18*D18*E18)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="81">
+        <f>ROUND(((B18+C18+D18+E18)/4), 1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I18" s="10">
+        <v>2</v>
+      </c>
+      <c r="J18" s="86">
+        <f>G18*I18</f>
+        <v>0.2</v>
+      </c>
+      <c r="K18" s="86">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L18" s="20">
+        <v>2</v>
+      </c>
+      <c r="M18" s="81">
+        <v>1</v>
+      </c>
+      <c r="N18" s="81">
+        <v>2</v>
+      </c>
+      <c r="O18" s="81">
+        <v>1</v>
+      </c>
+      <c r="P18" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="81">
+        <f>ROUND(((L18*M18*N18*O18)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="R18" s="77">
+        <v>2</v>
+      </c>
+      <c r="S18" s="86">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="20">
+        <v>2</v>
+      </c>
+      <c r="C19" s="81">
+        <v>2</v>
+      </c>
+      <c r="D19" s="81">
+        <v>3</v>
+      </c>
+      <c r="E19" s="81">
+        <v>3</v>
+      </c>
+      <c r="F19" s="82">
+        <v>2</v>
+      </c>
+      <c r="G19" s="81">
+        <f>ROUND(((B19*C19*D19*E19)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H19" s="81">
+        <f>ROUND(((B19+C19+D19+E19)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I19" s="10">
+        <v>4</v>
+      </c>
+      <c r="J19" s="86">
+        <f>G19*I19</f>
+        <v>5.2</v>
+      </c>
+      <c r="K19" s="86">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L19" s="20">
+        <v>2</v>
+      </c>
+      <c r="M19" s="81">
+        <v>2</v>
+      </c>
+      <c r="N19" s="81">
+        <v>3</v>
+      </c>
+      <c r="O19" s="81">
+        <v>3</v>
+      </c>
+      <c r="P19" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="81">
+        <f>ROUND(((L19*M19*N19*O19)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R19" s="77">
+        <v>4</v>
+      </c>
+      <c r="S19" s="86">
+        <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+      <c r="U19" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="77">
+        <v>2</v>
+      </c>
+      <c r="D20" s="77">
+        <v>3</v>
+      </c>
+      <c r="E20" s="77">
+        <v>3</v>
+      </c>
+      <c r="F20" s="82">
+        <v>2</v>
+      </c>
+      <c r="G20" s="81">
+        <f>ROUND(((B20*C20*D20*E20)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H20" s="81">
+        <f>ROUND(((B20+C20+D20+E20)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I20" s="10">
+        <v>2</v>
+      </c>
+      <c r="J20" s="86">
+        <f>G20*I20</f>
+        <v>2.6</v>
+      </c>
+      <c r="K20" s="86">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L20" s="20">
+        <v>2</v>
+      </c>
+      <c r="M20" s="77">
+        <v>2</v>
+      </c>
+      <c r="N20" s="77">
+        <v>3</v>
+      </c>
+      <c r="O20" s="77">
+        <v>3</v>
+      </c>
+      <c r="P20" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="81">
+        <f>ROUND(((L20*M20*N20*O20)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R20" s="77">
+        <v>2</v>
+      </c>
+      <c r="S20" s="86">
+        <f t="shared" si="1"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="20">
+        <v>2</v>
+      </c>
+      <c r="C21" s="77">
+        <v>2</v>
+      </c>
+      <c r="D21" s="77">
+        <v>3</v>
+      </c>
+      <c r="E21" s="77">
+        <v>3</v>
+      </c>
+      <c r="F21" s="82">
+        <v>2</v>
+      </c>
+      <c r="G21" s="81">
+        <f>ROUND(((B21*C21*D21*E21)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H21" s="81">
+        <f>ROUND(((B21+C21+D21+E21)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1</v>
+      </c>
+      <c r="J21" s="86">
+        <f>G21*I21</f>
+        <v>1.3</v>
+      </c>
+      <c r="K21" s="86">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L21" s="20">
+        <v>2</v>
+      </c>
+      <c r="M21" s="77">
+        <v>2</v>
+      </c>
+      <c r="N21" s="77">
+        <v>3</v>
+      </c>
+      <c r="O21" s="77">
+        <v>3</v>
+      </c>
+      <c r="P21" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="81">
+        <f>ROUND(((L21*M21*N21*O21)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R21" s="77">
+        <v>1</v>
+      </c>
+      <c r="S21" s="86">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="20">
+        <v>2</v>
+      </c>
+      <c r="C22" s="77">
+        <v>2</v>
+      </c>
+      <c r="D22" s="77">
+        <v>3</v>
+      </c>
+      <c r="E22" s="77">
+        <v>3</v>
+      </c>
+      <c r="F22" s="82">
+        <v>2</v>
+      </c>
+      <c r="G22" s="81">
+        <f>ROUND(((B22*C22*D22*E22)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H22" s="81">
+        <f>ROUND(((B22+C22+D22+E22)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22" s="86">
+        <f>G22*I22</f>
+        <v>1.3</v>
+      </c>
+      <c r="K22" s="86">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L22" s="20">
+        <v>2</v>
+      </c>
+      <c r="M22" s="77">
+        <v>2</v>
+      </c>
+      <c r="N22" s="77">
+        <v>3</v>
+      </c>
+      <c r="O22" s="77">
+        <v>3</v>
+      </c>
+      <c r="P22" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="81">
+        <f>ROUND(((L22*M22*N22*O22)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R22" s="77">
+        <v>1</v>
+      </c>
+      <c r="S22" s="86">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="20">
+        <v>1</v>
+      </c>
+      <c r="C23" s="77">
+        <v>2</v>
+      </c>
+      <c r="D23" s="77">
+        <v>3</v>
+      </c>
+      <c r="E23" s="77">
+        <v>3</v>
+      </c>
+      <c r="F23" s="82">
+        <v>2</v>
+      </c>
+      <c r="G23" s="81">
+        <f>ROUND(((B23*C23*D23*E23)/81*3), 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="H23" s="81">
+        <f>ROUND(((B23+C23+D23+E23)/4), 1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I23" s="10">
+        <v>4</v>
+      </c>
+      <c r="J23" s="86">
+        <f>G23*I23</f>
+        <v>2.8</v>
+      </c>
+      <c r="K23" s="86">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L23" s="20">
+        <v>1</v>
+      </c>
+      <c r="M23" s="77">
+        <v>2</v>
+      </c>
+      <c r="N23" s="77">
+        <v>3</v>
+      </c>
+      <c r="O23" s="77">
+        <v>3</v>
+      </c>
+      <c r="P23" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="81">
+        <f>ROUND(((L23*M23*N23*O23)/81*3), 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R23" s="77">
+        <v>2</v>
+      </c>
+      <c r="S23" s="86">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="U23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="20">
+        <v>1</v>
+      </c>
+      <c r="C24" s="77">
+        <v>2</v>
+      </c>
+      <c r="D24" s="77">
+        <v>3</v>
+      </c>
+      <c r="E24" s="77">
+        <v>3</v>
+      </c>
+      <c r="F24" s="82">
+        <v>2</v>
+      </c>
+      <c r="G24" s="81">
+        <f>ROUND(((B24*C24*D24*E24)/81*3), 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="H24" s="81">
+        <f>ROUND(((B24+C24+D24+E24)/4), 1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I24" s="10">
+        <v>2</v>
+      </c>
+      <c r="J24" s="86">
+        <f>G24*I24</f>
+        <v>1.4</v>
+      </c>
+      <c r="K24" s="86">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L24" s="20">
+        <v>1</v>
+      </c>
+      <c r="M24" s="77">
+        <v>2</v>
+      </c>
+      <c r="N24" s="77">
+        <v>3</v>
+      </c>
+      <c r="O24" s="77">
+        <v>3</v>
+      </c>
+      <c r="P24" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="81">
+        <f>ROUND(((L24*M24*N24*O24)/81*3), 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R24" s="77">
+        <v>3</v>
+      </c>
+      <c r="S24" s="86">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="20">
+        <v>2</v>
+      </c>
+      <c r="C25" s="77">
+        <v>1</v>
+      </c>
+      <c r="D25" s="77">
+        <v>3</v>
+      </c>
+      <c r="E25" s="77">
+        <v>3</v>
+      </c>
+      <c r="F25" s="82">
+        <v>1</v>
+      </c>
+      <c r="G25" s="81">
+        <f>ROUND(((B25*C25*D25*E25)/81*3), 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="H25" s="81">
+        <f>ROUND(((B25+C25+D25+E25)/4), 1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I25" s="10">
+        <v>2</v>
+      </c>
+      <c r="J25" s="86">
+        <f>G25*I25</f>
+        <v>1.4</v>
+      </c>
+      <c r="K25" s="86">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L25" s="20">
+        <v>2</v>
+      </c>
+      <c r="M25" s="77">
+        <v>1</v>
+      </c>
+      <c r="N25" s="77">
+        <v>3</v>
+      </c>
+      <c r="O25" s="77">
+        <v>3</v>
+      </c>
+      <c r="P25" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="81">
+        <f>ROUND(((L25*M25*N25*O25)/81*3), 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="R25" s="77">
+        <v>2</v>
+      </c>
+      <c r="S25" s="86">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="20">
+        <v>1</v>
+      </c>
+      <c r="C26" s="77">
+        <v>1</v>
+      </c>
+      <c r="D26" s="77">
+        <v>2</v>
+      </c>
+      <c r="E26" s="77">
+        <v>2</v>
+      </c>
+      <c r="F26" s="82">
+        <v>2</v>
+      </c>
+      <c r="G26" s="81">
+        <f>ROUND(((B26*C26*D26*E26)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="81">
+        <f>ROUND(((B26+C26+D26+E26)/4), 1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I26" s="10">
+        <v>4</v>
+      </c>
+      <c r="J26" s="86">
+        <f>G26*I26</f>
+        <v>0.4</v>
+      </c>
+      <c r="K26" s="86">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L26" s="20">
+        <v>1</v>
+      </c>
+      <c r="M26" s="77">
+        <v>1</v>
+      </c>
+      <c r="N26" s="77">
+        <v>2</v>
+      </c>
+      <c r="O26" s="77">
+        <v>1</v>
+      </c>
+      <c r="P26" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="81">
+        <f>ROUND(((L26*M26*N26*O26)/81*3), 1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="R26" s="77">
+        <v>4</v>
+      </c>
+      <c r="S26" s="86">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="U26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="20">
+        <v>1</v>
+      </c>
+      <c r="C27" s="77">
+        <v>1</v>
+      </c>
+      <c r="D27" s="77">
+        <v>2</v>
+      </c>
+      <c r="E27" s="77">
+        <v>3</v>
+      </c>
+      <c r="F27" s="82">
+        <v>1</v>
+      </c>
+      <c r="G27" s="81">
+        <f>ROUND(((B27*C27*D27*E27)/81*3), 1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H27" s="81">
+        <f>ROUND(((B27+C27+D27+E27)/4), 1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="I27" s="10">
+        <v>4</v>
+      </c>
+      <c r="J27" s="86">
+        <f>G27*I27</f>
+        <v>0.8</v>
+      </c>
+      <c r="K27" s="86">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="L27" s="20">
+        <v>1</v>
+      </c>
+      <c r="M27" s="77">
+        <v>1</v>
+      </c>
+      <c r="N27" s="77">
+        <v>2</v>
+      </c>
+      <c r="O27" s="77">
+        <v>3</v>
+      </c>
+      <c r="P27" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="81">
+        <f>ROUND(((L27*M27*N27*O27)/81*3), 1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="R27" s="77">
+        <v>4</v>
+      </c>
+      <c r="S27" s="86">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="U27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="82">
+        <v>1</v>
+      </c>
+      <c r="G28" s="81">
+        <v>0</v>
+      </c>
+      <c r="H28" s="81">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
+        <v>4</v>
+      </c>
+      <c r="J28" s="86">
+        <f>G28*I28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="56">
+        <v>1</v>
+      </c>
+      <c r="M28" s="77">
+        <v>3</v>
+      </c>
+      <c r="N28" s="77">
+        <v>3</v>
+      </c>
+      <c r="O28" s="77">
+        <v>3</v>
+      </c>
+      <c r="P28" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="81">
+        <f>ROUND(((L28*M28*N28*O28)/81*3), 1)</f>
+        <v>1</v>
+      </c>
+      <c r="R28" s="77">
+        <v>4</v>
+      </c>
+      <c r="S28" s="86">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="20">
+        <v>2</v>
+      </c>
+      <c r="C29" s="77">
+        <v>2</v>
+      </c>
+      <c r="D29" s="77">
+        <v>3</v>
+      </c>
+      <c r="E29" s="77">
+        <v>3</v>
+      </c>
+      <c r="F29" s="82">
+        <v>2</v>
+      </c>
+      <c r="G29" s="81">
+        <f>ROUND(((B29*C29*D29*E29)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H29" s="81">
+        <f>ROUND(((B29+C29+D29+E29)/4), 1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I29" s="10">
+        <v>2</v>
+      </c>
+      <c r="J29" s="86">
+        <f>G29*I29</f>
+        <v>2.6</v>
+      </c>
+      <c r="K29" s="86">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L29" s="20">
+        <v>2</v>
+      </c>
+      <c r="M29" s="77">
+        <v>2</v>
+      </c>
+      <c r="N29" s="77">
+        <v>3</v>
+      </c>
+      <c r="O29" s="77">
+        <v>3</v>
+      </c>
+      <c r="P29" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="81">
+        <f>ROUND(((L29*M29*N29*O29)/81*3), 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="R29" s="77">
+        <v>2</v>
+      </c>
+      <c r="S29" s="86">
+        <f t="shared" si="1"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="85">
+        <v>4</v>
+      </c>
+      <c r="C30" s="80">
+        <v>4</v>
+      </c>
+      <c r="D30" s="80">
+        <v>3</v>
+      </c>
+      <c r="E30" s="80">
+        <v>3</v>
+      </c>
+      <c r="F30" s="83">
+        <v>3</v>
+      </c>
+      <c r="G30" s="12">
+        <f>ROUND(((B30*C30*D30*E30)/81*3), 1)</f>
+        <v>5.3</v>
+      </c>
+      <c r="H30" s="12">
+        <f>ROUND(((B30+C30+D30+E30)/4), 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="I30" s="12">
+        <v>4</v>
+      </c>
+      <c r="J30" s="5">
+        <f>G30*I30</f>
+        <v>21.2</v>
+      </c>
+      <c r="K30" s="86">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="L30" s="85">
+        <v>4</v>
+      </c>
+      <c r="M30" s="80">
+        <v>4</v>
+      </c>
+      <c r="N30" s="80">
+        <v>3</v>
+      </c>
+      <c r="O30" s="80">
+        <v>3</v>
+      </c>
+      <c r="P30" s="83">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="12">
+        <f>ROUND(((L30*M30*N30*O30)/81*3), 1)</f>
+        <v>5.3</v>
+      </c>
+      <c r="R30" s="80">
+        <v>4</v>
+      </c>
+      <c r="S30" s="5">
+        <f t="shared" si="1"/>
+        <v>21.2</v>
+      </c>
+      <c r="U30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="L32" s="74"/>
+      <c r="M32" s="74"/>
+      <c r="N32" s="74"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="67"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="L33" s="74"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="74"/>
+      <c r="P33" s="67"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="87" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="H35" s="81"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="S4:S30 J4:J30">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="H2" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="21"/>
+      <c r="H4" s="64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <f>(F21+G21+H21+I21)/4</f>
+        <v>2.75</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <f>K21*J21</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <f>(F22+G22+H22+I22)/4</f>
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <f>K22*J22</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A21" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
@@ -4042,317 +6422,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="H2" s="32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="21"/>
-      <c r="H4" s="64" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="H7" s="29"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="63" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="62" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E19" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" t="s">
-        <v>102</v>
-      </c>
-      <c r="K20" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-      <c r="J21">
-        <f>(F21+G21+H21+I21)/4</f>
-        <v>2.75</v>
-      </c>
-      <c r="K21">
-        <v>3</v>
-      </c>
-      <c r="L21">
-        <f>K21*J21</f>
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <f>(F22+G22+H22+I22)/4</f>
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <v>4</v>
-      </c>
-      <c r="L22">
-        <f>K22*J22</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31">
-        <v>3</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <v>3</v>
-      </c>
-      <c r="I32">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
risk assessment pre-markus feedback
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vector Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="ISFOXClassificationInKeywords" hidden="1">"Public"</definedName>
     <definedName name="ISFOXClassificationName" hidden="1">"Public"</definedName>
     <definedName name="ISFOXOldClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
-    <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
+    <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"00000000-0000-0000-0000-000000000000"</definedName>
     <definedName name="ISFOXPrefix" hidden="1">"HvS"</definedName>
     <definedName name="ISFOXPreviousClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXSaveAsProcess" hidden="1">TRUE</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="169">
   <si>
     <t>Attack Vectors Overview</t>
   </si>
@@ -547,6 +547,15 @@
   </si>
   <si>
     <t>probability simple est.</t>
+  </si>
+  <si>
+    <t>Range (nach Runden): 0 bis 21,3</t>
+  </si>
+  <si>
+    <t>0-7,1 / 7,2-14,2 / 14,3 - 21,3</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -863,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1080,10 +1089,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1104,7 +1131,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1372,7 +1399,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1727,7 +1754,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
@@ -2663,13 +2690,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
@@ -2688,16 +2715,18 @@
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" customWidth="1"/>
-    <col min="18" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="D2" s="66" t="s">
         <v>131</v>
@@ -2706,7 +2735,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>41</v>
       </c>
@@ -2728,7 +2757,7 @@
       <c r="G3" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="31" t="s">
         <v>162</v>
       </c>
       <c r="I3" s="68" t="s">
@@ -2737,7 +2766,7 @@
       <c r="J3" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="71" t="s">
+      <c r="K3" s="90" t="s">
         <v>163</v>
       </c>
       <c r="L3" s="68" t="s">
@@ -2758,14 +2787,23 @@
       <c r="Q3" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="68" t="s">
+      <c r="R3" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="S3" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="68" t="s">
+      <c r="T3" s="68" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U3" s="90" t="s">
+        <v>163</v>
+      </c>
+      <c r="V3" s="97" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -2785,52 +2823,64 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="81">
-        <f>ROUND(((B4*C4*D4*E4)/81*3), 1)</f>
+        <f>ROUND(((B4*C4*D4*E4)/81*3), 2)</f>
+        <v>0.22</v>
+      </c>
+      <c r="H4" s="94">
+        <f>ROUND(((B4+C4+D4+E4)/4), 2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="86">
+        <f>ROUND(G4*I4, 1)</f>
         <v>0.2</v>
       </c>
-      <c r="H4" s="88">
-        <f>ROUND(((B4+C4+D4+E4)/4), 1)</f>
+      <c r="K4" s="92">
+        <f>ROUND(H4*I4, 1)</f>
         <v>1.8</v>
       </c>
-      <c r="I4" s="10">
-        <v>1</v>
-      </c>
-      <c r="J4" s="86">
-        <f>G4*I4</f>
+      <c r="L4" s="84">
+        <v>1</v>
+      </c>
+      <c r="M4" s="81">
+        <v>1</v>
+      </c>
+      <c r="N4" s="81">
+        <v>3</v>
+      </c>
+      <c r="O4" s="81">
+        <v>2</v>
+      </c>
+      <c r="P4" s="82">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="88">
+        <f>ROUND(((L4*M4*N4*O4)/81*3), 2)</f>
+        <v>0.22</v>
+      </c>
+      <c r="R4" s="94">
+        <f>ROUND(((L4+M4+N4+O4)/4), 2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="S4" s="10">
+        <v>1</v>
+      </c>
+      <c r="T4" s="86">
+        <f>ROUND(Q4*S4, 1)</f>
         <v>0.2</v>
       </c>
-      <c r="K4" s="86">
-        <f>H4*I4</f>
+      <c r="U4" s="92">
+        <f>ROUND(R4*S4, 1)</f>
         <v>1.8</v>
       </c>
-      <c r="L4" s="84">
-        <v>1</v>
-      </c>
-      <c r="M4" s="81">
-        <v>1</v>
-      </c>
-      <c r="N4" s="81">
-        <v>3</v>
-      </c>
-      <c r="O4" s="81">
-        <v>2</v>
-      </c>
-      <c r="P4" s="82">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="88">
-        <f>ROUND(((L4*M4*N4*O4)/81*3), 1)</f>
-        <v>0.2</v>
-      </c>
-      <c r="R4" s="10">
-        <v>1</v>
-      </c>
-      <c r="S4" s="86">
-        <f>Q4*R4</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V4">
+        <f>K4-U4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2850,22 +2900,22 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="81">
-        <f>ROUND(((B5*C5*D5*E5)/81*3), 1)</f>
-        <v>0.3</v>
-      </c>
-      <c r="H5" s="81">
-        <f>ROUND(((B5+C5+D5+E5)/4), 1)</f>
+        <f t="shared" ref="G5:G30" si="0">ROUND(((B5*C5*D5*E5)/81*3), 2)</f>
+        <v>0.33</v>
+      </c>
+      <c r="H5" s="95">
+        <f t="shared" ref="H5:H30" si="1">ROUND(((B5+C5+D5+E5)/4), 2)</f>
         <v>2</v>
       </c>
       <c r="I5" s="10">
         <v>4</v>
       </c>
       <c r="J5" s="86">
-        <f>G5*I5</f>
-        <v>1.2</v>
-      </c>
-      <c r="K5" s="86">
-        <f t="shared" ref="K5:K30" si="0">H5*I5</f>
+        <f t="shared" ref="J5:J30" si="2">ROUND(G5*I5, 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="K5" s="92">
+        <f t="shared" ref="K5:K30" si="3">ROUND(H5*I5, 1)</f>
         <v>8</v>
       </c>
       <c r="L5" s="20">
@@ -2884,21 +2934,33 @@
         <v>1</v>
       </c>
       <c r="Q5" s="81">
-        <f>ROUND(((L5*M5*N5*O5)/81*3), 1)</f>
-        <v>0.3</v>
-      </c>
-      <c r="R5" s="10">
-        <v>4</v>
-      </c>
-      <c r="S5" s="86">
-        <f t="shared" ref="S5:S30" si="1">Q5*R5</f>
-        <v>1.2</v>
-      </c>
-      <c r="U5" t="s">
+        <f t="shared" ref="Q5:Q30" si="4">ROUND(((L5*M5*N5*O5)/81*3), 2)</f>
+        <v>0.33</v>
+      </c>
+      <c r="R5" s="95">
+        <f t="shared" ref="R5:R30" si="5">ROUND(((L5+M5+N5+O5)/4), 2)</f>
+        <v>2</v>
+      </c>
+      <c r="S5" s="10">
+        <v>4</v>
+      </c>
+      <c r="T5" s="86">
+        <f t="shared" ref="T5:T30" si="6">ROUND(Q5*S5, 1)</f>
+        <v>1.3</v>
+      </c>
+      <c r="U5" s="92">
+        <f t="shared" ref="U5:U30" si="7">ROUND(R5*S5, 1)</f>
+        <v>8</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V30" si="8">K5-U5</f>
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2918,22 +2980,22 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="81">
-        <f>ROUND(((B6*C6*D6*E6)/81*3), 1)</f>
-        <v>0.3</v>
-      </c>
-      <c r="H6" s="81">
-        <f>ROUND(((B6+C6+D6+E6)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="H6" s="95">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I6" s="10">
         <v>4</v>
       </c>
       <c r="J6" s="86">
-        <f>G6*I6</f>
-        <v>1.2</v>
-      </c>
-      <c r="K6" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
+      <c r="K6" s="92">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L6" s="20">
@@ -2952,21 +3014,33 @@
         <v>1</v>
       </c>
       <c r="Q6" s="81">
-        <f>ROUND(((L6*M6*N6*O6)/81*3), 1)</f>
-        <v>0.3</v>
-      </c>
-      <c r="R6" s="10">
-        <v>4</v>
-      </c>
-      <c r="S6" s="86">
-        <f t="shared" si="1"/>
-        <v>1.2</v>
-      </c>
-      <c r="U6" t="s">
+        <f t="shared" si="4"/>
+        <v>0.33</v>
+      </c>
+      <c r="R6" s="95">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="S6" s="10">
+        <v>4</v>
+      </c>
+      <c r="T6" s="86">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="U6" s="92">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -2986,58 +3060,70 @@
         <v>2</v>
       </c>
       <c r="G7" s="81">
-        <f>ROUND(((B7*C7*D7*E7)/81*3), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H7" s="95">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="86">
+        <f t="shared" si="2"/>
         <v>1.3</v>
       </c>
-      <c r="H7" s="81">
-        <f>ROUND(((B7+C7+D7+E7)/4), 1)</f>
+      <c r="K7" s="92">
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="I7" s="10">
-        <v>1</v>
-      </c>
-      <c r="J7" s="86">
-        <f>G7*I7</f>
+      <c r="L7" s="20">
+        <v>3</v>
+      </c>
+      <c r="M7" s="81">
+        <v>3</v>
+      </c>
+      <c r="N7" s="81">
+        <v>2</v>
+      </c>
+      <c r="O7" s="81">
+        <v>2</v>
+      </c>
+      <c r="P7" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="81">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R7" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S7" s="10">
+        <v>1</v>
+      </c>
+      <c r="T7" s="86">
+        <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="K7" s="86">
-        <f t="shared" si="0"/>
+      <c r="U7" s="92">
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="L7" s="20">
-        <v>3</v>
-      </c>
-      <c r="M7" s="81">
-        <v>3</v>
-      </c>
-      <c r="N7" s="81">
-        <v>2</v>
-      </c>
-      <c r="O7" s="81">
-        <v>2</v>
-      </c>
-      <c r="P7" s="82">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="81">
-        <f>ROUND(((L7*M7*N7*O7)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R7" s="10">
-        <v>1</v>
-      </c>
-      <c r="S7" s="86">
-        <f t="shared" si="1"/>
-        <v>1.3</v>
-      </c>
-      <c r="Y7" s="68" t="s">
+      <c r="V7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="Z7" s="27" t="s">
+      <c r="AB7" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -3057,23 +3143,23 @@
         <v>1</v>
       </c>
       <c r="G8" s="81">
-        <f>ROUND(((B8*C8*D8*E8)/81*3), 1)</f>
-        <v>0.9</v>
-      </c>
-      <c r="H8" s="81">
-        <f>ROUND(((B8+C8+D8+E8)/4), 1)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.89</v>
+      </c>
+      <c r="H8" s="95">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
       </c>
       <c r="I8" s="10">
         <v>4</v>
       </c>
       <c r="J8" s="86">
-        <f>G8*I8</f>
+        <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
-      <c r="K8" s="86">
-        <f t="shared" si="0"/>
-        <v>9.1999999999999993</v>
+      <c r="K8" s="92">
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
       <c r="L8" s="20">
         <v>2</v>
@@ -3091,27 +3177,39 @@
         <v>1</v>
       </c>
       <c r="Q8" s="81">
-        <f>ROUND(((L8*M8*N8*O8)/81*3), 1)</f>
-        <v>0.9</v>
-      </c>
-      <c r="R8" s="10">
-        <v>4</v>
-      </c>
-      <c r="S8" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
+        <v>0.89</v>
+      </c>
+      <c r="R8" s="95">
+        <f t="shared" si="5"/>
+        <v>2.25</v>
+      </c>
+      <c r="S8" s="10">
+        <v>4</v>
+      </c>
+      <c r="T8" s="86">
+        <f t="shared" si="6"/>
         <v>3.6</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="92">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
         <v>153</v>
       </c>
-      <c r="Y8" s="69" t="s">
+      <c r="AA8" s="69" t="s">
         <v>134</v>
       </c>
-      <c r="Z8" s="21" t="s">
+      <c r="AB8" s="21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -3131,22 +3229,22 @@
         <v>1</v>
       </c>
       <c r="G9" s="81">
-        <f>ROUND(((B9*C9*D9*E9)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H9" s="81">
-        <f>ROUND(((B9+C9+D9+E9)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="H9" s="95">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="I9" s="10">
         <v>4</v>
       </c>
       <c r="J9" s="86">
-        <f>G9*I9</f>
-        <v>0.4</v>
-      </c>
-      <c r="K9" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="K9" s="92">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L9" s="20">
@@ -3165,27 +3263,39 @@
         <v>1</v>
       </c>
       <c r="Q9" s="81">
-        <f>ROUND(((L9*M9*N9*O9)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="R9" s="10">
-        <v>4</v>
-      </c>
-      <c r="S9" s="86">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="U9" t="s">
+        <f t="shared" si="4"/>
+        <v>0.15</v>
+      </c>
+      <c r="R9" s="95">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="S9" s="10">
+        <v>4</v>
+      </c>
+      <c r="T9" s="86">
+        <f t="shared" si="6"/>
+        <v>0.6</v>
+      </c>
+      <c r="U9" s="92">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
         <v>153</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="AA9" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="Z9" s="21" t="s">
+      <c r="AB9" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
         <v>148</v>
       </c>
@@ -3205,22 +3315,22 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="81">
-        <f>ROUND(((B10*C10*D10*E10)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H10" s="81">
-        <f>ROUND(((B10+C10+D10+E10)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>0.11</v>
+      </c>
+      <c r="H10" s="95">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="I10" s="10">
         <v>4</v>
       </c>
       <c r="J10" s="86">
-        <f>G10*I10</f>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="K10" s="86">
-        <f t="shared" si="0"/>
+      <c r="K10" s="92">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L10" s="20">
@@ -3239,27 +3349,39 @@
         <v>0.5</v>
       </c>
       <c r="Q10" s="81">
-        <f>ROUND(((L10*M10*N10*O10)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="R10" s="10">
-        <v>4</v>
-      </c>
-      <c r="S10" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
+        <v>0.11</v>
+      </c>
+      <c r="R10" s="95">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="S10" s="10">
+        <v>4</v>
+      </c>
+      <c r="T10" s="86">
+        <f t="shared" si="6"/>
         <v>0.4</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="92">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W10" t="s">
         <v>153</v>
       </c>
-      <c r="Y10" s="4" t="s">
+      <c r="AA10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Z10" s="21" t="s">
+      <c r="AB10" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -3281,18 +3403,18 @@
       <c r="G11" s="81">
         <v>0</v>
       </c>
-      <c r="H11" s="81">
+      <c r="H11" s="95">
         <v>0</v>
       </c>
       <c r="I11" s="10">
         <v>1</v>
       </c>
       <c r="J11" s="86">
-        <f>G11*I11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K11" s="86">
-        <f t="shared" si="0"/>
+      <c r="K11" s="92">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L11" s="56">
@@ -3311,24 +3433,36 @@
         <v>2</v>
       </c>
       <c r="Q11" s="81">
-        <f>ROUND(((L11*M11*N11*O11)/81*3), 1)</f>
+        <f t="shared" si="4"/>
+        <v>1.78</v>
+      </c>
+      <c r="R11" s="95">
+        <f t="shared" si="5"/>
+        <v>2.75</v>
+      </c>
+      <c r="S11" s="10">
+        <v>1</v>
+      </c>
+      <c r="T11" s="86">
+        <f t="shared" si="6"/>
         <v>1.8</v>
       </c>
-      <c r="R11" s="10">
-        <v>1</v>
-      </c>
-      <c r="S11" s="86">
-        <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-      <c r="Y11" s="70" t="s">
+      <c r="U11" s="92">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="8"/>
+        <v>-2.8</v>
+      </c>
+      <c r="AA11" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="Z11" s="21" t="s">
+      <c r="AB11" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -3350,18 +3484,18 @@
       <c r="G12" s="81">
         <v>0</v>
       </c>
-      <c r="H12" s="81">
+      <c r="H12" s="95">
         <v>0</v>
       </c>
       <c r="I12" s="10">
         <v>4</v>
       </c>
       <c r="J12" s="86">
-        <f>G12*I12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K12" s="86">
-        <f t="shared" si="0"/>
+      <c r="K12" s="92">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="56">
@@ -3380,21 +3514,33 @@
         <v>1</v>
       </c>
       <c r="Q12" s="81">
-        <f>ROUND(((L12*M12*N12*O12)/81*3), 1)</f>
-        <v>2.7</v>
-      </c>
-      <c r="R12" s="10">
-        <v>4</v>
-      </c>
-      <c r="S12" s="86">
-        <f t="shared" si="1"/>
-        <v>10.8</v>
-      </c>
-      <c r="Z12" s="21" t="s">
+        <f t="shared" si="4"/>
+        <v>2.67</v>
+      </c>
+      <c r="R12" s="95">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="S12" s="10">
+        <v>4</v>
+      </c>
+      <c r="T12" s="86">
+        <f t="shared" si="6"/>
+        <v>10.7</v>
+      </c>
+      <c r="U12" s="92">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="AB12" s="21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -3416,18 +3562,18 @@
       <c r="G13" s="81">
         <v>0</v>
       </c>
-      <c r="H13" s="81">
+      <c r="H13" s="95">
         <v>0</v>
       </c>
       <c r="I13" s="10">
         <v>4</v>
       </c>
       <c r="J13" s="86">
-        <f>G13*I13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K13" s="86">
-        <f t="shared" si="0"/>
+      <c r="K13" s="92">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13" s="56">
@@ -3446,21 +3592,33 @@
         <v>1</v>
       </c>
       <c r="Q13" s="81">
-        <f>ROUND(((L13*M13*N13*O13)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R13" s="10">
-        <v>4</v>
-      </c>
-      <c r="S13" s="86">
-        <f t="shared" si="1"/>
-        <v>5.2</v>
-      </c>
-      <c r="Z13" s="65" t="s">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R13" s="95">
+        <f t="shared" si="5"/>
+        <v>2.75</v>
+      </c>
+      <c r="S13" s="10">
+        <v>4</v>
+      </c>
+      <c r="T13" s="86">
+        <f t="shared" si="6"/>
+        <v>5.3</v>
+      </c>
+      <c r="U13" s="92">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="AB13" s="65" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -3480,22 +3638,22 @@
         <v>3</v>
       </c>
       <c r="G14" s="81">
-        <f>ROUND(((B14*C14*D14*E14)/81*3), 1)</f>
-        <v>5.3</v>
-      </c>
-      <c r="H14" s="81">
-        <f>ROUND(((B14+C14+D14+E14)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>5.33</v>
+      </c>
+      <c r="H14" s="95">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="I14" s="10">
         <v>2</v>
       </c>
       <c r="J14" s="86">
-        <f>G14*I14</f>
-        <v>10.6</v>
-      </c>
-      <c r="K14" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>10.7</v>
+      </c>
+      <c r="K14" s="92">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L14" s="20">
@@ -3514,19 +3672,31 @@
         <v>3</v>
       </c>
       <c r="Q14" s="81">
-        <f>ROUND(((L14*M14*N14*O14)/81*3), 1)</f>
-        <v>5.3</v>
-      </c>
-      <c r="R14" s="77">
-        <v>2</v>
-      </c>
-      <c r="S14" s="86">
-        <f t="shared" si="1"/>
-        <v>10.6</v>
-      </c>
-      <c r="Z14" s="22"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>5.33</v>
+      </c>
+      <c r="R14" s="95">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
+      <c r="S14" s="77">
+        <v>2</v>
+      </c>
+      <c r="T14" s="86">
+        <f t="shared" si="6"/>
+        <v>10.7</v>
+      </c>
+      <c r="U14" s="92">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="22"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -3546,23 +3716,23 @@
         <v>2.5</v>
       </c>
       <c r="G15" s="81">
-        <f>ROUND(((B15*C15*D15*E15)/81*3), 1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="H15" s="81">
-        <f>ROUND(((B15+C15+D15+E15)/4), 1)</f>
-        <v>3.3</v>
+        <f t="shared" si="0"/>
+        <v>3.56</v>
+      </c>
+      <c r="H15" s="95">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
       </c>
       <c r="I15" s="10">
         <v>4</v>
       </c>
       <c r="J15" s="86">
-        <f>G15*I15</f>
-        <v>14.4</v>
-      </c>
-      <c r="K15" s="86">
-        <f t="shared" si="0"/>
-        <v>13.2</v>
+        <f t="shared" si="2"/>
+        <v>14.2</v>
+      </c>
+      <c r="K15" s="92">
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="L15" s="20">
         <v>4</v>
@@ -3580,24 +3750,36 @@
         <v>2.5</v>
       </c>
       <c r="Q15" s="81">
-        <f>ROUND(((L15*M15*N15*O15)/81*3), 1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="R15" s="77">
-        <v>4</v>
-      </c>
-      <c r="S15" s="86">
-        <f t="shared" si="1"/>
-        <v>14.4</v>
-      </c>
-      <c r="U15" t="s">
+        <f t="shared" si="4"/>
+        <v>3.56</v>
+      </c>
+      <c r="R15" s="95">
+        <f t="shared" si="5"/>
+        <v>3.25</v>
+      </c>
+      <c r="S15" s="77">
+        <v>4</v>
+      </c>
+      <c r="T15" s="86">
+        <f t="shared" si="6"/>
+        <v>14.2</v>
+      </c>
+      <c r="U15" s="92">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
         <v>153</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AB15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3617,22 +3799,22 @@
         <v>2</v>
       </c>
       <c r="G16" s="81">
-        <f>ROUND(((B16*C16*D16*E16)/81*3), 1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="H16" s="81">
-        <f>ROUND(((B16+C16+D16+E16)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="H16" s="95">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I16" s="10">
         <v>2</v>
       </c>
       <c r="J16" s="86">
-        <f>G16*I16</f>
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="K16" s="86">
-        <f t="shared" si="0"/>
+      <c r="K16" s="92">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L16" s="56">
@@ -3651,21 +3833,33 @@
         <v>2</v>
       </c>
       <c r="Q16" s="81">
-        <f>ROUND(((L16*M16*N16*O16)/81*3), 1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="R16" s="77">
-        <v>2</v>
-      </c>
-      <c r="S16" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
+        <v>0.59</v>
+      </c>
+      <c r="R16" s="95">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="S16" s="77">
+        <v>2</v>
+      </c>
+      <c r="T16" s="86">
+        <f t="shared" si="6"/>
         <v>1.2</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="U16" s="92">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>64</v>
       </c>
@@ -3685,22 +3879,22 @@
         <v>2</v>
       </c>
       <c r="G17" s="81">
-        <f>ROUND(((B17*C17*D17*E17)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="H17" s="81">
-        <f>ROUND(((B17+C17+D17+E17)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H17" s="95">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="I17" s="10">
         <v>4</v>
       </c>
       <c r="J17" s="86">
-        <f>G17*I17</f>
-        <v>5.2</v>
-      </c>
-      <c r="K17" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>5.3</v>
+      </c>
+      <c r="K17" s="92">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L17" s="20">
@@ -3719,24 +3913,36 @@
         <v>2</v>
       </c>
       <c r="Q17" s="81">
-        <f>ROUND(((L17*M17*N17*O17)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R17" s="77">
-        <v>4</v>
-      </c>
-      <c r="S17" s="86">
-        <f t="shared" si="1"/>
-        <v>5.2</v>
-      </c>
-      <c r="U17" t="s">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R17" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S17" s="77">
+        <v>4</v>
+      </c>
+      <c r="T17" s="86">
+        <f t="shared" si="6"/>
+        <v>5.3</v>
+      </c>
+      <c r="U17" s="92">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
         <v>153</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AB17" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -3756,22 +3962,22 @@
         <v>1</v>
       </c>
       <c r="G18" s="81">
-        <f>ROUND(((B18*C18*D18*E18)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="81">
-        <f>ROUND(((B18+C18+D18+E18)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="H18" s="95">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="I18" s="10">
         <v>2</v>
       </c>
       <c r="J18" s="86">
-        <f>G18*I18</f>
-        <v>0.2</v>
-      </c>
-      <c r="K18" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="K18" s="92">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L18" s="20">
@@ -3790,21 +3996,33 @@
         <v>1</v>
       </c>
       <c r="Q18" s="81">
-        <f>ROUND(((L18*M18*N18*O18)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="R18" s="77">
-        <v>2</v>
-      </c>
-      <c r="S18" s="86">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="Z18" t="s">
+        <f t="shared" si="4"/>
+        <v>0.15</v>
+      </c>
+      <c r="R18" s="95">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="S18" s="77">
+        <v>2</v>
+      </c>
+      <c r="T18" s="86">
+        <f t="shared" si="6"/>
+        <v>0.3</v>
+      </c>
+      <c r="U18" s="92">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -3824,22 +4042,22 @@
         <v>2</v>
       </c>
       <c r="G19" s="81">
-        <f>ROUND(((B19*C19*D19*E19)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="H19" s="81">
-        <f>ROUND(((B19+C19+D19+E19)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H19" s="95">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="I19" s="10">
         <v>4</v>
       </c>
       <c r="J19" s="86">
-        <f>G19*I19</f>
-        <v>5.2</v>
-      </c>
-      <c r="K19" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>5.3</v>
+      </c>
+      <c r="K19" s="92">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L19" s="20">
@@ -3858,24 +4076,36 @@
         <v>2</v>
       </c>
       <c r="Q19" s="81">
-        <f>ROUND(((L19*M19*N19*O19)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R19" s="77">
-        <v>4</v>
-      </c>
-      <c r="S19" s="86">
-        <f t="shared" si="1"/>
-        <v>5.2</v>
-      </c>
-      <c r="U19" t="s">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R19" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S19" s="77">
+        <v>4</v>
+      </c>
+      <c r="T19" s="86">
+        <f t="shared" si="6"/>
+        <v>5.3</v>
+      </c>
+      <c r="U19" s="92">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
         <v>153</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AB19" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>87</v>
       </c>
@@ -3895,22 +4125,22 @@
         <v>2</v>
       </c>
       <c r="G20" s="81">
-        <f>ROUND(((B20*C20*D20*E20)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="H20" s="81">
-        <f>ROUND(((B20+C20+D20+E20)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H20" s="95">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="I20" s="10">
         <v>2</v>
       </c>
       <c r="J20" s="86">
-        <f>G20*I20</f>
-        <v>2.6</v>
-      </c>
-      <c r="K20" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
+      <c r="K20" s="92">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L20" s="20">
@@ -3929,18 +4159,30 @@
         <v>2</v>
       </c>
       <c r="Q20" s="81">
-        <f>ROUND(((L20*M20*N20*O20)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R20" s="77">
-        <v>2</v>
-      </c>
-      <c r="S20" s="86">
-        <f t="shared" si="1"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R20" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S20" s="77">
+        <v>2</v>
+      </c>
+      <c r="T20" s="86">
+        <f t="shared" si="6"/>
+        <v>2.7</v>
+      </c>
+      <c r="U20" s="92">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -3960,52 +4202,64 @@
         <v>2</v>
       </c>
       <c r="G21" s="81">
-        <f>ROUND(((B21*C21*D21*E21)/81*3), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H21" s="95">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1</v>
+      </c>
+      <c r="J21" s="86">
+        <f t="shared" si="2"/>
         <v>1.3</v>
       </c>
-      <c r="H21" s="81">
-        <f>ROUND(((B21+C21+D21+E21)/4), 1)</f>
+      <c r="K21" s="92">
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="I21" s="10">
-        <v>1</v>
-      </c>
-      <c r="J21" s="86">
-        <f>G21*I21</f>
+      <c r="L21" s="20">
+        <v>2</v>
+      </c>
+      <c r="M21" s="77">
+        <v>2</v>
+      </c>
+      <c r="N21" s="77">
+        <v>3</v>
+      </c>
+      <c r="O21" s="77">
+        <v>3</v>
+      </c>
+      <c r="P21" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="81">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R21" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S21" s="77">
+        <v>1</v>
+      </c>
+      <c r="T21" s="86">
+        <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="K21" s="86">
-        <f t="shared" si="0"/>
+      <c r="U21" s="92">
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="L21" s="20">
-        <v>2</v>
-      </c>
-      <c r="M21" s="77">
-        <v>2</v>
-      </c>
-      <c r="N21" s="77">
-        <v>3</v>
-      </c>
-      <c r="O21" s="77">
-        <v>3</v>
-      </c>
-      <c r="P21" s="82">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="81">
-        <f>ROUND(((L21*M21*N21*O21)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R21" s="77">
-        <v>1</v>
-      </c>
-      <c r="S21" s="86">
-        <f t="shared" si="1"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -4025,52 +4279,64 @@
         <v>2</v>
       </c>
       <c r="G22" s="81">
-        <f>ROUND(((B22*C22*D22*E22)/81*3), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H22" s="95">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22" s="86">
+        <f t="shared" si="2"/>
         <v>1.3</v>
       </c>
-      <c r="H22" s="81">
-        <f>ROUND(((B22+C22+D22+E22)/4), 1)</f>
+      <c r="K22" s="92">
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="I22" s="10">
-        <v>1</v>
-      </c>
-      <c r="J22" s="86">
-        <f>G22*I22</f>
+      <c r="L22" s="20">
+        <v>2</v>
+      </c>
+      <c r="M22" s="77">
+        <v>2</v>
+      </c>
+      <c r="N22" s="77">
+        <v>3</v>
+      </c>
+      <c r="O22" s="77">
+        <v>3</v>
+      </c>
+      <c r="P22" s="82">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="81">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R22" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S22" s="77">
+        <v>1</v>
+      </c>
+      <c r="T22" s="86">
+        <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
-      <c r="K22" s="86">
-        <f t="shared" si="0"/>
+      <c r="U22" s="92">
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="L22" s="20">
-        <v>2</v>
-      </c>
-      <c r="M22" s="77">
-        <v>2</v>
-      </c>
-      <c r="N22" s="77">
-        <v>3</v>
-      </c>
-      <c r="O22" s="77">
-        <v>3</v>
-      </c>
-      <c r="P22" s="82">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="81">
-        <f>ROUND(((L22*M22*N22*O22)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R22" s="77">
-        <v>1</v>
-      </c>
-      <c r="S22" s="86">
-        <f t="shared" si="1"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -4090,23 +4356,23 @@
         <v>2</v>
       </c>
       <c r="G23" s="81">
-        <f>ROUND(((B23*C23*D23*E23)/81*3), 1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="H23" s="81">
-        <f>ROUND(((B23+C23+D23+E23)/4), 1)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.67</v>
+      </c>
+      <c r="H23" s="95">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
       </c>
       <c r="I23" s="10">
         <v>4</v>
       </c>
       <c r="J23" s="86">
-        <f>G23*I23</f>
-        <v>2.8</v>
-      </c>
-      <c r="K23" s="86">
-        <f t="shared" si="0"/>
-        <v>9.1999999999999993</v>
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
+      <c r="K23" s="92">
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
       <c r="L23" s="20">
         <v>1</v>
@@ -4124,21 +4390,33 @@
         <v>2</v>
       </c>
       <c r="Q23" s="81">
-        <f>ROUND(((L23*M23*N23*O23)/81*3), 1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="R23" s="77">
-        <v>2</v>
-      </c>
-      <c r="S23" s="86">
-        <f t="shared" si="1"/>
-        <v>1.4</v>
-      </c>
-      <c r="U23" t="s">
+        <f t="shared" si="4"/>
+        <v>0.67</v>
+      </c>
+      <c r="R23" s="95">
+        <f t="shared" si="5"/>
+        <v>2.25</v>
+      </c>
+      <c r="S23" s="77">
+        <v>2</v>
+      </c>
+      <c r="T23" s="86">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="U23" s="92">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="W23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -4158,23 +4436,23 @@
         <v>2</v>
       </c>
       <c r="G24" s="81">
-        <f>ROUND(((B24*C24*D24*E24)/81*3), 1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="H24" s="81">
-        <f>ROUND(((B24+C24+D24+E24)/4), 1)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.67</v>
+      </c>
+      <c r="H24" s="95">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
       </c>
       <c r="I24" s="10">
         <v>2</v>
       </c>
       <c r="J24" s="86">
-        <f>G24*I24</f>
-        <v>1.4</v>
-      </c>
-      <c r="K24" s="86">
-        <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
+      <c r="K24" s="92">
+        <f t="shared" si="3"/>
+        <v>4.5</v>
       </c>
       <c r="L24" s="20">
         <v>1</v>
@@ -4192,18 +4470,30 @@
         <v>2</v>
       </c>
       <c r="Q24" s="81">
-        <f>ROUND(((L24*M24*N24*O24)/81*3), 1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="R24" s="77">
-        <v>3</v>
-      </c>
-      <c r="S24" s="86">
-        <f t="shared" si="1"/>
-        <v>2.0999999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.67</v>
+      </c>
+      <c r="R24" s="95">
+        <f t="shared" si="5"/>
+        <v>2.25</v>
+      </c>
+      <c r="S24" s="77">
+        <v>3</v>
+      </c>
+      <c r="T24" s="86">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="U24" s="92">
+        <f t="shared" si="7"/>
+        <v>6.8</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="8"/>
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -4223,23 +4513,23 @@
         <v>1</v>
       </c>
       <c r="G25" s="81">
-        <f>ROUND(((B25*C25*D25*E25)/81*3), 1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="H25" s="81">
-        <f>ROUND(((B25+C25+D25+E25)/4), 1)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.67</v>
+      </c>
+      <c r="H25" s="95">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
       </c>
       <c r="I25" s="10">
         <v>2</v>
       </c>
       <c r="J25" s="86">
-        <f>G25*I25</f>
-        <v>1.4</v>
-      </c>
-      <c r="K25" s="86">
-        <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
+      <c r="K25" s="92">
+        <f t="shared" si="3"/>
+        <v>4.5</v>
       </c>
       <c r="L25" s="20">
         <v>2</v>
@@ -4257,18 +4547,30 @@
         <v>1</v>
       </c>
       <c r="Q25" s="81">
-        <f>ROUND(((L25*M25*N25*O25)/81*3), 1)</f>
-        <v>0.7</v>
-      </c>
-      <c r="R25" s="77">
-        <v>2</v>
-      </c>
-      <c r="S25" s="86">
-        <f t="shared" si="1"/>
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.67</v>
+      </c>
+      <c r="R25" s="95">
+        <f t="shared" si="5"/>
+        <v>2.25</v>
+      </c>
+      <c r="S25" s="77">
+        <v>2</v>
+      </c>
+      <c r="T25" s="86">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="U25" s="92">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
@@ -4288,22 +4590,22 @@
         <v>2</v>
       </c>
       <c r="G26" s="81">
-        <f>ROUND(((B26*C26*D26*E26)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H26" s="81">
-        <f>ROUND(((B26+C26+D26+E26)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="H26" s="95">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="I26" s="10">
         <v>4</v>
       </c>
       <c r="J26" s="86">
-        <f>G26*I26</f>
-        <v>0.4</v>
-      </c>
-      <c r="K26" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="K26" s="92">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L26" s="20">
@@ -4322,21 +4624,33 @@
         <v>1</v>
       </c>
       <c r="Q26" s="81">
-        <f>ROUND(((L26*M26*N26*O26)/81*3), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="R26" s="77">
-        <v>4</v>
-      </c>
-      <c r="S26" s="86">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="U26" t="s">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R26" s="95">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="S26" s="77">
+        <v>4</v>
+      </c>
+      <c r="T26" s="86">
+        <f t="shared" si="6"/>
+        <v>0.3</v>
+      </c>
+      <c r="U26" s="92">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="W26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>154</v>
       </c>
@@ -4356,23 +4670,23 @@
         <v>1</v>
       </c>
       <c r="G27" s="81">
-        <f>ROUND(((B27*C27*D27*E27)/81*3), 1)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H27" s="81">
-        <f>ROUND(((B27+C27+D27+E27)/4), 1)</f>
-        <v>1.8</v>
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="H27" s="95">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
       </c>
       <c r="I27" s="10">
         <v>4</v>
       </c>
       <c r="J27" s="86">
-        <f>G27*I27</f>
-        <v>0.8</v>
-      </c>
-      <c r="K27" s="86">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="K27" s="92">
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="L27" s="20">
         <v>1</v>
@@ -4390,21 +4704,33 @@
         <v>1</v>
       </c>
       <c r="Q27" s="81">
-        <f>ROUND(((L27*M27*N27*O27)/81*3), 1)</f>
-        <v>0.2</v>
-      </c>
-      <c r="R27" s="77">
-        <v>4</v>
-      </c>
-      <c r="S27" s="86">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="U27" t="s">
+        <f t="shared" si="4"/>
+        <v>0.22</v>
+      </c>
+      <c r="R27" s="95">
+        <f t="shared" si="5"/>
+        <v>1.75</v>
+      </c>
+      <c r="S27" s="77">
+        <v>4</v>
+      </c>
+      <c r="T27" s="86">
+        <f t="shared" si="6"/>
+        <v>0.9</v>
+      </c>
+      <c r="U27" s="92">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W27" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>155</v>
       </c>
@@ -4426,18 +4752,18 @@
       <c r="G28" s="81">
         <v>0</v>
       </c>
-      <c r="H28" s="81">
+      <c r="H28" s="95">
         <v>0</v>
       </c>
       <c r="I28" s="10">
         <v>4</v>
       </c>
       <c r="J28" s="86">
-        <f>G28*I28</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K28" s="86">
-        <f t="shared" si="0"/>
+      <c r="K28" s="92">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L28" s="56">
@@ -4456,18 +4782,30 @@
         <v>1</v>
       </c>
       <c r="Q28" s="81">
-        <f>ROUND(((L28*M28*N28*O28)/81*3), 1)</f>
-        <v>1</v>
-      </c>
-      <c r="R28" s="77">
-        <v>4</v>
-      </c>
-      <c r="S28" s="86">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R28" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S28" s="77">
+        <v>4</v>
+      </c>
+      <c r="T28" s="86">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="U28" s="92">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>149</v>
       </c>
@@ -4487,22 +4825,22 @@
         <v>2</v>
       </c>
       <c r="G29" s="81">
-        <f>ROUND(((B29*C29*D29*E29)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="H29" s="81">
-        <f>ROUND(((B29+C29+D29+E29)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>1.33</v>
+      </c>
+      <c r="H29" s="95">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="I29" s="10">
         <v>2</v>
       </c>
       <c r="J29" s="86">
-        <f>G29*I29</f>
-        <v>2.6</v>
-      </c>
-      <c r="K29" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
+      <c r="K29" s="92">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L29" s="20">
@@ -4521,18 +4859,30 @@
         <v>2</v>
       </c>
       <c r="Q29" s="81">
-        <f>ROUND(((L29*M29*N29*O29)/81*3), 1)</f>
-        <v>1.3</v>
-      </c>
-      <c r="R29" s="77">
-        <v>2</v>
-      </c>
-      <c r="S29" s="86">
-        <f t="shared" si="1"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="R29" s="95">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="S29" s="77">
+        <v>2</v>
+      </c>
+      <c r="T29" s="86">
+        <f t="shared" si="6"/>
+        <v>2.7</v>
+      </c>
+      <c r="U29" s="92">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="70" t="s">
         <v>150</v>
       </c>
@@ -4552,22 +4902,22 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <f>ROUND(((B30*C30*D30*E30)/81*3), 1)</f>
-        <v>5.3</v>
-      </c>
-      <c r="H30" s="12">
-        <f>ROUND(((B30+C30+D30+E30)/4), 1)</f>
+        <f t="shared" si="0"/>
+        <v>5.33</v>
+      </c>
+      <c r="H30" s="96">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="I30" s="12">
         <v>4</v>
       </c>
       <c r="J30" s="5">
-        <f>G30*I30</f>
-        <v>21.2</v>
-      </c>
-      <c r="K30" s="86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>21.3</v>
+      </c>
+      <c r="K30" s="93">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="L30" s="85">
@@ -4586,21 +4936,33 @@
         <v>2</v>
       </c>
       <c r="Q30" s="12">
-        <f>ROUND(((L30*M30*N30*O30)/81*3), 1)</f>
-        <v>5.3</v>
-      </c>
-      <c r="R30" s="80">
-        <v>4</v>
-      </c>
-      <c r="S30" s="5">
-        <f t="shared" si="1"/>
-        <v>21.2</v>
-      </c>
-      <c r="U30" t="s">
+        <f t="shared" si="4"/>
+        <v>5.33</v>
+      </c>
+      <c r="R30" s="96">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
+      <c r="S30" s="80">
+        <v>4</v>
+      </c>
+      <c r="T30" s="5">
+        <f t="shared" si="6"/>
+        <v>21.3</v>
+      </c>
+      <c r="U30" s="93">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W30" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="87" t="s">
         <v>152</v>
       </c>
@@ -4610,7 +4972,7 @@
       <c r="O32" s="74"/>
       <c r="P32" s="67"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="87" t="s">
         <v>151</v>
       </c>
@@ -4620,40 +4982,61 @@
       <c r="O33" s="74"/>
       <c r="P33" s="67"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="87" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="89" t="s">
         <v>164</v>
       </c>
       <c r="H35" s="81"/>
+      <c r="R35" s="81"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="89" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S4:S30 J4:J30">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="J4:J30">
+    <cfRule type="iconSet" priority="4">
+      <iconSet reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7.2"/>
+        <cfvo type="num" val="14.3"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T30">
+    <cfRule type="iconSet" priority="3">
+      <iconSet reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7.2"/>
+        <cfvo type="num" val="14.3"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K30">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+    <cfRule type="iconSet" priority="2">
+      <iconSet reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="4.5999999999999996"/>
+        <cfvo type="num" val="9.3000000000000007"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:U30">
+    <cfRule type="iconSet" priority="1">
+      <iconSet reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="4.5999999999999996"/>
+        <cfvo type="num" val="9.3000000000000007"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4665,11 +5048,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
@@ -4982,7 +5365,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="10" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
implemented Markus feedback round 2, decoupled multi-tenant influence
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vector Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Vectors simple" sheetId="4" r:id="rId2"/>
-    <sheet name="Vectors detailed" sheetId="5" r:id="rId3"/>
-    <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
+    <sheet name="Vectors detailed" sheetId="5" r:id="rId2"/>
+    <sheet name="Risk assessment formula" sheetId="2" r:id="rId3"/>
+    <sheet name="Vectors simple" sheetId="4" r:id="rId4"/>
     <sheet name="Vector Details_OLD" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="171">
   <si>
     <t>Attack Vectors Overview</t>
   </si>
@@ -324,12 +324,6 @@
     <t>unauthenticated (4)</t>
   </si>
   <si>
-    <t>read only (3)</t>
-  </si>
-  <si>
-    <t>cluster/system user (2)</t>
-  </si>
-  <si>
     <t>cluster/system admin (1)</t>
   </si>
   <si>
@@ -381,15 +375,9 @@
     <t>Unpublished 0-Days = Theoretical</t>
   </si>
   <si>
-    <t>Multi-tenant pwning = Severe</t>
-  </si>
-  <si>
     <t>Intermediate Step = Low</t>
   </si>
   <si>
-    <t>Single-Tenant pwning = Moderate</t>
-  </si>
-  <si>
     <t>Range: 0,25 - 3,5 (  0,25-1,25 Low; 1,5-2,25 Medium; 2,5-3,5  High )</t>
   </si>
   <si>
@@ -513,28 +501,67 @@
     <t>entry through known, unpatched vulnerabilities</t>
   </si>
   <si>
-    <t>^Risk = ROUND( (Probability * Impact) /14 * 10 )</t>
-  </si>
-  <si>
-    <t>Range: 0 - 10 ( 0-3 Low; 4-7 Medium; 8-10 High )</t>
-  </si>
-  <si>
-    <t>Reconaissance through dashboard, kubelets, k8s-/cloud-apiserver</t>
-  </si>
-  <si>
-    <t>Read confidentials through dashboard, kubelets, k8s-apiserver</t>
-  </si>
-  <si>
-    <t>Change configuration through dashboard,  k8s-apiserver, kubelets</t>
-  </si>
-  <si>
-    <t>breakout or R/W to host, Privilege Escalation</t>
-  </si>
-  <si>
-    <t>gain persistence in k8s control plane / cloud mgmt</t>
-  </si>
-  <si>
-    <t>(Range normalised to 0 through 10)</t>
+    <t>add malicious container</t>
+  </si>
+  <si>
+    <t>add malicious node</t>
+  </si>
+  <si>
+    <t>Incufficient base infrastructure hardening</t>
+  </si>
+  <si>
+    <t>Bad user practice (outside of cluster)</t>
+  </si>
+  <si>
+    <t>misuse node resources (DOS, cryptojacking)</t>
+  </si>
+  <si>
+    <t>compromise application components (lateral movement from container)</t>
+  </si>
+  <si>
+    <t>cluster/system user (read) (2)</t>
+  </si>
+  <si>
+    <t>cluster/system user (R/W) (2)</t>
+  </si>
+  <si>
+    <t>&lt;- less multi-tenant impact on cluster split</t>
+  </si>
+  <si>
+    <t>&lt;- On-Prem:  less multi-tenant impact on cluster split</t>
+  </si>
+  <si>
+    <t>Reconaissance through k8s control plane &amp; cloud provider interfaces</t>
+  </si>
+  <si>
+    <t>Read confidentials through cloud provider interfaces (mgmt console/API)</t>
+  </si>
+  <si>
+    <t>Change configuration through  cloud provider interfaces (mgmt console/API)</t>
+  </si>
+  <si>
+    <t>Compromise internal k8s control plane components (etcd, scheduler, controller-manager)</t>
+  </si>
+  <si>
+    <t>Change configuration through k8s control plane interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R/W &amp; breakout to host, Privilege Escalation</t>
+  </si>
+  <si>
+    <t>Read confidentials through k8s control plane interfaces (dashboard, apiserver)</t>
+  </si>
+  <si>
+    <t>Severe security principle violation = Severe</t>
+  </si>
+  <si>
+    <t>Non-severe security principle violation = Moderate</t>
+  </si>
+  <si>
+    <t>^Risk = Probability * Impact, rounded to 0.1 intervals, capped at 10</t>
+  </si>
+  <si>
+    <t>Range: 0 - 10 ( 0-3 Low; 4-6 Medium; 7-10 High )</t>
   </si>
 </sst>
 </file>
@@ -630,7 +657,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -837,12 +864,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1032,9 +1068,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1057,6 +1090,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1347,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,6 +1741,1531 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="73.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="10"/>
+      <c r="D2" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="95" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="82">
+        <v>3</v>
+      </c>
+      <c r="C4" s="94">
+        <v>3</v>
+      </c>
+      <c r="D4" s="81">
+        <v>2</v>
+      </c>
+      <c r="E4" s="81">
+        <v>2</v>
+      </c>
+      <c r="F4" s="90">
+        <f>ROUND(((C4+B4+D4+E4)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
+      <c r="H4" s="88">
+        <f>MIN(10, ROUND(F4*G4, 1))</f>
+        <v>2.5</v>
+      </c>
+      <c r="I4" s="81">
+        <v>3</v>
+      </c>
+      <c r="J4" s="94">
+        <v>3</v>
+      </c>
+      <c r="K4" s="81">
+        <v>2</v>
+      </c>
+      <c r="L4" s="81">
+        <v>2</v>
+      </c>
+      <c r="M4" s="90">
+        <f>ROUND(((J4+I4+K4+L4)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="88">
+        <f>MIN(10, ROUND(M4*N4, 1))</f>
+        <v>2.5</v>
+      </c>
+      <c r="P4">
+        <f>H4-O4</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="20">
+        <v>3</v>
+      </c>
+      <c r="C5" s="81">
+        <v>2</v>
+      </c>
+      <c r="D5" s="77">
+        <v>2</v>
+      </c>
+      <c r="E5" s="77">
+        <v>2</v>
+      </c>
+      <c r="F5" s="56">
+        <f>ROUND(((C5+B5+D5+E5)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="G5" s="10">
+        <v>3</v>
+      </c>
+      <c r="H5" s="88">
+        <f t="shared" ref="H5:H23" si="0">MIN(10, ROUND(F5*G5, 1))</f>
+        <v>6.8</v>
+      </c>
+      <c r="I5" s="81">
+        <v>3</v>
+      </c>
+      <c r="J5" s="81">
+        <v>2</v>
+      </c>
+      <c r="K5" s="77">
+        <v>2</v>
+      </c>
+      <c r="L5" s="77">
+        <v>2</v>
+      </c>
+      <c r="M5" s="56">
+        <f>ROUND(((J5+I5+K5+L5)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="N5" s="10">
+        <v>3</v>
+      </c>
+      <c r="O5" s="88">
+        <f t="shared" ref="O5:O23" si="1">MIN(10, ROUND(M5*N5, 1))</f>
+        <v>6.8</v>
+      </c>
+      <c r="P5">
+        <f>H5-O5</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="20">
+        <v>3</v>
+      </c>
+      <c r="C6" s="81">
+        <v>1</v>
+      </c>
+      <c r="D6" s="81">
+        <v>3</v>
+      </c>
+      <c r="E6" s="81">
+        <v>3</v>
+      </c>
+      <c r="F6" s="56">
+        <f>ROUND(((C6+B6+D6+E6)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="88">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="I6" s="81">
+        <v>3</v>
+      </c>
+      <c r="J6" s="81">
+        <v>1</v>
+      </c>
+      <c r="K6" s="81">
+        <v>3</v>
+      </c>
+      <c r="L6" s="81">
+        <v>3</v>
+      </c>
+      <c r="M6" s="56">
+        <f>ROUND(((J6+I6+K6+L6)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N6" s="10">
+        <v>3</v>
+      </c>
+      <c r="O6" s="88">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="P6">
+        <f>H6-O6</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="81" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F7" s="56">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>3</v>
+      </c>
+      <c r="H7" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="77">
+        <v>4</v>
+      </c>
+      <c r="J7" s="77">
+        <v>2</v>
+      </c>
+      <c r="K7" s="77">
+        <v>3</v>
+      </c>
+      <c r="L7" s="77">
+        <v>3</v>
+      </c>
+      <c r="M7" s="56">
+        <f>ROUND(((J7+I7+K7+L7)/4), 2)</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="10">
+        <v>3</v>
+      </c>
+      <c r="O7" s="88">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P7">
+        <f>H7-O7</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="56">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>3</v>
+      </c>
+      <c r="H8" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="77">
+        <v>4</v>
+      </c>
+      <c r="J8" s="77">
+        <v>1</v>
+      </c>
+      <c r="K8" s="77">
+        <v>3</v>
+      </c>
+      <c r="L8" s="77">
+        <v>3</v>
+      </c>
+      <c r="M8" s="56">
+        <f>ROUND(((J8+I8+K8+L8)/4), 2)</f>
+        <v>2.75</v>
+      </c>
+      <c r="N8" s="10">
+        <v>3</v>
+      </c>
+      <c r="O8" s="88">
+        <f t="shared" si="1"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P8">
+        <f>H8-O8</f>
+        <v>-8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="20">
+        <v>3</v>
+      </c>
+      <c r="C9" s="81">
+        <v>1</v>
+      </c>
+      <c r="D9" s="81">
+        <v>1</v>
+      </c>
+      <c r="E9" s="81">
+        <v>0</v>
+      </c>
+      <c r="F9" s="56">
+        <f>ROUND(((C9+B9+D9+E9)/4), 2)</f>
+        <v>1.25</v>
+      </c>
+      <c r="G9" s="10">
+        <v>3</v>
+      </c>
+      <c r="H9" s="88">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="I9" s="81">
+        <v>3</v>
+      </c>
+      <c r="J9" s="81">
+        <v>1</v>
+      </c>
+      <c r="K9" s="81">
+        <v>1</v>
+      </c>
+      <c r="L9" s="81">
+        <v>0</v>
+      </c>
+      <c r="M9" s="56">
+        <f>ROUND(((J9+I9+K9+L9)/4), 2)</f>
+        <v>1.25</v>
+      </c>
+      <c r="N9" s="10">
+        <v>3</v>
+      </c>
+      <c r="O9" s="88">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+      <c r="P9">
+        <f>H9-O9</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="20">
+        <v>4</v>
+      </c>
+      <c r="C10" s="81">
+        <v>4</v>
+      </c>
+      <c r="D10" s="81">
+        <v>3</v>
+      </c>
+      <c r="E10" s="81">
+        <v>3</v>
+      </c>
+      <c r="F10" s="56">
+        <f>ROUND(((C10+B10+D10+E10)/4), 2)</f>
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="88">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I10" s="81">
+        <v>4</v>
+      </c>
+      <c r="J10" s="81">
+        <v>4</v>
+      </c>
+      <c r="K10" s="81">
+        <v>3</v>
+      </c>
+      <c r="L10" s="81">
+        <v>3</v>
+      </c>
+      <c r="M10" s="56">
+        <f>ROUND(((J10+I10+K10+L10)/4), 2)</f>
+        <v>3.5</v>
+      </c>
+      <c r="N10" s="77">
+        <v>2</v>
+      </c>
+      <c r="O10" s="88">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <f>H10-O10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="20">
+        <v>4</v>
+      </c>
+      <c r="C11" s="81">
+        <v>4</v>
+      </c>
+      <c r="D11" s="81">
+        <v>3</v>
+      </c>
+      <c r="E11" s="81">
+        <v>2</v>
+      </c>
+      <c r="F11" s="56">
+        <f>ROUND(((C11+B11+D11+E11)/4), 2)</f>
+        <v>3.25</v>
+      </c>
+      <c r="G11" s="10">
+        <v>3</v>
+      </c>
+      <c r="H11" s="88">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I11" s="81">
+        <v>4</v>
+      </c>
+      <c r="J11" s="81">
+        <v>4</v>
+      </c>
+      <c r="K11" s="81">
+        <v>3</v>
+      </c>
+      <c r="L11" s="81">
+        <v>2</v>
+      </c>
+      <c r="M11" s="56">
+        <f>ROUND(((J11+I11+K11+L11)/4), 2)</f>
+        <v>3.25</v>
+      </c>
+      <c r="N11" s="77">
+        <v>3</v>
+      </c>
+      <c r="O11" s="88">
+        <f t="shared" si="1"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="P11">
+        <f>H11-O11</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="20">
+        <v>2</v>
+      </c>
+      <c r="C12" s="77">
+        <v>2</v>
+      </c>
+      <c r="D12" s="81">
+        <v>2</v>
+      </c>
+      <c r="E12" s="81">
+        <v>2</v>
+      </c>
+      <c r="F12" s="56">
+        <f>ROUND(((C12+B12+D12+E12)/4), 2)</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2</v>
+      </c>
+      <c r="H12" s="88">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I12" s="81">
+        <v>2</v>
+      </c>
+      <c r="J12" s="77">
+        <v>2</v>
+      </c>
+      <c r="K12" s="81">
+        <v>2</v>
+      </c>
+      <c r="L12" s="81">
+        <v>2</v>
+      </c>
+      <c r="M12" s="56">
+        <f>ROUND(((J12+I12+K12+L12)/4), 2)</f>
+        <v>2</v>
+      </c>
+      <c r="N12" s="77">
+        <v>2</v>
+      </c>
+      <c r="O12" s="88">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <f>H12-O12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="91" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="56">
+        <v>2</v>
+      </c>
+      <c r="C13" s="81">
+        <v>3</v>
+      </c>
+      <c r="D13" s="77">
+        <v>3</v>
+      </c>
+      <c r="E13" s="77">
+        <v>2</v>
+      </c>
+      <c r="F13" s="56">
+        <f>ROUND(((C13+B13+D13+E13)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="10">
+        <v>3</v>
+      </c>
+      <c r="H13" s="88">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="I13" s="77">
+        <v>2</v>
+      </c>
+      <c r="J13" s="81">
+        <v>3</v>
+      </c>
+      <c r="K13" s="77">
+        <v>3</v>
+      </c>
+      <c r="L13" s="77">
+        <v>2</v>
+      </c>
+      <c r="M13" s="56">
+        <f>ROUND(((J13+I13+K13+L13)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N13" s="77">
+        <v>3</v>
+      </c>
+      <c r="O13" s="88">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="P13">
+        <f>H13-O13</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20">
+        <v>1</v>
+      </c>
+      <c r="C14" s="81">
+        <v>2</v>
+      </c>
+      <c r="D14" s="81">
+        <v>2</v>
+      </c>
+      <c r="E14" s="81">
+        <v>1</v>
+      </c>
+      <c r="F14" s="56">
+        <f>ROUND(((C14+B14+D14+E14)/4), 2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2</v>
+      </c>
+      <c r="H14" s="88">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I14" s="81">
+        <v>1</v>
+      </c>
+      <c r="J14" s="81">
+        <v>2</v>
+      </c>
+      <c r="K14" s="81">
+        <v>2</v>
+      </c>
+      <c r="L14" s="81">
+        <v>1</v>
+      </c>
+      <c r="M14" s="56">
+        <f>ROUND(((J14+I14+K14+L14)/4), 2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N14" s="77">
+        <v>2</v>
+      </c>
+      <c r="O14" s="88">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <f>H14-O14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="92" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="56">
+        <v>2</v>
+      </c>
+      <c r="C15" s="81">
+        <v>2</v>
+      </c>
+      <c r="D15" s="77">
+        <v>3</v>
+      </c>
+      <c r="E15" s="77">
+        <v>3</v>
+      </c>
+      <c r="F15" s="56">
+        <f>ROUND(((C15+B15+D15+E15)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="10">
+        <v>2</v>
+      </c>
+      <c r="H15" s="88">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I15" s="77">
+        <v>2</v>
+      </c>
+      <c r="J15" s="81">
+        <v>2</v>
+      </c>
+      <c r="K15" s="77">
+        <v>3</v>
+      </c>
+      <c r="L15" s="77">
+        <v>3</v>
+      </c>
+      <c r="M15" s="56">
+        <f>ROUND(((J15+I15+K15+L15)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N15" s="77">
+        <v>2</v>
+      </c>
+      <c r="O15" s="88">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <f>H15-O15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="91" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="56">
+        <v>2</v>
+      </c>
+      <c r="C16" s="81">
+        <v>2</v>
+      </c>
+      <c r="D16" s="77">
+        <v>3</v>
+      </c>
+      <c r="E16" s="77">
+        <v>3</v>
+      </c>
+      <c r="F16" s="56">
+        <f>ROUND(((C16+B16+D16+E16)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1</v>
+      </c>
+      <c r="H16" s="88">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="I16" s="77">
+        <v>2</v>
+      </c>
+      <c r="J16" s="81">
+        <v>2</v>
+      </c>
+      <c r="K16" s="77">
+        <v>3</v>
+      </c>
+      <c r="L16" s="77">
+        <v>3</v>
+      </c>
+      <c r="M16" s="56">
+        <f>ROUND(((J16+I16+K16+L16)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N16" s="77">
+        <v>1</v>
+      </c>
+      <c r="O16" s="88">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="P16">
+        <f>H16-O16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="56">
+        <v>2</v>
+      </c>
+      <c r="C17" s="81">
+        <v>1</v>
+      </c>
+      <c r="D17" s="77">
+        <v>3</v>
+      </c>
+      <c r="E17" s="77">
+        <v>3</v>
+      </c>
+      <c r="F17" s="56">
+        <f>ROUND(((C17+B17+D17+E17)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="G17" s="10">
+        <v>3</v>
+      </c>
+      <c r="H17" s="88">
+        <f t="shared" si="0"/>
+        <v>6.8</v>
+      </c>
+      <c r="I17" s="77">
+        <v>2</v>
+      </c>
+      <c r="J17" s="81">
+        <v>1</v>
+      </c>
+      <c r="K17" s="77">
+        <v>3</v>
+      </c>
+      <c r="L17" s="77">
+        <v>3</v>
+      </c>
+      <c r="M17" s="56">
+        <f>ROUND(((J17+I17+K17+L17)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="N17" s="77">
+        <v>2</v>
+      </c>
+      <c r="O17" s="88">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="P17">
+        <f>H17-O17</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="56">
+        <v>2</v>
+      </c>
+      <c r="C18" s="81">
+        <v>1</v>
+      </c>
+      <c r="D18" s="77">
+        <v>3</v>
+      </c>
+      <c r="E18" s="77">
+        <v>3</v>
+      </c>
+      <c r="F18" s="56">
+        <f>ROUND(((C18+B18+D18+E18)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2</v>
+      </c>
+      <c r="H18" s="88">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="I18" s="77">
+        <v>2</v>
+      </c>
+      <c r="J18" s="81">
+        <v>1</v>
+      </c>
+      <c r="K18" s="77">
+        <v>3</v>
+      </c>
+      <c r="L18" s="77">
+        <v>3</v>
+      </c>
+      <c r="M18" s="56">
+        <f>ROUND(((J18+I18+K18+L18)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="N18" s="77">
+        <v>3</v>
+      </c>
+      <c r="O18" s="88">
+        <f t="shared" si="1"/>
+        <v>6.8</v>
+      </c>
+      <c r="P18">
+        <f>H18-O18</f>
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="91" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="56">
+        <v>1</v>
+      </c>
+      <c r="C19" s="81">
+        <v>2</v>
+      </c>
+      <c r="D19" s="77">
+        <v>3</v>
+      </c>
+      <c r="E19" s="77">
+        <v>3</v>
+      </c>
+      <c r="F19" s="56">
+        <f>ROUND(((C19+B19+D19+E19)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2</v>
+      </c>
+      <c r="H19" s="88">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="I19" s="77">
+        <v>1</v>
+      </c>
+      <c r="J19" s="81">
+        <v>2</v>
+      </c>
+      <c r="K19" s="77">
+        <v>3</v>
+      </c>
+      <c r="L19" s="77">
+        <v>3</v>
+      </c>
+      <c r="M19" s="56">
+        <f>ROUND(((J19+I19+K19+L19)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="N19" s="77">
+        <v>2</v>
+      </c>
+      <c r="O19" s="88">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="P19">
+        <f>H19-O19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="91" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="56">
+        <v>1</v>
+      </c>
+      <c r="C20" s="81">
+        <v>1</v>
+      </c>
+      <c r="D20" s="77">
+        <v>2</v>
+      </c>
+      <c r="E20" s="77">
+        <v>2</v>
+      </c>
+      <c r="F20" s="56">
+        <f>ROUND(((C20+B20+D20+E20)/4), 2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="G20" s="10">
+        <v>3</v>
+      </c>
+      <c r="H20" s="88">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="I20" s="77">
+        <v>1</v>
+      </c>
+      <c r="J20" s="81">
+        <v>1</v>
+      </c>
+      <c r="K20" s="77">
+        <v>2</v>
+      </c>
+      <c r="L20" s="77">
+        <v>1</v>
+      </c>
+      <c r="M20" s="56">
+        <f>ROUND(((J20+I20+K20+L20)/4), 2)</f>
+        <v>1.25</v>
+      </c>
+      <c r="N20" s="77">
+        <v>3</v>
+      </c>
+      <c r="O20" s="88">
+        <f t="shared" si="1"/>
+        <v>3.8</v>
+      </c>
+      <c r="P20">
+        <f>H20-O20</f>
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="91" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="56">
+        <v>4</v>
+      </c>
+      <c r="C21" s="81">
+        <v>4</v>
+      </c>
+      <c r="D21" s="77">
+        <v>1</v>
+      </c>
+      <c r="E21" s="77">
+        <v>2</v>
+      </c>
+      <c r="F21" s="56">
+        <f>ROUND(((C21+B21+D21+E21)/4), 2)</f>
+        <v>2.75</v>
+      </c>
+      <c r="G21" s="10">
+        <v>3</v>
+      </c>
+      <c r="H21" s="88">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I21" s="77">
+        <v>4</v>
+      </c>
+      <c r="J21" s="81">
+        <v>4</v>
+      </c>
+      <c r="K21" s="77">
+        <v>1</v>
+      </c>
+      <c r="L21" s="77">
+        <v>2</v>
+      </c>
+      <c r="M21" s="56">
+        <f>ROUND(((J21+I21+K21+L21)/4), 2)</f>
+        <v>2.75</v>
+      </c>
+      <c r="N21" s="77">
+        <v>3</v>
+      </c>
+      <c r="O21" s="88">
+        <f t="shared" si="1"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P21">
+        <f>H21-O21</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="91" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="56">
+        <v>3</v>
+      </c>
+      <c r="C22" s="81">
+        <v>4</v>
+      </c>
+      <c r="D22" s="77">
+        <v>2</v>
+      </c>
+      <c r="E22" s="77">
+        <v>2</v>
+      </c>
+      <c r="F22" s="56">
+        <f>ROUND(((C22+B22+D22+E22)/4), 2)</f>
+        <v>2.75</v>
+      </c>
+      <c r="G22" s="10">
+        <v>3</v>
+      </c>
+      <c r="H22" s="88">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I22" s="77">
+        <v>3</v>
+      </c>
+      <c r="J22" s="81">
+        <v>4</v>
+      </c>
+      <c r="K22" s="77">
+        <v>2</v>
+      </c>
+      <c r="L22" s="77">
+        <v>1</v>
+      </c>
+      <c r="M22" s="56">
+        <f>ROUND(((J22+I22+K22+L22)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N22" s="77">
+        <v>3</v>
+      </c>
+      <c r="O22" s="88">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="P22">
+        <f>H22-O22</f>
+        <v>0.80000000000000071</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="78">
+        <v>4</v>
+      </c>
+      <c r="C23" s="12">
+        <v>4</v>
+      </c>
+      <c r="D23" s="80">
+        <v>3</v>
+      </c>
+      <c r="E23" s="80">
+        <v>3</v>
+      </c>
+      <c r="F23" s="78">
+        <f>ROUND(((C23+B23+D23+E23)/4), 2)</f>
+        <v>3.5</v>
+      </c>
+      <c r="G23" s="12">
+        <v>3</v>
+      </c>
+      <c r="H23" s="89">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I23" s="80">
+        <v>4</v>
+      </c>
+      <c r="J23" s="12">
+        <v>4</v>
+      </c>
+      <c r="K23" s="80">
+        <v>3</v>
+      </c>
+      <c r="L23" s="80">
+        <v>3</v>
+      </c>
+      <c r="M23" s="78">
+        <f>ROUND(((J23+I23+K23+L23)/4), 2)</f>
+        <v>3.5</v>
+      </c>
+      <c r="N23" s="80">
+        <v>3</v>
+      </c>
+      <c r="O23" s="89">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P23">
+        <f>H23-O23</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="83" t="s">
+        <v>137</v>
+      </c>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="83" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="84" t="s">
+        <v>148</v>
+      </c>
+      <c r="F28" s="81"/>
+      <c r="M28" s="81"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="84"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="26" id="{C3AE2D12-9E74-4EE7-8231-DDF7849D71FE}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>O4:O23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="28" id="{5E9329EA-C652-4249-86D0-68688582C30D}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H4:H23</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="H2" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="21"/>
+      <c r="H4" s="64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="63" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A21" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O37"/>
   <sheetViews>
@@ -1723,15 +3290,15 @@
   <sheetData>
     <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" s="66" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G2" s="66" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1739,28 +3306,28 @@
         <v>41</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C3" s="68" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="68" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G3" s="68" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="68" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B4" s="20">
         <v>0.5</v>
@@ -1773,7 +3340,7 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F4" s="20">
         <v>1</v>
@@ -1788,7 +3355,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B5" s="20">
         <v>0.5</v>
@@ -1801,7 +3368,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F5" s="20">
         <v>1</v>
@@ -1814,12 +3381,12 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B6" s="20">
         <v>0.5</v>
@@ -1832,7 +3399,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F6" s="20">
         <v>1</v>
@@ -1845,12 +3412,12 @@
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B7" s="56">
         <v>2</v>
@@ -1874,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="N7" s="68" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O7" s="27" t="s">
         <v>36</v>
@@ -1882,7 +3449,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B8" s="56">
         <v>1</v>
@@ -1906,18 +3473,18 @@
         <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N8" s="69" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B9" s="56">
         <v>1</v>
@@ -1941,10 +3508,10 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O9" s="21" t="s">
         <v>48</v>
@@ -1952,7 +3519,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B10" s="20">
         <v>0.5</v>
@@ -1976,7 +3543,7 @@
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>46</v>
@@ -1987,7 +3554,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B11" s="20">
         <v>0</v>
@@ -2000,7 +3567,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F11" s="56">
         <v>2</v>
@@ -2021,7 +3588,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B12" s="20">
         <v>0</v>
@@ -2034,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F12" s="56">
         <v>1</v>
@@ -2047,12 +3614,12 @@
         <v>4</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B13" s="20">
         <v>0</v>
@@ -2065,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F13" s="56">
         <v>1</v>
@@ -2078,7 +3645,7 @@
         <v>4</v>
       </c>
       <c r="O13" s="65" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2110,7 +3677,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B15" s="20">
         <v>2.5</v>
@@ -2134,15 +3701,15 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B16" s="20">
         <v>2</v>
@@ -2166,7 +3733,7 @@
         <v>4</v>
       </c>
       <c r="O16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2195,10 +3762,10 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2227,7 +3794,7 @@
         <v>2</v>
       </c>
       <c r="O18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2256,10 +3823,10 @@
         <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2355,7 +3922,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F23" s="56">
         <v>2</v>
@@ -2368,7 +3935,7 @@
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2386,7 +3953,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F24" s="56">
         <v>2</v>
@@ -2440,7 +4007,7 @@
         <v>8</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F26" s="56">
         <v>1</v>
@@ -2453,12 +4020,12 @@
         <v>4</v>
       </c>
       <c r="J26" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B27" s="56">
         <v>1</v>
@@ -2482,12 +4049,12 @@
         <v>4</v>
       </c>
       <c r="J27" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B28" s="56">
         <v>1</v>
@@ -2513,7 +4080,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B29" s="56">
         <v>2</v>
@@ -2539,7 +4106,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="70" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B30" s="78">
         <v>3</v>
@@ -2552,7 +4119,7 @@
         <v>12</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F30" s="78">
         <v>2</v>
@@ -2565,18 +4132,18 @@
         <v>8</v>
       </c>
       <c r="J30" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E32" s="67" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F32" s="74"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E33" s="67" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F33" s="74"/>
     </row>
@@ -2623,7 +4190,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23 D23">
+  <conditionalFormatting sqref="D23 H23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2637,1559 +4204,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:Q31"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="65.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="D2" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="K2" s="66" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="87" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>148</v>
-      </c>
-      <c r="J3" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="87" t="s">
-        <v>116</v>
-      </c>
-      <c r="N3" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="P3" s="86" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="82">
-        <v>3</v>
-      </c>
-      <c r="C4" s="81">
-        <v>3</v>
-      </c>
-      <c r="D4" s="81">
-        <v>2</v>
-      </c>
-      <c r="E4" s="81">
-        <v>2</v>
-      </c>
-      <c r="F4" s="91">
-        <f>ROUND(((B4+C4+D4+E4)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1</v>
-      </c>
-      <c r="H4" s="89">
-        <f>ROUND(F4*G4/14*10, 1)</f>
-        <v>1.8</v>
-      </c>
-      <c r="I4" s="82">
-        <v>3</v>
-      </c>
-      <c r="J4" s="81">
-        <v>3</v>
-      </c>
-      <c r="K4" s="81">
-        <v>2</v>
-      </c>
-      <c r="L4" s="81">
-        <v>2</v>
-      </c>
-      <c r="M4" s="91">
-        <f>ROUND(((I4+J4+K4+L4)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="89">
-        <f>ROUND(M4*N4/14*10, 1)</f>
-        <v>1.8</v>
-      </c>
-      <c r="P4">
-        <f>H4-O4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B5" s="20">
-        <v>2</v>
-      </c>
-      <c r="C5" s="81">
-        <v>3</v>
-      </c>
-      <c r="D5" s="77">
-        <v>2</v>
-      </c>
-      <c r="E5" s="77">
-        <v>2</v>
-      </c>
-      <c r="F5" s="56">
-        <f>ROUND(((B5+C5+D5+E5)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="G5" s="10">
-        <v>4</v>
-      </c>
-      <c r="H5" s="89">
-        <f t="shared" ref="H5:H24" si="0">ROUND(F5*G5/14*10, 1)</f>
-        <v>6.4</v>
-      </c>
-      <c r="I5" s="20">
-        <v>2</v>
-      </c>
-      <c r="J5" s="81">
-        <v>3</v>
-      </c>
-      <c r="K5" s="77">
-        <v>2</v>
-      </c>
-      <c r="L5" s="77">
-        <v>2</v>
-      </c>
-      <c r="M5" s="56">
-        <f>ROUND(((I5+J5+K5+L5)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="N5" s="10">
-        <v>4</v>
-      </c>
-      <c r="O5" s="89">
-        <f t="shared" ref="O5:O24" si="1">ROUND(M5*N5/14*10, 1)</f>
-        <v>6.4</v>
-      </c>
-      <c r="P5">
-        <f>H5-O5</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="20">
-        <v>1</v>
-      </c>
-      <c r="C6" s="81">
-        <v>1</v>
-      </c>
-      <c r="D6" s="81">
-        <v>3</v>
-      </c>
-      <c r="E6" s="81">
-        <v>3</v>
-      </c>
-      <c r="F6" s="56">
-        <f>ROUND(((B6+C6+D6+E6)/4), 2)</f>
-        <v>2</v>
-      </c>
-      <c r="G6" s="10">
-        <v>4</v>
-      </c>
-      <c r="H6" s="89">
-        <f t="shared" si="0"/>
-        <v>5.7</v>
-      </c>
-      <c r="I6" s="20">
-        <v>1</v>
-      </c>
-      <c r="J6" s="81">
-        <v>1</v>
-      </c>
-      <c r="K6" s="81">
-        <v>3</v>
-      </c>
-      <c r="L6" s="81">
-        <v>3</v>
-      </c>
-      <c r="M6" s="56">
-        <f>ROUND(((I6+J6+K6+L6)/4), 2)</f>
-        <v>2</v>
-      </c>
-      <c r="N6" s="10">
-        <v>4</v>
-      </c>
-      <c r="O6" s="89">
-        <f t="shared" si="1"/>
-        <v>5.7</v>
-      </c>
-      <c r="P6">
-        <f>H6-O6</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F7" s="56">
-        <v>0</v>
-      </c>
-      <c r="G7" s="10">
-        <v>4</v>
-      </c>
-      <c r="H7" s="89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="56">
-        <v>2</v>
-      </c>
-      <c r="J7" s="77">
-        <v>4</v>
-      </c>
-      <c r="K7" s="77">
-        <v>3</v>
-      </c>
-      <c r="L7" s="77">
-        <v>3</v>
-      </c>
-      <c r="M7" s="56">
-        <f>ROUND(((I7+J7+K7+L7)/4), 2)</f>
-        <v>3</v>
-      </c>
-      <c r="N7" s="10">
-        <v>4</v>
-      </c>
-      <c r="O7" s="89">
-        <f t="shared" si="1"/>
-        <v>8.6</v>
-      </c>
-      <c r="P7">
-        <f>H7-O7</f>
-        <v>-8.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" s="56">
-        <v>0</v>
-      </c>
-      <c r="G8" s="10">
-        <v>4</v>
-      </c>
-      <c r="H8" s="89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="56">
-        <v>1</v>
-      </c>
-      <c r="J8" s="77">
-        <v>4</v>
-      </c>
-      <c r="K8" s="77">
-        <v>3</v>
-      </c>
-      <c r="L8" s="77">
-        <v>3</v>
-      </c>
-      <c r="M8" s="56">
-        <f>ROUND(((I8+J8+K8+L8)/4), 2)</f>
-        <v>2.75</v>
-      </c>
-      <c r="N8" s="10">
-        <v>4</v>
-      </c>
-      <c r="O8" s="89">
-        <f t="shared" si="1"/>
-        <v>7.9</v>
-      </c>
-      <c r="P8">
-        <f>H8-O8</f>
-        <v>-7.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="20">
-        <v>1</v>
-      </c>
-      <c r="C9" s="81">
-        <v>3</v>
-      </c>
-      <c r="D9" s="81">
-        <v>1</v>
-      </c>
-      <c r="E9" s="81">
-        <v>0</v>
-      </c>
-      <c r="F9" s="56">
-        <f>ROUND(((B9+C9+D9+E9)/4), 2)</f>
-        <v>1.25</v>
-      </c>
-      <c r="G9" s="10">
-        <v>4</v>
-      </c>
-      <c r="H9" s="89">
-        <f>ROUND(F9*G9/14*10, 1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="I9" s="20">
-        <v>1</v>
-      </c>
-      <c r="J9" s="81">
-        <v>3</v>
-      </c>
-      <c r="K9" s="81">
-        <v>1</v>
-      </c>
-      <c r="L9" s="81">
-        <v>0</v>
-      </c>
-      <c r="M9" s="56">
-        <f>ROUND(((I9+J9+K9+L9)/4), 2)</f>
-        <v>1.25</v>
-      </c>
-      <c r="N9" s="10">
-        <v>4</v>
-      </c>
-      <c r="O9" s="89">
-        <f>ROUND(M9*N9/14*10, 1)</f>
-        <v>3.6</v>
-      </c>
-      <c r="P9">
-        <f>H9-O9</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="20">
-        <v>4</v>
-      </c>
-      <c r="C10" s="81">
-        <v>4</v>
-      </c>
-      <c r="D10" s="81">
-        <v>3</v>
-      </c>
-      <c r="E10" s="81">
-        <v>3</v>
-      </c>
-      <c r="F10" s="56">
-        <f>ROUND(((B10+C10+D10+E10)/4), 2)</f>
-        <v>3.5</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2</v>
-      </c>
-      <c r="H10" s="89">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I10" s="20">
-        <v>4</v>
-      </c>
-      <c r="J10" s="81">
-        <v>4</v>
-      </c>
-      <c r="K10" s="81">
-        <v>3</v>
-      </c>
-      <c r="L10" s="81">
-        <v>3</v>
-      </c>
-      <c r="M10" s="56">
-        <f>ROUND(((I10+J10+K10+L10)/4), 2)</f>
-        <v>3.5</v>
-      </c>
-      <c r="N10" s="77">
-        <v>2</v>
-      </c>
-      <c r="O10" s="89">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="P10">
-        <f>H10-O10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="20">
-        <v>4</v>
-      </c>
-      <c r="C11" s="81">
-        <v>4</v>
-      </c>
-      <c r="D11" s="81">
-        <v>3</v>
-      </c>
-      <c r="E11" s="81">
-        <v>2</v>
-      </c>
-      <c r="F11" s="56">
-        <f>ROUND(((B11+C11+D11+E11)/4), 2)</f>
-        <v>3.25</v>
-      </c>
-      <c r="G11" s="10">
-        <v>4</v>
-      </c>
-      <c r="H11" s="89">
-        <f t="shared" si="0"/>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="I11" s="20">
-        <v>4</v>
-      </c>
-      <c r="J11" s="81">
-        <v>4</v>
-      </c>
-      <c r="K11" s="81">
-        <v>3</v>
-      </c>
-      <c r="L11" s="81">
-        <v>2</v>
-      </c>
-      <c r="M11" s="56">
-        <f>ROUND(((I11+J11+K11+L11)/4), 2)</f>
-        <v>3.25</v>
-      </c>
-      <c r="N11" s="77">
-        <v>4</v>
-      </c>
-      <c r="O11" s="89">
-        <f t="shared" si="1"/>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="P11">
-        <f>H11-O11</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="56">
-        <v>2</v>
-      </c>
-      <c r="C12" s="81">
-        <v>2</v>
-      </c>
-      <c r="D12" s="81">
-        <v>2</v>
-      </c>
-      <c r="E12" s="81">
-        <v>2</v>
-      </c>
-      <c r="F12" s="56">
-        <f>ROUND(((B12+C12+D12+E12)/4), 2)</f>
-        <v>2</v>
-      </c>
-      <c r="G12" s="10">
-        <v>2</v>
-      </c>
-      <c r="H12" s="89">
-        <f t="shared" si="0"/>
-        <v>2.9</v>
-      </c>
-      <c r="I12" s="56">
-        <v>2</v>
-      </c>
-      <c r="J12" s="81">
-        <v>2</v>
-      </c>
-      <c r="K12" s="81">
-        <v>2</v>
-      </c>
-      <c r="L12" s="81">
-        <v>2</v>
-      </c>
-      <c r="M12" s="56">
-        <f>ROUND(((I12+J12+K12+L12)/4), 2)</f>
-        <v>2</v>
-      </c>
-      <c r="N12" s="77">
-        <v>2</v>
-      </c>
-      <c r="O12" s="89">
-        <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="P12">
-        <f>H12-O12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="20">
-        <v>3</v>
-      </c>
-      <c r="C13" s="77">
-        <v>2</v>
-      </c>
-      <c r="D13" s="77">
-        <v>3</v>
-      </c>
-      <c r="E13" s="77">
-        <v>2</v>
-      </c>
-      <c r="F13" s="56">
-        <f>ROUND(((B13+C13+D13+E13)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G13" s="10">
-        <v>4</v>
-      </c>
-      <c r="H13" s="89">
-        <f t="shared" si="0"/>
-        <v>7.1</v>
-      </c>
-      <c r="I13" s="20">
-        <v>3</v>
-      </c>
-      <c r="J13" s="77">
-        <v>2</v>
-      </c>
-      <c r="K13" s="77">
-        <v>3</v>
-      </c>
-      <c r="L13" s="77">
-        <v>2</v>
-      </c>
-      <c r="M13" s="56">
-        <f>ROUND(((I13+J13+K13+L13)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="N13" s="77">
-        <v>4</v>
-      </c>
-      <c r="O13" s="89">
-        <f t="shared" si="1"/>
-        <v>7.1</v>
-      </c>
-      <c r="P13">
-        <f>H13-O13</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="20">
-        <v>2</v>
-      </c>
-      <c r="C14" s="81">
-        <v>1</v>
-      </c>
-      <c r="D14" s="81">
-        <v>2</v>
-      </c>
-      <c r="E14" s="81">
-        <v>1</v>
-      </c>
-      <c r="F14" s="56">
-        <f>ROUND(((B14+C14+D14+E14)/4), 2)</f>
-        <v>1.5</v>
-      </c>
-      <c r="G14" s="10">
-        <v>2</v>
-      </c>
-      <c r="H14" s="89">
-        <f t="shared" si="0"/>
-        <v>2.1</v>
-      </c>
-      <c r="I14" s="20">
-        <v>2</v>
-      </c>
-      <c r="J14" s="81">
-        <v>1</v>
-      </c>
-      <c r="K14" s="81">
-        <v>2</v>
-      </c>
-      <c r="L14" s="81">
-        <v>1</v>
-      </c>
-      <c r="M14" s="56">
-        <f>ROUND(((I14+J14+K14+L14)/4), 2)</f>
-        <v>1.5</v>
-      </c>
-      <c r="N14" s="77">
-        <v>2</v>
-      </c>
-      <c r="O14" s="89">
-        <f t="shared" si="1"/>
-        <v>2.1</v>
-      </c>
-      <c r="P14">
-        <f>H14-O14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="20">
-        <v>2</v>
-      </c>
-      <c r="C15" s="77">
-        <v>2</v>
-      </c>
-      <c r="D15" s="77">
-        <v>3</v>
-      </c>
-      <c r="E15" s="77">
-        <v>3</v>
-      </c>
-      <c r="F15" s="56">
-        <f>ROUND(((B15+C15+D15+E15)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G15" s="10">
-        <v>2</v>
-      </c>
-      <c r="H15" s="89">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="I15" s="20">
-        <v>2</v>
-      </c>
-      <c r="J15" s="77">
-        <v>2</v>
-      </c>
-      <c r="K15" s="77">
-        <v>3</v>
-      </c>
-      <c r="L15" s="77">
-        <v>3</v>
-      </c>
-      <c r="M15" s="56">
-        <f>ROUND(((I15+J15+K15+L15)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="N15" s="77">
-        <v>2</v>
-      </c>
-      <c r="O15" s="89">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="P15">
-        <f>H15-O15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="20">
-        <v>2</v>
-      </c>
-      <c r="C16" s="77">
-        <v>2</v>
-      </c>
-      <c r="D16" s="77">
-        <v>3</v>
-      </c>
-      <c r="E16" s="77">
-        <v>3</v>
-      </c>
-      <c r="F16" s="56">
-        <f>ROUND(((B16+C16+D16+E16)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G16" s="10">
-        <v>1</v>
-      </c>
-      <c r="H16" s="89">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="I16" s="20">
-        <v>2</v>
-      </c>
-      <c r="J16" s="77">
-        <v>2</v>
-      </c>
-      <c r="K16" s="77">
-        <v>3</v>
-      </c>
-      <c r="L16" s="77">
-        <v>3</v>
-      </c>
-      <c r="M16" s="56">
-        <f>ROUND(((I16+J16+K16+L16)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="N16" s="77">
-        <v>1</v>
-      </c>
-      <c r="O16" s="89">
-        <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-      <c r="P16">
-        <f>H16-O16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="20">
-        <v>2</v>
-      </c>
-      <c r="C17" s="77">
-        <v>2</v>
-      </c>
-      <c r="D17" s="77">
-        <v>3</v>
-      </c>
-      <c r="E17" s="77">
-        <v>3</v>
-      </c>
-      <c r="F17" s="56">
-        <f>ROUND(((B17+C17+D17+E17)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G17" s="10">
-        <v>1</v>
-      </c>
-      <c r="H17" s="89">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="I17" s="20">
-        <v>2</v>
-      </c>
-      <c r="J17" s="77">
-        <v>2</v>
-      </c>
-      <c r="K17" s="77">
-        <v>3</v>
-      </c>
-      <c r="L17" s="77">
-        <v>3</v>
-      </c>
-      <c r="M17" s="56">
-        <f>ROUND(((I17+J17+K17+L17)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="N17" s="77">
-        <v>1</v>
-      </c>
-      <c r="O17" s="89">
-        <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-      <c r="P17">
-        <f>H17-O17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="20">
-        <v>1</v>
-      </c>
-      <c r="C18" s="77">
-        <v>2</v>
-      </c>
-      <c r="D18" s="77">
-        <v>3</v>
-      </c>
-      <c r="E18" s="77">
-        <v>3</v>
-      </c>
-      <c r="F18" s="56">
-        <f>ROUND(((B18+C18+D18+E18)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="G18" s="10">
-        <v>4</v>
-      </c>
-      <c r="H18" s="89">
-        <f t="shared" si="0"/>
-        <v>6.4</v>
-      </c>
-      <c r="I18" s="20">
-        <v>1</v>
-      </c>
-      <c r="J18" s="77">
-        <v>2</v>
-      </c>
-      <c r="K18" s="77">
-        <v>3</v>
-      </c>
-      <c r="L18" s="77">
-        <v>3</v>
-      </c>
-      <c r="M18" s="56">
-        <f>ROUND(((I18+J18+K18+L18)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="N18" s="77">
-        <v>2</v>
-      </c>
-      <c r="O18" s="89">
-        <f t="shared" si="1"/>
-        <v>3.2</v>
-      </c>
-      <c r="P18">
-        <f>H18-O18</f>
-        <v>3.2</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="20">
-        <v>1</v>
-      </c>
-      <c r="C19" s="77">
-        <v>2</v>
-      </c>
-      <c r="D19" s="77">
-        <v>3</v>
-      </c>
-      <c r="E19" s="77">
-        <v>3</v>
-      </c>
-      <c r="F19" s="56">
-        <f>ROUND(((B19+C19+D19+E19)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2</v>
-      </c>
-      <c r="H19" s="89">
-        <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="I19" s="20">
-        <v>1</v>
-      </c>
-      <c r="J19" s="77">
-        <v>2</v>
-      </c>
-      <c r="K19" s="77">
-        <v>3</v>
-      </c>
-      <c r="L19" s="77">
-        <v>3</v>
-      </c>
-      <c r="M19" s="56">
-        <f>ROUND(((I19+J19+K19+L19)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="N19" s="77">
-        <v>3</v>
-      </c>
-      <c r="O19" s="89">
-        <f t="shared" si="1"/>
-        <v>4.8</v>
-      </c>
-      <c r="P19">
-        <f>H19-O19</f>
-        <v>-1.5999999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="20">
-        <v>2</v>
-      </c>
-      <c r="C20" s="77">
-        <v>1</v>
-      </c>
-      <c r="D20" s="77">
-        <v>3</v>
-      </c>
-      <c r="E20" s="77">
-        <v>3</v>
-      </c>
-      <c r="F20" s="56">
-        <f>ROUND(((B20+C20+D20+E20)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="G20" s="10">
-        <v>2</v>
-      </c>
-      <c r="H20" s="89">
-        <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="I20" s="20">
-        <v>2</v>
-      </c>
-      <c r="J20" s="77">
-        <v>1</v>
-      </c>
-      <c r="K20" s="77">
-        <v>3</v>
-      </c>
-      <c r="L20" s="77">
-        <v>3</v>
-      </c>
-      <c r="M20" s="56">
-        <f>ROUND(((I20+J20+K20+L20)/4), 2)</f>
-        <v>2.25</v>
-      </c>
-      <c r="N20" s="77">
-        <v>2</v>
-      </c>
-      <c r="O20" s="89">
-        <f t="shared" si="1"/>
-        <v>3.2</v>
-      </c>
-      <c r="P20">
-        <f>H20-O20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="20">
-        <v>1</v>
-      </c>
-      <c r="C21" s="77">
-        <v>1</v>
-      </c>
-      <c r="D21" s="77">
-        <v>2</v>
-      </c>
-      <c r="E21" s="77">
-        <v>2</v>
-      </c>
-      <c r="F21" s="56">
-        <f>ROUND(((B21+C21+D21+E21)/4), 2)</f>
-        <v>1.5</v>
-      </c>
-      <c r="G21" s="10">
-        <v>4</v>
-      </c>
-      <c r="H21" s="89">
-        <f t="shared" si="0"/>
-        <v>4.3</v>
-      </c>
-      <c r="I21" s="20">
-        <v>1</v>
-      </c>
-      <c r="J21" s="77">
-        <v>1</v>
-      </c>
-      <c r="K21" s="77">
-        <v>2</v>
-      </c>
-      <c r="L21" s="77">
-        <v>1</v>
-      </c>
-      <c r="M21" s="56">
-        <f>ROUND(((I21+J21+K21+L21)/4), 2)</f>
-        <v>1.25</v>
-      </c>
-      <c r="N21" s="77">
-        <v>4</v>
-      </c>
-      <c r="O21" s="89">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="P21">
-        <f>H21-O21</f>
-        <v>0.69999999999999973</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="20">
-        <v>1</v>
-      </c>
-      <c r="C22" s="77">
-        <v>1</v>
-      </c>
-      <c r="D22" s="77">
-        <v>2</v>
-      </c>
-      <c r="E22" s="77">
-        <v>3</v>
-      </c>
-      <c r="F22" s="56">
-        <f>ROUND(((B22+C22+D22+E22)/4), 2)</f>
-        <v>1.75</v>
-      </c>
-      <c r="G22" s="10">
-        <v>4</v>
-      </c>
-      <c r="H22" s="89">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I22" s="20">
-        <v>1</v>
-      </c>
-      <c r="J22" s="77">
-        <v>1</v>
-      </c>
-      <c r="K22" s="77">
-        <v>2</v>
-      </c>
-      <c r="L22" s="77">
-        <v>3</v>
-      </c>
-      <c r="M22" s="56">
-        <f>ROUND(((I22+J22+K22+L22)/4), 2)</f>
-        <v>1.75</v>
-      </c>
-      <c r="N22" s="77">
-        <v>4</v>
-      </c>
-      <c r="O22" s="89">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="P22">
-        <f>H22-O22</f>
-        <v>0</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="20">
-        <v>2</v>
-      </c>
-      <c r="C23" s="77">
-        <v>2</v>
-      </c>
-      <c r="D23" s="77">
-        <v>3</v>
-      </c>
-      <c r="E23" s="77">
-        <v>3</v>
-      </c>
-      <c r="F23" s="56">
-        <f>ROUND(((B23+C23+D23+E23)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G23" s="10">
-        <v>2</v>
-      </c>
-      <c r="H23" s="89">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="I23" s="20">
-        <v>2</v>
-      </c>
-      <c r="J23" s="77">
-        <v>2</v>
-      </c>
-      <c r="K23" s="77">
-        <v>3</v>
-      </c>
-      <c r="L23" s="77">
-        <v>3</v>
-      </c>
-      <c r="M23" s="56">
-        <f>ROUND(((I23+J23+K23+L23)/4), 2)</f>
-        <v>2.5</v>
-      </c>
-      <c r="N23" s="77">
-        <v>2</v>
-      </c>
-      <c r="O23" s="89">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="P23">
-        <f>H23-O23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="70" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="83">
-        <v>4</v>
-      </c>
-      <c r="C24" s="80">
-        <v>4</v>
-      </c>
-      <c r="D24" s="80">
-        <v>3</v>
-      </c>
-      <c r="E24" s="80">
-        <v>3</v>
-      </c>
-      <c r="F24" s="78">
-        <f>ROUND(((B24+C24+D24+E24)/4), 2)</f>
-        <v>3.5</v>
-      </c>
-      <c r="G24" s="12">
-        <v>4</v>
-      </c>
-      <c r="H24" s="90">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I24" s="83">
-        <v>4</v>
-      </c>
-      <c r="J24" s="80">
-        <v>4</v>
-      </c>
-      <c r="K24" s="80">
-        <v>3</v>
-      </c>
-      <c r="L24" s="80">
-        <v>3</v>
-      </c>
-      <c r="M24" s="78">
-        <f>ROUND(((I24+J24+K24+L24)/4), 2)</f>
-        <v>3.5</v>
-      </c>
-      <c r="N24" s="80">
-        <v>4</v>
-      </c>
-      <c r="O24" s="90">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="P24">
-        <f>H24-O24</f>
-        <v>0</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="84" t="s">
-        <v>141</v>
-      </c>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="74"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="84" t="s">
-        <v>140</v>
-      </c>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="84" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="85" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="81"/>
-      <c r="M29" s="81"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="85"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="H4:H24">
-    <cfRule type="iconSet" priority="19">
-      <iconSet reverse="1">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="4"/>
-        <cfvo type="num" val="7"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O24">
-    <cfRule type="iconSet" priority="21">
-      <iconSet reverse="1">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="4"/>
-        <cfvo type="num" val="7"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:H22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="H2" s="32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="21"/>
-      <c r="H4" s="64" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="H7" s="29"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" s="63" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5583,7 +5597,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -5597,7 +5611,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -5611,7 +5625,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -5625,7 +5639,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C74">
         <v>3</v>

</xml_diff>

<commit_message>
added measure template to risk assess doc
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
-    <sheet name="Vector risk assessment" sheetId="5" r:id="rId2"/>
-    <sheet name="Risk assessment formula" sheetId="2" r:id="rId3"/>
+    <sheet name="Security Measures" sheetId="7" r:id="rId2"/>
+    <sheet name="Vector risk assessment" sheetId="5" r:id="rId3"/>
+    <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ISFOXAutomaticLabelingDisabled" hidden="1">TRUE</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="144">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -267,66 +268,6 @@
     <t>Vector descriptions</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -342,18 +283,9 @@
     <t>Change the existing configuration through the Kubernetes dashboard &amp; apiserver (cloud provider interfaces are separately evaluated)</t>
   </si>
   <si>
-    <t>(Security measure package IDs)</t>
-  </si>
-  <si>
-    <t>VID</t>
-  </si>
-  <si>
     <t>(Vector ID)</t>
   </si>
   <si>
-    <t>MID</t>
-  </si>
-  <si>
     <t>Change the existing configuration through potential cloud provider webinterfaces &amp; apiserver(s) (Kubernetes interfaces are separately evaluated)</t>
   </si>
   <si>
@@ -406,6 +338,138 @@
   </si>
   <si>
     <t>The underlying nodes could allow an attacker easy entry, even if the containers themselves are hardened</t>
+  </si>
+  <si>
+    <t>Security Measures</t>
+  </si>
+  <si>
+    <t>V01</t>
+  </si>
+  <si>
+    <t>V02</t>
+  </si>
+  <si>
+    <t>V03</t>
+  </si>
+  <si>
+    <t>V04</t>
+  </si>
+  <si>
+    <t>V05</t>
+  </si>
+  <si>
+    <t>V06</t>
+  </si>
+  <si>
+    <t>V07</t>
+  </si>
+  <si>
+    <t>V08</t>
+  </si>
+  <si>
+    <t>V09</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>V13</t>
+  </si>
+  <si>
+    <t>V14</t>
+  </si>
+  <si>
+    <t>V15</t>
+  </si>
+  <si>
+    <t>V16</t>
+  </si>
+  <si>
+    <t>V17</t>
+  </si>
+  <si>
+    <t>V18</t>
+  </si>
+  <si>
+    <t>V19</t>
+  </si>
+  <si>
+    <t>V20</t>
+  </si>
+  <si>
+    <t>M01</t>
+  </si>
+  <si>
+    <t>M02</t>
+  </si>
+  <si>
+    <t>M03</t>
+  </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>MP01, MPxx, …</t>
+  </si>
+  <si>
+    <t>How to assess?</t>
+  </si>
+  <si>
+    <t>How to implement?</t>
+  </si>
+  <si>
+    <t>How to enforce?</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Kubernetes management measures</t>
+  </si>
+  <si>
+    <t>Organisational measures</t>
+  </si>
+  <si>
+    <t>Mxx</t>
+  </si>
+  <si>
+    <t>Cloud provider management measures</t>
+  </si>
+  <si>
+    <t>Container / build pipeline measures</t>
+  </si>
+  <si>
+    <t>Base infrastructure measures</t>
+  </si>
+  <si>
+    <t>MP-ID</t>
+  </si>
+  <si>
+    <t>V-ID</t>
+  </si>
+  <si>
+    <t>VI-D</t>
+  </si>
+  <si>
+    <t>M-ID</t>
+  </si>
+  <si>
+    <t>(measure packet ID)</t>
+  </si>
+  <si>
+    <t>MPxx, Mpxy, …</t>
+  </si>
+  <si>
+    <t>(Security measure package ID)</t>
+  </si>
+  <si>
+    <t>LOREM IPSUM Measure name / desc</t>
   </si>
 </sst>
 </file>
@@ -654,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -784,6 +848,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1073,15 +1146,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="245.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1092,272 +1165,630 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="36" t="s">
+        <v>141</v>
+      </c>
       <c r="D4" s="36" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="37" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A4:A23" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="62"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A24:G24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1365,7 +1796,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,7 +1825,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="34" t="s">
@@ -1406,7 +1837,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>10</v>
@@ -1459,7 +1890,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>63</v>
@@ -1520,7 +1951,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>69</v>
@@ -1581,7 +2012,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>67</v>
@@ -1642,7 +2073,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>64</v>
@@ -1699,7 +2130,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
@@ -1756,7 +2187,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>66</v>
@@ -1817,7 +2248,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -1875,7 +2306,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
@@ -1936,7 +2367,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
@@ -1994,7 +2425,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B13" s="53" t="s">
         <v>68</v>
@@ -2055,7 +2486,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>1</v>
@@ -2113,7 +2544,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>23</v>
@@ -2171,7 +2602,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>57</v>
@@ -2229,7 +2660,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="B17" s="53" t="s">
         <v>2</v>
@@ -2290,7 +2721,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>3</v>
@@ -2348,7 +2779,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>53</v>
@@ -2406,7 +2837,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>54</v>
@@ -2467,7 +2898,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>56</v>
@@ -2528,7 +2959,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>55</v>
@@ -2586,7 +3017,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B23" s="55" t="s">
         <v>52</v>
@@ -2681,9 +3112,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A4:A23" numberStoredAsText="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2731,7 +3159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
updated thesis structure (not typeset yet)
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="ISFOXClassificationInKeywords" hidden="1">"Public"</definedName>
     <definedName name="ISFOXClassificationName" hidden="1">"Public"</definedName>
     <definedName name="ISFOXOldClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
-    <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
+    <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"00000000-0000-0000-0000-000000000000"</definedName>
     <definedName name="ISFOXPrefix" hidden="1">"HvS"</definedName>
     <definedName name="ISFOXPreviousClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXSaveAsProcess" hidden="1">TRUE</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="172">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -217,9 +217,6 @@
     <t>compromise application components (lateral movement from container)</t>
   </si>
   <si>
-    <t>cluster/system user (read) (2)</t>
-  </si>
-  <si>
     <t>cluster/system user (R/W) (2)</t>
   </si>
   <si>
@@ -250,12 +247,6 @@
     <t>Read confidentials through k8s control plane interfaces (dashboard, apiserver)</t>
   </si>
   <si>
-    <t>Severe security principle violation = Severe</t>
-  </si>
-  <si>
-    <t>Non-severe security principle violation = Moderate</t>
-  </si>
-  <si>
     <t>^Risk = Probability * Impact, rounded to 0.1-intervals</t>
   </si>
   <si>
@@ -470,6 +461,99 @@
   </si>
   <si>
     <t>LOREM IPSUM Measure name / desc</t>
+  </si>
+  <si>
+    <t>Regularly train technical users and administrators in contact with the cluster</t>
+  </si>
+  <si>
+    <t>Regularly train managers responsible for users and projects on the cluster</t>
+  </si>
+  <si>
+    <t>Identify and classify all data handled within the cluster</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>CSVS, chapter 5.2</t>
+  </si>
+  <si>
+    <t>M04</t>
+  </si>
+  <si>
+    <t>A service or application can consist of multiple containers. A security concept provides information on the security needs of the service/application and how they are or will be addressed.</t>
+  </si>
+  <si>
+    <t>Created and regularly update a security concept for each service/application within the cluster</t>
+  </si>
+  <si>
+    <t>Create, enforce and regularly update vulnerability &amp; risk management responsibilities and processes</t>
+  </si>
+  <si>
+    <t>M05</t>
+  </si>
+  <si>
+    <t>Define roles and responsibilities within the cluster infrastructure</t>
+  </si>
+  <si>
+    <t>M06</t>
+  </si>
+  <si>
+    <t>Ex.: Who does cluster upgrades? Who is responsible for vulnerabilities in which container images?</t>
+  </si>
+  <si>
+    <t>Ex.: What warrants a cluster version upgrade? If a vulnerability is identified, what is to be done (when it may affect availability)?</t>
+  </si>
+  <si>
+    <t>Synonymous to "traditional" security measures and processes</t>
+  </si>
+  <si>
+    <t>TODO: Azure patch management?</t>
+  </si>
+  <si>
+    <t>TODO: Add CSVS chapters 6.2 &amp; 11.2 measures</t>
+  </si>
+  <si>
+    <t>TODO: Add CSVS chapters 8.2 measures</t>
+  </si>
+  <si>
+    <t>TODO: Add CSVS chapters 7.2 &amp; 9.2 measures</t>
+  </si>
+  <si>
+    <t>TODO: Add CSVS chapters 10.2 &amp; 12.2 through 16.2 measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO IMPLEMENT: </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vTgQLzeBfRU</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/azure/aks/operator-best-practices-cluster-isolation?view=tfs-2018</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/azure/aks/concepts-security</t>
+  </si>
+  <si>
+    <t>https://docs.openshift.com/container-platform/3.5/security/index.html</t>
+  </si>
+  <si>
+    <t>CIS-Benchmarks (Docker + Kubernetes)</t>
+  </si>
+  <si>
+    <t>Azure-Securing guide</t>
+  </si>
+  <si>
+    <t>Kubernetes-Security-Book?</t>
+  </si>
+  <si>
+    <t>Severe security principle violation / high monetary damage = Severe</t>
+  </si>
+  <si>
+    <t>Non-severe security principle violation / moderate monetary damage = Moderate</t>
+  </si>
+  <si>
+    <t>cluster/system user (read) (3)</t>
   </si>
 </sst>
 </file>
@@ -527,7 +611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +627,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,7 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -849,6 +939,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1146,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,268 +1255,268 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1431,202 +1526,244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B3" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>127</v>
-      </c>
       <c r="F3" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="67"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>146</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>152</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="58"/>
+      <c r="B11" s="61" t="s">
+        <v>156</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="19"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="F12" s="37"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="67"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1634,58 +1771,65 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>158</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="67"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="62"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1693,10 +1837,11 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1704,47 +1849,51 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="67"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="62"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1752,39 +1901,149 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="B27" s="62" t="s">
+        <v>159</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="67"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="B29" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="63"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="64" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A28:H28"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B38" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1796,7 +2055,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,12 +2079,12 @@
   <sheetData>
     <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="34" t="s">
@@ -1837,7 +2096,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>10</v>
@@ -1890,10 +2149,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="44">
         <v>3</v>
@@ -1946,15 +2205,15 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="11">
         <v>3</v>
@@ -2007,15 +2266,15 @@
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="11">
         <v>3</v>
@@ -2068,15 +2327,15 @@
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>48</v>
@@ -2130,10 +2389,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>48</v>
@@ -2187,10 +2446,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="11">
         <v>3</v>
@@ -2243,12 +2502,12 @@
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -2306,7 +2565,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
@@ -2362,12 +2621,12 @@
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
@@ -2425,10 +2684,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="25">
         <v>2</v>
@@ -2481,12 +2740,12 @@
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>1</v>
@@ -2544,7 +2803,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>23</v>
@@ -2602,7 +2861,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>57</v>
@@ -2660,7 +2919,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B17" s="53" t="s">
         <v>2</v>
@@ -2716,12 +2975,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="R17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>3</v>
@@ -2779,7 +3038,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>53</v>
@@ -2837,7 +3096,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>54</v>
@@ -2893,12 +3152,12 @@
         <v>0.70000000000000018</v>
       </c>
       <c r="R20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>56</v>
@@ -2954,12 +3213,12 @@
         <v>0</v>
       </c>
       <c r="R21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>55</v>
@@ -3017,7 +3276,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B23" s="55" t="s">
         <v>52</v>
@@ -3073,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="R23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -3167,7 +3426,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,7 +3493,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>59</v>
+        <v>171</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>31</v>
@@ -3253,7 +3512,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>30</v>
@@ -3317,7 +3576,7 @@
         <v>39</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3329,17 +3588,17 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added additional measures to draft
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
     <sheet name="Security Measures" sheetId="7" r:id="rId2"/>
     <sheet name="Vector risk assessment" sheetId="5" r:id="rId3"/>
     <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
+    <sheet name="Measure TempDump" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ISFOXAutomaticLabelingDisabled" hidden="1">TRUE</definedName>
@@ -19,7 +20,7 @@
     <definedName name="ISFOXClassificationInKeywords" hidden="1">"Public"</definedName>
     <definedName name="ISFOXClassificationName" hidden="1">"Public"</definedName>
     <definedName name="ISFOXOldClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
-    <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"00000000-0000-0000-0000-000000000000"</definedName>
+    <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXPrefix" hidden="1">"HvS"</definedName>
     <definedName name="ISFOXPreviousClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXSaveAsProcess" hidden="1">TRUE</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="204">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -241,9 +242,6 @@
     <t>Change configuration through k8s control plane interfaces</t>
   </si>
   <si>
-    <t xml:space="preserve"> R/W &amp; breakout to host, Privilege Escalation</t>
-  </si>
-  <si>
     <t>Read confidentials through k8s control plane interfaces (dashboard, apiserver)</t>
   </si>
   <si>
@@ -554,13 +552,112 @@
   </si>
   <si>
     <t>cluster/system user (read) (3)</t>
+  </si>
+  <si>
+    <t>Define responsibilities for Patch Management Guidelines and their execution (while accounting for vacation time and sick days)</t>
+  </si>
+  <si>
+    <t>Define Patch Management Guideline(s) covering all components, I.e. when to patch, when to upgrade, when to take offline</t>
+  </si>
+  <si>
+    <t>Executing people: subscribe to vulnerability notification feeds or set up automated patching</t>
+  </si>
+  <si>
+    <t>Regularly assess all components for conformity with the desired state</t>
+  </si>
+  <si>
+    <t>(Components: Hosts, Kubernetes cluster, containers, other cluster tools (Jenkins, …)</t>
+  </si>
+  <si>
+    <t>Patch Management measures</t>
+  </si>
+  <si>
+    <t>Minimal setup</t>
+  </si>
+  <si>
+    <t>Container-optimised node OS (i.e. CoreOS, Google Container-optimized OS)</t>
+  </si>
+  <si>
+    <t>Use mimimal base images (slim is good, alpine is better) for your containers</t>
+  </si>
+  <si>
+    <t>Install only tools required for the operation each specific container on the images used</t>
+  </si>
+  <si>
+    <t>Avoid and eliminate tool functionality overlap (i.e. you don’t need two different tools to gather the same logs, each might be at risk through vulns)</t>
+  </si>
+  <si>
+    <t>AKS-specific: Security Updates are not rolled out automatically if that would result in downtime! Someone has to restart nodes manually or set up automated process!</t>
+  </si>
+  <si>
+    <t>Restrict the set of potentially used images</t>
+  </si>
+  <si>
+    <t>Vet images before usage</t>
+  </si>
+  <si>
+    <t>Policies for container images</t>
+  </si>
+  <si>
+    <t>Define what makes an image safe (enough) for usage. (light: only allow verified dockerhub images. Heavy: run images through a vetting process or build them from scratch)</t>
+  </si>
+  <si>
+    <t>Define in what intervals both policy and set of base images are reviewed</t>
+  </si>
+  <si>
+    <t>Run your defined image vetting process for every container before it becomes available for use</t>
+  </si>
+  <si>
+    <t>Re-vet new versions before they are admitted for usage</t>
+  </si>
+  <si>
+    <t>Use a dedicated private image registry which only gets vetted images OR enforce image whitelisting from public sources (including restricting versions, only allow the ones you vetted!)</t>
+  </si>
+  <si>
+    <t>Host: Conventional patch management measures</t>
+  </si>
+  <si>
+    <t>Kubernetes: execute guidelines</t>
+  </si>
+  <si>
+    <t>Container: automated scanning (i.e. with clair) or regular manual assessment, subscribe to alerts</t>
+  </si>
+  <si>
+    <t>OpenShift-specific: execute guidelines</t>
+  </si>
+  <si>
+    <t>Raise operator awareness</t>
+  </si>
+  <si>
+    <t>Train operators (cluster administrators) regularly</t>
+  </si>
+  <si>
+    <t>Make sure that operators are aware of the risks of copy-pasting</t>
+  </si>
+  <si>
+    <t>write guidelines with good security policies (what to use by default, what exceptions could be allowed and what processes have to be followed before admitted)</t>
+  </si>
+  <si>
+    <t>other organizational measures</t>
+  </si>
+  <si>
+    <t>K8s PodSecurityPolicies</t>
+  </si>
+  <si>
+    <t>Enable and configure global ( &amp; potentially additional namespace-identified) Pod Security Policies, which define default values and enforce specific settings if defined. ATTENTION: currently in preview for AKS!</t>
+  </si>
+  <si>
+    <t>(recommentations: TODO! RunAsUser=MustRunAsNonRoot , RunAsGroup=MustRunAsNonRoot, AllowPrivilegeEscalation=false (&lt;- careful, might break setuid binaries! Not-as-good-alternative: DefaultAllowPrivilegeEscalation=false), privileged=false)</t>
+  </si>
+  <si>
+    <t>(openshift security context constraints)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,6 +701,14 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -808,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -944,6 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1241,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,268 +1361,268 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1545,162 +1651,162 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="F3" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>125</v>
-      </c>
       <c r="G3" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="67"/>
+      <c r="A4" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
       <c r="G5" s="60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
       <c r="B11" s="61" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1711,7 +1817,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1722,26 +1828,26 @@
       <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="A13" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
@@ -1751,7 +1857,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1763,7 +1869,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1775,10 +1881,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1788,26 +1894,26 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="67"/>
+      <c r="A18" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="68"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" s="36"/>
       <c r="E19" s="36"/>
@@ -1817,7 +1923,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1829,7 +1935,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1841,7 +1947,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1852,26 +1958,26 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="67"/>
+      <c r="A23" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="36"/>
@@ -1881,7 +1987,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1893,7 +1999,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1905,10 +2011,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1918,26 +2024,26 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="67"/>
+      <c r="A28" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="36"/>
@@ -1947,7 +2053,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1959,7 +2065,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1971,10 +2077,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
@@ -1988,47 +2094,47 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2161,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,12 +2185,12 @@
   <sheetData>
     <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="34" t="s">
@@ -2096,7 +2202,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>10</v>
@@ -2149,7 +2255,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>62</v>
@@ -2210,10 +2316,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="11">
         <v>3</v>
@@ -2271,7 +2377,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>66</v>
@@ -2332,7 +2438,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>63</v>
@@ -2389,7 +2495,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>64</v>
@@ -2446,7 +2552,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -2507,7 +2613,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -2565,7 +2671,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>44</v>
@@ -2626,7 +2732,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
@@ -2684,10 +2790,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C13" s="25">
         <v>2</v>
@@ -2745,7 +2851,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="53" t="s">
         <v>1</v>
@@ -2803,7 +2909,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>23</v>
@@ -2861,7 +2967,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>57</v>
@@ -2919,7 +3025,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="53" t="s">
         <v>2</v>
@@ -2980,7 +3086,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>3</v>
@@ -3038,7 +3144,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>53</v>
@@ -3096,7 +3202,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>54</v>
@@ -3157,7 +3263,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>56</v>
@@ -3218,7 +3324,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>55</v>
@@ -3276,7 +3382,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B23" s="55" t="s">
         <v>52</v>
@@ -3493,7 +3599,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>31</v>
@@ -3576,7 +3682,7 @@
         <v>39</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3588,17 +3694,17 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3636,4 +3742,179 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed measure sketch for all 20 vectors
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="289">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -251,9 +251,6 @@
     <t>Supplying a malicious kubernetes configuration leading to security violations on the cluster (remote access for an attacker, resource misuse, data leakage, …). Most easily done untargeted (tutorials/ help forums), but can be done targeted, too.</t>
   </si>
   <si>
-    <t>Once an attacker gains access to a container, he may try to access more lucrative application components, i.e. databases or containers with more confidential information/traffic.</t>
-  </si>
-  <si>
     <t>Once inside a container, an attacker may try to gain access to the underlying host by a multitude of means. This includes invoking syscalls, accessing the host file system and elevation priviledges within or outside of the container environment</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>The resources of the whole cluster may be misconfigured or misused for financial gains (mining cryptocurrencies)</t>
   </si>
   <si>
-    <t>A malicious container me be started within the cluster</t>
-  </si>
-  <si>
     <t>A malicious node may be added to the cluster</t>
   </si>
   <si>
@@ -578,18 +572,12 @@
     <t>Kubernetes: execute guidelines</t>
   </si>
   <si>
-    <t>Container: automated scanning (i.e. with clair) or regular manual assessment, subscribe to alerts</t>
-  </si>
-  <si>
     <t>OpenShift-specific: execute guidelines</t>
   </si>
   <si>
     <t>Raise operator awareness</t>
   </si>
   <si>
-    <t>Train operators (cluster administrators) regularly</t>
-  </si>
-  <si>
     <t>Make sure that operators are aware of the risks of copy-pasting</t>
   </si>
   <si>
@@ -608,9 +596,6 @@
     <t>(recommentations: TODO! RunAsUser=MustRunAsNonRoot , RunAsGroup=MustRunAsNonRoot, AllowPrivilegeEscalation=false (&lt;- careful, might break setuid binaries! Not-as-good-alternative: DefaultAllowPrivilegeEscalation=false), privileged=false)</t>
   </si>
   <si>
-    <t>(openshift security context constraints)</t>
-  </si>
-  <si>
     <t>^Risk = Probability * Impact, rounded to integers</t>
   </si>
   <si>
@@ -644,9 +629,6 @@
     <t>^Probability = (Vantage + RAL + Detectability + Exploitability)/4, rounded to 0.01 intervals</t>
   </si>
   <si>
-    <t>Supplying a malicious container image leading to security violations on the cluster (remote access for an attacker, resource misuse, data leakage, …). Most easily done untargeted (dockerhub images or dockerfiles on tutorials/help forums), but can be done targeted, too. Additionally, an image build process typically runs as root, leading to compromise possibilities to compromise the node where an image is built from a rogue dockerfile.</t>
-  </si>
-  <si>
     <t>CVSSv3 Scoring</t>
   </si>
   <si>
@@ -666,6 +648,264 @@
   </si>
   <si>
     <t>AV:N/AC:L/PR:N/UI:N/S:C/C:H/I:H/A:H</t>
+  </si>
+  <si>
+    <t>restrict communication</t>
+  </si>
+  <si>
+    <t>no traffic to oder projects (OCP) or namespaces (AKS)</t>
+  </si>
+  <si>
+    <t>All of these: either implemented by dev or enforced by admin. Suggestion: enforced by cluster admin (scc / networkpolicy in podsecuritypolicy) with exceptions granted when needed</t>
+  </si>
+  <si>
+    <t>restrict host impact</t>
+  </si>
+  <si>
+    <t>restrict images</t>
+  </si>
+  <si>
+    <t>use private repo / dockerhub-official images only</t>
+  </si>
+  <si>
+    <t>verify with tool / 3rd party</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>log all the things</t>
+  </si>
+  <si>
+    <t>monitoring &amp; alerting</t>
+  </si>
+  <si>
+    <t>prometheus, grafana (visualization), neuvector, (sysdig) falco, aqua, twistlock</t>
+  </si>
+  <si>
+    <t>Train operators (cluster administrators &amp; users) regularly</t>
+  </si>
+  <si>
+    <t>scan with fossa, clair, microscanner, OPA policies</t>
+  </si>
+  <si>
+    <t>secrets management</t>
+  </si>
+  <si>
+    <t>DO NOT load secrets from dockerfile / podconfig / env vars or other shit! DO use kubernetes secrets (or better: external key mgmt like hashicorp vault or azure ad pod identity / openshift vault) TODO: how to enforce?</t>
+  </si>
+  <si>
+    <t>put through kubesec.io offline/ kube-bench/ kubeaudit / kubeatf (enforce: k8guard) or 4-eyes-principle or security clearance on config changes (probably too overkill)</t>
+  </si>
+  <si>
+    <t>(openshift SCCs)</t>
+  </si>
+  <si>
+    <t>limit capabilities</t>
+  </si>
+  <si>
+    <t>Container: automated scanning (i.e. with clair) or regular manual assessment, subscribe to alerts (new vulns im container images / code OR other components!)</t>
+  </si>
+  <si>
+    <t>from container: network policies blacklisting APIs/consoles</t>
+  </si>
+  <si>
+    <t>secure access</t>
+  </si>
+  <si>
+    <t>no unauth, no ABAC, integrate existing RBAC you are managing anyway</t>
+  </si>
+  <si>
+    <t>from company network: firewall (bad practice)</t>
+  </si>
+  <si>
+    <t>use 2FA when possible (i.e. for dev and/or admin access to cloud) &lt;- openstack: 2FA may be integratable to AD? TODO</t>
+  </si>
+  <si>
+    <t>enable alerting</t>
+  </si>
+  <si>
+    <t>"conventional" hardening</t>
+  </si>
+  <si>
+    <t>established resources like CIS benchmarks</t>
+  </si>
+  <si>
+    <t>(V20 node patch mgmt measures)</t>
+  </si>
+  <si>
+    <t>(V20 node minimal OS measures)</t>
+  </si>
+  <si>
+    <t>additional restrictions available</t>
+  </si>
+  <si>
+    <t>disable SSH access to hosts whenever possible (access through physical when bare-metal / hypervisor interfaces if VM nodes). If needed and risk accepted, enable ssh access through bastion host</t>
+  </si>
+  <si>
+    <t>on events like adding admin / granting admin privs / creating namespace / touching things deemed critical. TODO: how?</t>
+  </si>
+  <si>
+    <t>close exposed ports configured, but not needed (dangling container runtime daemon?)</t>
+  </si>
+  <si>
+    <t>CSVS chapter: infrastructure</t>
+  </si>
+  <si>
+    <t>CIS Kubernetes Benchmark chapters: Worker Node Security Configuration &amp; Configuration Files</t>
+  </si>
+  <si>
+    <t>CIS Docker Benchmark chapters: Chapters 1-3 &amp; 5 (+ Docker Content trust)</t>
+  </si>
+  <si>
+    <t>Supplying a malicious container image leading to security violations on the cluster (remote access for an attacker, resource misuse, data leakage, …). Most easily done untargeted (dockerhub images or dockerfiles on tutorials/help forums), but can be done targeted, too. Additionally, an image build process typically runs as root, leading to compromise possibilities to compromise the node where an image is built from a rogue dockerfile. (TODO: provoking stale image usage to exploit vulns, too?)</t>
+  </si>
+  <si>
+    <t>NIST-SP800-190 chapters: 3.5, 4.5, 4.6</t>
+  </si>
+  <si>
+    <t>require admin to authorize node add</t>
+  </si>
+  <si>
+    <t>Source: NIST-SP800-190, chapter 4.3.5      TODO: how to in ocp / AKS?</t>
+  </si>
+  <si>
+    <t>(V08 limit capabilities)</t>
+  </si>
+  <si>
+    <t>deactivate/block unused interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">administration: uninstall / deactivate configurable interfaces </t>
+  </si>
+  <si>
+    <t>deactivate capabilities to the highest authority level  whenever possible/applicable</t>
+  </si>
+  <si>
+    <t>limit interface capabilities</t>
+  </si>
+  <si>
+    <t>change configuration through additional interfaces (mgmt console/API)</t>
+  </si>
+  <si>
+    <t>(ALL of V04 - but k8s-specific settings)</t>
+  </si>
+  <si>
+    <t>same as V04</t>
+  </si>
+  <si>
+    <t>organizational Measures</t>
+  </si>
+  <si>
+    <t>inform users &amp; admins of risks regarding…</t>
+  </si>
+  <si>
+    <t>…phishing (classic awareness)</t>
+  </si>
+  <si>
+    <t>…openly publishing stuff (open source (repos), presentations, talking to external people, troubleshooting threads on stackoverflow, potential partners/vendors, …) TODO: are there infosec modules/courses/resources for this?</t>
+  </si>
+  <si>
+    <t>no priviledged containers, no priviledge escalation (asking to become priviledged), restrict kernel capabilities, no root containers (maybe yes, but with user namespace remapping only?), procmounttype default (apply restrictions by container runtimes in /proc), restrict mount volume types and host volume paths, (maybe use sandboxing through gvisor / kata containers?)</t>
+  </si>
+  <si>
+    <t>(V08-&gt;limit capabilities-&gt;restrict host impact)</t>
+  </si>
+  <si>
+    <t>ELK/EFK-stack or Splunk with log forwarding/aggregation (container AND nodes), k8s audit logging (k8s)</t>
+  </si>
+  <si>
+    <t>Once an attacker gains access to a container, he may try to access more lucrative application components or information, i.e. sniffing traffic or accessing databases or containers with more confidential information/traffic.</t>
+  </si>
+  <si>
+    <t>implement least privilege principle</t>
+  </si>
+  <si>
+    <t>limit access to each user in their scope (possibly further - need to know principle?)</t>
+  </si>
+  <si>
+    <t>see V04, but for dashboard / apiserver</t>
+  </si>
+  <si>
+    <t>see V04, but for dashboard / apiserver. Apiserver: no anonymous-auth, please :/</t>
+  </si>
+  <si>
+    <t>re-assess all versions of all images regularly</t>
+  </si>
+  <si>
+    <t>regularly scan all available images in all their versions and disable images that are (or have become) vulnerable. Especially old image versions should be purged, since those can be vulnerable to well-documented exploits.</t>
+  </si>
+  <si>
+    <t>limit resource usage</t>
+  </si>
+  <si>
+    <t>isolation of components</t>
+  </si>
+  <si>
+    <t>different namespaces (with different resource limits) for different parts of app, depending on criticality</t>
+  </si>
+  <si>
+    <t>logging / monitoring config changes</t>
+  </si>
+  <si>
+    <t>limit account capabilities</t>
+  </si>
+  <si>
+    <t>least privilege for dev accounts to limit misconfiguration (i.e. to his own namespace) &lt;- no creation of new namespaces except for within his own resource limits!</t>
+  </si>
+  <si>
+    <t>see V14 -&gt; all except component isolation</t>
+  </si>
+  <si>
+    <t>per-app / per-namespace resource limits on CPU, Storage, RAM, Bandwidth, cloud budget, what else?</t>
+  </si>
+  <si>
+    <t>A malicious container may be started within the cluster</t>
+  </si>
+  <si>
+    <t>limit admission / capabilities</t>
+  </si>
+  <si>
+    <t>container runtime: V19-&gt;additional restrictions + V20-&gt;minimal node setup</t>
+  </si>
+  <si>
+    <t>see generic -&gt; logging/monitoring</t>
+  </si>
+  <si>
+    <t>k8s: V08 -&gt; limit capabilities</t>
+  </si>
+  <si>
+    <t>like V16, but during runtime</t>
+  </si>
+  <si>
+    <t>encrypt cross-container traffic</t>
+  </si>
+  <si>
+    <t>istio with mTLS for traffic encryption and signing OR guideline for devs to use TLS everywhere OR enforce with OPA?</t>
+  </si>
+  <si>
+    <t>authorization/authentication for access, even within</t>
+  </si>
+  <si>
+    <t>namespace isolation, network restriction, ...appSec problem?</t>
+  </si>
+  <si>
+    <t>cluster isolation</t>
+  </si>
+  <si>
+    <t>follow additional tips by supplied</t>
+  </si>
+  <si>
+    <t>same as V02</t>
+  </si>
+  <si>
+    <t>ensure image provenance</t>
+  </si>
+  <si>
+    <t>docker content trust, code signing</t>
+  </si>
+  <si>
+    <t>same as V14, V15, V10</t>
   </si>
 </sst>
 </file>
@@ -928,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1061,6 +1301,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1070,6 +1312,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1359,7 +1602,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,18 +1620,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>61</v>
@@ -1396,13 +1639,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>62</v>
@@ -1410,10 +1653,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -1422,10 +1665,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -1434,10 +1677,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
@@ -1446,10 +1689,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>199</v>
+        <v>248</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -1458,10 +1701,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
@@ -1470,19 +1713,19 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>42</v>
@@ -1494,146 +1737,146 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="51" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="52" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B18" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" s="51" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>77</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="51" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" s="51" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22" s="51" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B23" s="53" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1662,162 +1905,162 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="33" t="s">
+      <c r="E3" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>110</v>
-      </c>
       <c r="G3" s="33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H3" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="66"/>
+      <c r="A4" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
       <c r="G5" s="58" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" s="59" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1828,7 +2071,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1839,26 +2082,26 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="66"/>
+      <c r="A13" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -1868,7 +2111,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1880,7 +2123,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1892,10 +2135,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B17" s="60" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1905,26 +2148,26 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="A18" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="68"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
@@ -1934,7 +2177,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1946,7 +2189,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1958,7 +2201,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1969,26 +2212,26 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
+      <c r="A23" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="34"/>
@@ -1998,7 +2241,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2010,7 +2253,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2022,10 +2265,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="60" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2035,26 +2278,26 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="66"/>
+      <c r="A28" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -2064,7 +2307,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2076,7 +2319,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2088,10 +2331,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="57" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32" s="60" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
@@ -2105,47 +2348,47 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="62" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2172,7 +2415,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,7 +2456,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>9</v>
@@ -2266,10 +2509,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C4" s="42">
         <v>3</v>
@@ -2327,10 +2570,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -2388,10 +2631,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C6" s="10">
         <v>3</v>
@@ -2449,10 +2692,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C7" s="10">
         <v>3</v>
@@ -2510,10 +2753,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C8" s="10">
         <v>3</v>
@@ -2571,10 +2814,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
@@ -2632,7 +2875,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -2690,7 +2933,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>42</v>
@@ -2751,7 +2994,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>54</v>
@@ -2809,10 +3052,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C13" s="23">
         <v>2</v>
@@ -2870,7 +3113,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="51" t="s">
         <v>1</v>
@@ -2928,7 +3171,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="52" t="s">
         <v>22</v>
@@ -2986,10 +3229,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C16" s="23">
         <v>2</v>
@@ -3044,10 +3287,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C17" s="23">
         <v>2</v>
@@ -3105,7 +3348,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B18" s="51" t="s">
         <v>2</v>
@@ -3163,7 +3406,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19" s="51" t="s">
         <v>50</v>
@@ -3221,7 +3464,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="51" t="s">
         <v>51</v>
@@ -3282,7 +3525,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" s="51" t="s">
         <v>53</v>
@@ -3343,7 +3586,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22" s="51" t="s">
         <v>52</v>
@@ -3401,7 +3644,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B23" s="53" t="s">
         <v>49</v>
@@ -3493,20 +3736,20 @@
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B30" s="44"/>
       <c r="R30" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="R31" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="T31" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>42</v>
@@ -3521,16 +3764,17 @@
         <v>3</v>
       </c>
       <c r="F32" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="23">
         <v>3.25</v>
       </c>
       <c r="H32" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I32" s="48">
-        <v>10</v>
+        <f>MIN(10, ROUND(G32*H32, 0))</f>
+        <v>7</v>
       </c>
       <c r="J32" s="41">
         <v>4</v>
@@ -3560,18 +3804,18 @@
         <v>9.6</v>
       </c>
       <c r="S32" s="5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="T32" s="38">
         <v>9.6</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B33" s="53" t="s">
         <v>49</v>
@@ -3625,21 +3869,21 @@
         <v>10</v>
       </c>
       <c r="S33" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="T33" s="4">
         <v>10</v>
       </c>
       <c r="U33" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C34" s="10">
         <v>3</v>
@@ -3690,18 +3934,18 @@
         <v>6.5</v>
       </c>
       <c r="S34" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="T34" s="4">
         <v>7.4</v>
       </c>
       <c r="U34" s="5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35" s="51" t="s">
         <v>52</v>
@@ -3756,10 +4000,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C36" s="10">
         <v>3</v>
@@ -3811,10 +4055,10 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C37" s="10">
         <v>3</v>
@@ -3866,10 +4110,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C38" s="23">
         <v>2</v>
@@ -3921,7 +4165,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="51" t="s">
         <v>53</v>
@@ -3976,10 +4220,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C40" s="10">
         <v>3</v>
@@ -4031,7 +4275,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>0</v>
@@ -4086,10 +4330,10 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C42" s="23">
         <v>2</v>
@@ -4141,7 +4385,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B43" s="51" t="s">
         <v>2</v>
@@ -4209,7 +4453,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="32" id="{C3AE2D12-9E74-4EE7-8231-DDF7849D71FE}">
+          <x14:cfRule type="iconSet" priority="33" id="{C3AE2D12-9E74-4EE7-8231-DDF7849D71FE}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4228,7 +4472,7 @@
           <xm:sqref>P4:P23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="34" id="{5E9329EA-C652-4249-86D0-68688582C30D}">
+          <x14:cfRule type="iconSet" priority="35" id="{5E9329EA-C652-4249-86D0-68688582C30D}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4247,7 +4491,7 @@
           <xm:sqref>I4:I23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="38" id="{F0FC799B-F499-49C2-BEC1-A5AB0AC47363}">
+          <x14:cfRule type="iconSet" priority="39" id="{F0FC799B-F499-49C2-BEC1-A5AB0AC47363}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4266,7 +4510,7 @@
           <xm:sqref>P32:P33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="39" id="{C5E4184D-EE7B-438D-963A-E1850DA55180}">
+          <x14:cfRule type="iconSet" priority="40" id="{C5E4184D-EE7B-438D-963A-E1850DA55180}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4282,10 +4526,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I32:I33</xm:sqref>
+          <xm:sqref>I33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{EB89C6B2-878D-4A02-AB23-11F5756EFA34}">
+          <x14:cfRule type="iconSet" priority="4" id="{EB89C6B2-878D-4A02-AB23-11F5756EFA34}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4304,7 +4548,7 @@
           <xm:sqref>P36:P43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{E111A834-19E3-4D22-9799-4BE59182D58C}">
+          <x14:cfRule type="iconSet" priority="5" id="{E111A834-19E3-4D22-9799-4BE59182D58C}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4323,7 +4567,7 @@
           <xm:sqref>I36:I43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{5325B94A-1D08-46D0-9452-A80083BF36C8}">
+          <x14:cfRule type="iconSet" priority="2" id="{5325B94A-1D08-46D0-9452-A80083BF36C8}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4342,7 +4586,7 @@
           <xm:sqref>P34:P35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{5C1E872B-F551-46D8-8C32-67D6A9002AC8}">
+          <x14:cfRule type="iconSet" priority="3" id="{5C1E872B-F551-46D8-8C32-67D6A9002AC8}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4360,6 +4604,25 @@
           </x14:cfRule>
           <xm:sqref>I34:I35</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{BFB65072-4CDB-4F49-8CAF-E7FE7D200585}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I32</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -4374,7 +4637,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4444,7 +4707,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>18</v>
@@ -4516,7 +4779,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="27" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="7"/>
@@ -4524,7 +4787,7 @@
         <v>37</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4541,12 +4804,12 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4588,10 +4851,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C35"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C35"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4599,160 +4862,655 @@
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>161</v>
+      <c r="C4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>179</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>163</v>
-      </c>
       <c r="C15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>166</v>
-      </c>
-    </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
       <c r="C18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" t="s">
-        <v>171</v>
-      </c>
       <c r="C21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>169</v>
-      </c>
-      <c r="C24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" t="s">
-        <v>174</v>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>263</v>
+      </c>
       <c r="C27" t="s">
-        <v>175</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>186</v>
-      </c>
-      <c r="C34" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" t="s">
-        <v>188</v>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F37" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>207</v>
+      </c>
+      <c r="F38" t="s">
+        <v>208</v>
+      </c>
+      <c r="L38" s="65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>206</v>
+      </c>
+      <c r="F39" t="s">
+        <v>255</v>
+      </c>
+      <c r="L39" s="64"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>209</v>
+      </c>
+      <c r="F40" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>244</v>
+      </c>
+      <c r="C42" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="C43" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>247</v>
+      </c>
+      <c r="C46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>259</v>
+      </c>
+      <c r="C51" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>227</v>
+      </c>
+      <c r="C55" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="51"/>
+      <c r="B58" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>232</v>
+      </c>
+      <c r="C61" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="B68" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="61"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="61"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="51"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="61"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76" t="s">
+        <v>251</v>
+      </c>
+      <c r="C76" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="51"/>
+      <c r="D77" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="17"/>
+      <c r="D78" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="61"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>244</v>
+      </c>
+      <c r="C81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" t="s">
+        <v>247</v>
+      </c>
+      <c r="C82" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="61"/>
+      <c r="B83" t="s">
+        <v>223</v>
+      </c>
+      <c r="C83" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="61"/>
+      <c r="B84" t="s">
+        <v>227</v>
+      </c>
+      <c r="C84" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="61"/>
+      <c r="C85" s="17"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" t="s">
+        <v>266</v>
+      </c>
+      <c r="C86" s="69" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="51"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="61"/>
+      <c r="B88" t="s">
+        <v>265</v>
+      </c>
+      <c r="C88" s="69" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="61"/>
+      <c r="C89" s="69"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="61"/>
+      <c r="B90" t="s">
+        <v>269</v>
+      </c>
+      <c r="C90" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="61"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="61"/>
+      <c r="B92" t="s">
+        <v>268</v>
+      </c>
+      <c r="C92" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="61"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="61"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>274</v>
+      </c>
+      <c r="C96" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="61"/>
+      <c r="C97" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="61"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99" t="s">
+        <v>220</v>
+      </c>
+      <c r="C99" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="61"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" t="s">
+        <v>241</v>
+      </c>
+      <c r="C101" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="61"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B103" t="s">
+        <v>279</v>
+      </c>
+      <c r="C103" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="61"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="61"/>
+      <c r="B105" t="s">
+        <v>281</v>
+      </c>
+      <c r="E105" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="61"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="61"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="61"/>
+      <c r="B109" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="61"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B111" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="61"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B113" t="s">
+        <v>286</v>
+      </c>
+      <c r="C113" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="61"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="B115" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="61"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="B117" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>212</v>
+      </c>
+      <c r="C118" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further rating update prep
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
-    <sheet name="Vector risk assessment" sheetId="5" r:id="rId2"/>
-    <sheet name="Risk assessment formula" sheetId="2" r:id="rId3"/>
-    <sheet name="Vector Risk assessment OWASP" sheetId="11" r:id="rId4"/>
-    <sheet name="Measure TempDump" sheetId="8" r:id="rId5"/>
-    <sheet name="Security Measures" sheetId="7" r:id="rId6"/>
-    <sheet name="OWASP Rating" sheetId="10" r:id="rId7"/>
-    <sheet name="OWASP risk value deriving" sheetId="13" r:id="rId8"/>
+    <sheet name="Vector risk assessment 2" sheetId="14" r:id="rId2"/>
+    <sheet name="Vector risk assessment" sheetId="5" r:id="rId3"/>
+    <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
+    <sheet name="Vector Risk assessment OWASP" sheetId="11" r:id="rId5"/>
+    <sheet name="Measure TempDump" sheetId="8" r:id="rId6"/>
+    <sheet name="Security Measures" sheetId="7" r:id="rId7"/>
+    <sheet name="OWASP Rating" sheetId="10" r:id="rId8"/>
+    <sheet name="OWASP risk value deriving" sheetId="13" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Awareness">'OWASP Rating'!$H$15:$H$24</definedName>
@@ -30,10 +31,10 @@
     <definedName name="ISFOXOldClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXOldClassificationIdBackup" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXPrefix" hidden="1">" "</definedName>
-    <definedName name="ISFOXPreviousClassificationId" localSheetId="6" hidden="1">"d4c75f49-f1ee-485c-aa75-2c54e2ab5223"</definedName>
+    <definedName name="ISFOXPreviousClassificationId" localSheetId="7" hidden="1">"d4c75f49-f1ee-485c-aa75-2c54e2ab5223"</definedName>
     <definedName name="ISFOXPreviousClassificationId" hidden="1">"7d788e96-5802-48f7-b87f-ef0226e41b7c"</definedName>
     <definedName name="ISFOXSaveAsProcess" hidden="1">TRUE</definedName>
-    <definedName name="ISFOXShowClassificationRequestWindow" localSheetId="6" hidden="1">TRUE</definedName>
+    <definedName name="ISFOXShowClassificationRequestWindow" localSheetId="7" hidden="1">TRUE</definedName>
     <definedName name="ISFOXShowClassificationRequestWindow" hidden="1">FALSE</definedName>
     <definedName name="ISFOXVersionHistoryCount" hidden="1">1</definedName>
     <definedName name="ISFOXVersioningChanged" hidden="1">FALSE</definedName>
@@ -163,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="458">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -1534,6 +1535,9 @@
   </si>
   <si>
     <t>The underlying nodes could allow an attacker easy entry, even if the containers themselves are hardened. This includes Side-Channel attacks like Spectre &amp; Meltdown</t>
+  </si>
+  <si>
+    <t>Vector risk assessment - Round 4</t>
   </si>
 </sst>
 </file>
@@ -2203,7 +2207,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2456,6 +2460,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2889,7 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3173,6 +3186,1416 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:R43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="111" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="111" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" s="110">
+        <v>3</v>
+      </c>
+      <c r="D4" s="54">
+        <v>3</v>
+      </c>
+      <c r="E4" s="41">
+        <v>2</v>
+      </c>
+      <c r="F4" s="41">
+        <v>2</v>
+      </c>
+      <c r="G4" s="50">
+        <f>ROUND(((D4+C4+E4+F4)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="48">
+        <f>MIN(10, ROUND(G4*H4, 0))</f>
+        <v>3</v>
+      </c>
+      <c r="J4" s="41">
+        <v>3</v>
+      </c>
+      <c r="K4" s="54">
+        <v>3</v>
+      </c>
+      <c r="L4" s="41">
+        <v>2</v>
+      </c>
+      <c r="M4" s="41">
+        <v>2</v>
+      </c>
+      <c r="N4" s="50">
+        <f>ROUND(((K4+J4+L4+M4)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="48">
+        <f>MIN(10, ROUND(N4*O4, 0))</f>
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q23" si="0">I4-P4</f>
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C5" s="10">
+        <v>3</v>
+      </c>
+      <c r="D5" s="41">
+        <v>2</v>
+      </c>
+      <c r="E5" s="38">
+        <v>2</v>
+      </c>
+      <c r="F5" s="38">
+        <v>2</v>
+      </c>
+      <c r="G5" s="23">
+        <f>ROUND(((D5+C5+E5+F5)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="48">
+        <f>MIN(10, ROUND(G5*H5, 0))</f>
+        <v>7</v>
+      </c>
+      <c r="J5" s="41">
+        <v>3</v>
+      </c>
+      <c r="K5" s="41">
+        <v>2</v>
+      </c>
+      <c r="L5" s="38">
+        <v>2</v>
+      </c>
+      <c r="M5" s="38">
+        <v>2</v>
+      </c>
+      <c r="N5" s="23">
+        <f>ROUND(((K5+J5+L5+M5)/4), 2)</f>
+        <v>2.25</v>
+      </c>
+      <c r="O5" s="4">
+        <v>3</v>
+      </c>
+      <c r="P5" s="48">
+        <f t="shared" ref="P5:P23" si="1">MIN(10, ROUND(N5*O5, 0))</f>
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="C6" s="10">
+        <v>3</v>
+      </c>
+      <c r="D6" s="41">
+        <v>2</v>
+      </c>
+      <c r="E6" s="41">
+        <v>3</v>
+      </c>
+      <c r="F6" s="41">
+        <v>3</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" ref="G6:G22" si="2">ROUND(((D6+C6+E6+F6)/4), 2)</f>
+        <v>2.75</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3</v>
+      </c>
+      <c r="I6" s="48">
+        <f t="shared" ref="I6:I23" si="3">MIN(10, ROUND(G6*H6, 0))</f>
+        <v>8</v>
+      </c>
+      <c r="J6" s="41">
+        <v>3</v>
+      </c>
+      <c r="K6" s="41">
+        <v>1</v>
+      </c>
+      <c r="L6" s="41">
+        <v>3</v>
+      </c>
+      <c r="M6" s="41">
+        <v>3</v>
+      </c>
+      <c r="N6" s="23">
+        <f t="shared" ref="N6:N22" si="4">ROUND(((K6+J6+L6+M6)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="O6" s="4">
+        <v>3</v>
+      </c>
+      <c r="P6" s="48">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C7" s="10">
+        <v>3</v>
+      </c>
+      <c r="D7" s="41">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="I7" s="48">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="38">
+        <v>4</v>
+      </c>
+      <c r="K7" s="38">
+        <v>2</v>
+      </c>
+      <c r="L7" s="38">
+        <v>3</v>
+      </c>
+      <c r="M7" s="38">
+        <v>3</v>
+      </c>
+      <c r="N7" s="23">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>3</v>
+      </c>
+      <c r="P7" s="48">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C8" s="10">
+        <v>3</v>
+      </c>
+      <c r="D8" s="41">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3</v>
+      </c>
+      <c r="I8" s="48">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="J8" s="38">
+        <v>4</v>
+      </c>
+      <c r="K8" s="38">
+        <v>1</v>
+      </c>
+      <c r="L8" s="38">
+        <v>3</v>
+      </c>
+      <c r="M8" s="38">
+        <v>3</v>
+      </c>
+      <c r="N8" s="23">
+        <f t="shared" si="4"/>
+        <v>2.75</v>
+      </c>
+      <c r="O8" s="4">
+        <v>3</v>
+      </c>
+      <c r="P8" s="48">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3</v>
+      </c>
+      <c r="D9" s="41">
+        <v>1</v>
+      </c>
+      <c r="E9" s="41">
+        <v>1</v>
+      </c>
+      <c r="F9" s="41">
+        <v>0</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="H9" s="4">
+        <v>3</v>
+      </c>
+      <c r="I9" s="48">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J9" s="41">
+        <v>3</v>
+      </c>
+      <c r="K9" s="41">
+        <v>1</v>
+      </c>
+      <c r="L9" s="41">
+        <v>1</v>
+      </c>
+      <c r="M9" s="41">
+        <v>0</v>
+      </c>
+      <c r="N9" s="23">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="O9" s="4">
+        <v>3</v>
+      </c>
+      <c r="P9" s="48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="41">
+        <v>4</v>
+      </c>
+      <c r="E10" s="41">
+        <v>3</v>
+      </c>
+      <c r="F10" s="41">
+        <v>3</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
+      <c r="I10" s="48">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="J10" s="41">
+        <v>4</v>
+      </c>
+      <c r="K10" s="41">
+        <v>4</v>
+      </c>
+      <c r="L10" s="41">
+        <v>3</v>
+      </c>
+      <c r="M10" s="41">
+        <v>3</v>
+      </c>
+      <c r="N10" s="23">
+        <f t="shared" si="4"/>
+        <v>3.5</v>
+      </c>
+      <c r="O10" s="38">
+        <v>2</v>
+      </c>
+      <c r="P10" s="48">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="41">
+        <v>4</v>
+      </c>
+      <c r="E11" s="41">
+        <v>3</v>
+      </c>
+      <c r="F11" s="41">
+        <v>2</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="2"/>
+        <v>3.25</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3</v>
+      </c>
+      <c r="I11" s="48">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="J11" s="41">
+        <v>4</v>
+      </c>
+      <c r="K11" s="41">
+        <v>4</v>
+      </c>
+      <c r="L11" s="41">
+        <v>3</v>
+      </c>
+      <c r="M11" s="41">
+        <v>2</v>
+      </c>
+      <c r="N11" s="23">
+        <f t="shared" si="4"/>
+        <v>3.25</v>
+      </c>
+      <c r="O11" s="38">
+        <v>3</v>
+      </c>
+      <c r="P11" s="48">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>453</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="38">
+        <v>2</v>
+      </c>
+      <c r="E12" s="41">
+        <v>2</v>
+      </c>
+      <c r="F12" s="41">
+        <v>2</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3</v>
+      </c>
+      <c r="I12" s="48">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="J12" s="41">
+        <v>2</v>
+      </c>
+      <c r="K12" s="38">
+        <v>2</v>
+      </c>
+      <c r="L12" s="41">
+        <v>2</v>
+      </c>
+      <c r="M12" s="41">
+        <v>2</v>
+      </c>
+      <c r="N12" s="23">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="O12" s="38">
+        <v>2</v>
+      </c>
+      <c r="P12" s="48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="C13" s="23">
+        <v>2</v>
+      </c>
+      <c r="D13" s="41">
+        <v>3</v>
+      </c>
+      <c r="E13" s="38">
+        <v>3</v>
+      </c>
+      <c r="F13" s="38">
+        <v>2</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>3</v>
+      </c>
+      <c r="I13" s="48">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="J13" s="38">
+        <v>2</v>
+      </c>
+      <c r="K13" s="41">
+        <v>3</v>
+      </c>
+      <c r="L13" s="38">
+        <v>3</v>
+      </c>
+      <c r="M13" s="38">
+        <v>2</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="O13" s="38">
+        <v>3</v>
+      </c>
+      <c r="P13" s="48">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="41">
+        <v>2</v>
+      </c>
+      <c r="E14" s="41">
+        <v>2</v>
+      </c>
+      <c r="F14" s="41">
+        <v>1</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2</v>
+      </c>
+      <c r="I14" s="48">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J14" s="41">
+        <v>1</v>
+      </c>
+      <c r="K14" s="41">
+        <v>2</v>
+      </c>
+      <c r="L14" s="41">
+        <v>2</v>
+      </c>
+      <c r="M14" s="41">
+        <v>1</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="O14" s="38">
+        <v>2</v>
+      </c>
+      <c r="P14" s="48">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>440</v>
+      </c>
+      <c r="C15" s="23">
+        <v>2</v>
+      </c>
+      <c r="D15" s="41">
+        <v>2</v>
+      </c>
+      <c r="E15" s="38">
+        <v>3</v>
+      </c>
+      <c r="F15" s="38">
+        <v>3</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2</v>
+      </c>
+      <c r="I15" s="48">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J15" s="38">
+        <v>2</v>
+      </c>
+      <c r="K15" s="41">
+        <v>2</v>
+      </c>
+      <c r="L15" s="38">
+        <v>3</v>
+      </c>
+      <c r="M15" s="38">
+        <v>3</v>
+      </c>
+      <c r="N15" s="23">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="O15" s="38">
+        <v>2</v>
+      </c>
+      <c r="P15" s="48">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>441</v>
+      </c>
+      <c r="C16" s="23">
+        <v>2</v>
+      </c>
+      <c r="D16" s="41">
+        <v>2</v>
+      </c>
+      <c r="E16" s="38">
+        <v>3</v>
+      </c>
+      <c r="F16" s="38">
+        <v>3</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="48">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J16" s="38">
+        <v>2</v>
+      </c>
+      <c r="K16" s="41">
+        <v>2</v>
+      </c>
+      <c r="L16" s="38">
+        <v>3</v>
+      </c>
+      <c r="M16" s="38">
+        <v>3</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="O16" s="38">
+        <v>1</v>
+      </c>
+      <c r="P16" s="48">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="C17" s="23">
+        <v>2</v>
+      </c>
+      <c r="D17" s="41">
+        <v>1</v>
+      </c>
+      <c r="E17" s="38">
+        <v>3</v>
+      </c>
+      <c r="F17" s="38">
+        <v>3</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="H17" s="4">
+        <v>3</v>
+      </c>
+      <c r="I17" s="48">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="J17" s="38">
+        <v>2</v>
+      </c>
+      <c r="K17" s="41">
+        <v>1</v>
+      </c>
+      <c r="L17" s="38">
+        <v>3</v>
+      </c>
+      <c r="M17" s="38">
+        <v>3</v>
+      </c>
+      <c r="N17" s="23">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="O17" s="38">
+        <v>2</v>
+      </c>
+      <c r="P17" s="48">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>443</v>
+      </c>
+      <c r="C18" s="23">
+        <v>2</v>
+      </c>
+      <c r="D18" s="41">
+        <v>1</v>
+      </c>
+      <c r="E18" s="38">
+        <v>3</v>
+      </c>
+      <c r="F18" s="38">
+        <v>3</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2</v>
+      </c>
+      <c r="I18" s="48">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J18" s="38">
+        <v>2</v>
+      </c>
+      <c r="K18" s="41">
+        <v>1</v>
+      </c>
+      <c r="L18" s="38">
+        <v>3</v>
+      </c>
+      <c r="M18" s="38">
+        <v>3</v>
+      </c>
+      <c r="N18" s="23">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="O18" s="38">
+        <v>3</v>
+      </c>
+      <c r="P18" s="48">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>444</v>
+      </c>
+      <c r="C19" s="23">
+        <v>1</v>
+      </c>
+      <c r="D19" s="41">
+        <v>2</v>
+      </c>
+      <c r="E19" s="38">
+        <v>3</v>
+      </c>
+      <c r="F19" s="38">
+        <v>3</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2</v>
+      </c>
+      <c r="I19" s="48">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J19" s="38">
+        <v>1</v>
+      </c>
+      <c r="K19" s="41">
+        <v>2</v>
+      </c>
+      <c r="L19" s="38">
+        <v>3</v>
+      </c>
+      <c r="M19" s="38">
+        <v>3</v>
+      </c>
+      <c r="N19" s="23">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="O19" s="38">
+        <v>2</v>
+      </c>
+      <c r="P19" s="48">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>445</v>
+      </c>
+      <c r="C20" s="23">
+        <v>1</v>
+      </c>
+      <c r="D20" s="41">
+        <v>1</v>
+      </c>
+      <c r="E20" s="38">
+        <v>2</v>
+      </c>
+      <c r="F20" s="38">
+        <v>2</v>
+      </c>
+      <c r="G20" s="23">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>3</v>
+      </c>
+      <c r="I20" s="48">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J20" s="38">
+        <v>1</v>
+      </c>
+      <c r="K20" s="41">
+        <v>1</v>
+      </c>
+      <c r="L20" s="38">
+        <v>2</v>
+      </c>
+      <c r="M20" s="38">
+        <v>1</v>
+      </c>
+      <c r="N20" s="23">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="O20" s="38">
+        <v>3</v>
+      </c>
+      <c r="P20" s="48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="23">
+        <v>4</v>
+      </c>
+      <c r="D21" s="41">
+        <v>4</v>
+      </c>
+      <c r="E21" s="38">
+        <v>1</v>
+      </c>
+      <c r="F21" s="38">
+        <v>2</v>
+      </c>
+      <c r="G21" s="23">
+        <f t="shared" si="2"/>
+        <v>2.75</v>
+      </c>
+      <c r="H21" s="4">
+        <v>3</v>
+      </c>
+      <c r="I21" s="48">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="J21" s="38">
+        <v>4</v>
+      </c>
+      <c r="K21" s="41">
+        <v>4</v>
+      </c>
+      <c r="L21" s="38">
+        <v>1</v>
+      </c>
+      <c r="M21" s="38">
+        <v>2</v>
+      </c>
+      <c r="N21" s="23">
+        <f t="shared" si="4"/>
+        <v>2.75</v>
+      </c>
+      <c r="O21" s="38">
+        <v>3</v>
+      </c>
+      <c r="P21" s="48">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="23">
+        <v>4</v>
+      </c>
+      <c r="D22" s="41">
+        <v>4</v>
+      </c>
+      <c r="E22" s="38">
+        <v>2</v>
+      </c>
+      <c r="F22" s="38">
+        <v>2</v>
+      </c>
+      <c r="G22" s="23">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="4">
+        <v>3</v>
+      </c>
+      <c r="I22" s="48">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="J22" s="38">
+        <v>4</v>
+      </c>
+      <c r="K22" s="41">
+        <v>4</v>
+      </c>
+      <c r="L22" s="38">
+        <v>2</v>
+      </c>
+      <c r="M22" s="38">
+        <v>1</v>
+      </c>
+      <c r="N22" s="23">
+        <f t="shared" si="4"/>
+        <v>2.75</v>
+      </c>
+      <c r="O22" s="38">
+        <v>3</v>
+      </c>
+      <c r="P22" s="48">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>446</v>
+      </c>
+      <c r="C23" s="39">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6">
+        <v>4</v>
+      </c>
+      <c r="E23" s="40">
+        <v>3</v>
+      </c>
+      <c r="F23" s="40">
+        <v>3</v>
+      </c>
+      <c r="G23" s="39">
+        <f>ROUND(((D23+C23+E23+F23)/4), 2)</f>
+        <v>3.5</v>
+      </c>
+      <c r="H23" s="6">
+        <v>3</v>
+      </c>
+      <c r="I23" s="49">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="J23" s="40">
+        <v>4</v>
+      </c>
+      <c r="K23" s="6">
+        <v>4</v>
+      </c>
+      <c r="L23" s="40">
+        <v>3</v>
+      </c>
+      <c r="M23" s="40">
+        <v>3</v>
+      </c>
+      <c r="N23" s="39">
+        <f>ROUND(((K23+J23+L23+M23)/4), 2)</f>
+        <v>3.5</v>
+      </c>
+      <c r="O23" s="40">
+        <v>3</v>
+      </c>
+      <c r="P23" s="49">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="43"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="43"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="43"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="44"/>
+      <c r="G28" s="41"/>
+      <c r="N28" s="41"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K30"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="6" id="{CE3E1A35-17C1-4254-BDAA-DB91301DFA4F}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>P4:P23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="7" id="{709B235F-63E3-4660-B256-0309169812CD}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I4:I23</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5394,14 +6817,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5612,7 +7037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W61"/>
   <sheetViews>
@@ -5663,30 +7088,30 @@
       <c r="A4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="121" t="s">
         <v>286</v>
       </c>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="118" t="s">
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="122"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="119"/>
-      <c r="P4" s="119"/>
-      <c r="Q4" s="119"/>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
-      <c r="T4" s="119"/>
-      <c r="U4" s="119"/>
-      <c r="V4" s="119"/>
-      <c r="W4" s="120"/>
+      <c r="O4" s="122"/>
+      <c r="P4" s="122"/>
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122"/>
+      <c r="S4" s="122"/>
+      <c r="T4" s="122"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="122"/>
+      <c r="W4" s="123"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -7136,30 +8561,30 @@
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="118" t="s">
+      <c r="D28" s="121" t="s">
         <v>286</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119"/>
-      <c r="I28" s="119"/>
-      <c r="J28" s="119"/>
-      <c r="K28" s="119"/>
-      <c r="L28" s="119"/>
-      <c r="M28" s="120"/>
-      <c r="N28" s="118" t="s">
+      <c r="E28" s="122"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="122"/>
+      <c r="H28" s="122"/>
+      <c r="I28" s="122"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="123"/>
+      <c r="N28" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="O28" s="119"/>
-      <c r="P28" s="119"/>
-      <c r="Q28" s="119"/>
-      <c r="R28" s="119"/>
-      <c r="S28" s="119"/>
-      <c r="T28" s="119"/>
-      <c r="U28" s="119"/>
-      <c r="V28" s="119"/>
-      <c r="W28" s="120"/>
+      <c r="O28" s="122"/>
+      <c r="P28" s="122"/>
+      <c r="Q28" s="122"/>
+      <c r="R28" s="122"/>
+      <c r="S28" s="122"/>
+      <c r="T28" s="122"/>
+      <c r="U28" s="122"/>
+      <c r="V28" s="122"/>
+      <c r="W28" s="123"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -8602,26 +10027,26 @@
       </c>
     </row>
     <row r="53" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="121" t="s">
+      <c r="C53" s="124" t="s">
         <v>378</v>
       </c>
-      <c r="D53" s="122"/>
-      <c r="E53" s="123"/>
-      <c r="F53" s="123"/>
-      <c r="G53" s="124"/>
-      <c r="I53" s="125" t="s">
+      <c r="D53" s="125"/>
+      <c r="E53" s="126"/>
+      <c r="F53" s="126"/>
+      <c r="G53" s="127"/>
+      <c r="I53" s="128" t="s">
         <v>379</v>
       </c>
-      <c r="J53" s="124"/>
+      <c r="J53" s="127"/>
     </row>
     <row r="54" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="110"/>
-      <c r="D54" s="111"/>
-      <c r="E54" s="114" t="s">
+      <c r="C54" s="113"/>
+      <c r="D54" s="114"/>
+      <c r="E54" s="117" t="s">
         <v>286</v>
       </c>
-      <c r="F54" s="114"/>
-      <c r="G54" s="115"/>
+      <c r="F54" s="117"/>
+      <c r="G54" s="118"/>
       <c r="I54" s="78" t="s">
         <v>388</v>
       </c>
@@ -8630,8 +10055,8 @@
       </c>
     </row>
     <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="112"/>
-      <c r="D55" s="113"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="116"/>
       <c r="E55" s="89" t="s">
         <v>385</v>
       </c>
@@ -8649,7 +10074,7 @@
       </c>
     </row>
     <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="116" t="s">
+      <c r="C56" s="119" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="78" t="s">
@@ -8672,7 +10097,7 @@
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C57" s="116"/>
+      <c r="C57" s="119"/>
       <c r="D57" s="78" t="s">
         <v>386</v>
       </c>
@@ -8687,7 +10112,7 @@
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C58" s="117"/>
+      <c r="C58" s="120"/>
       <c r="D58" s="88" t="s">
         <v>380</v>
       </c>
@@ -8829,7 +10254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
@@ -9504,7 +10929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
@@ -9560,16 +10985,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="126" t="s">
+      <c r="A4" s="129" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="128"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="131"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -9702,16 +11127,16 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="129" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="127"/>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="128"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="131"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
@@ -9768,16 +11193,16 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="126" t="s">
+      <c r="A18" s="129" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="127"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="128"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="131"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
@@ -9832,16 +11257,16 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="126" t="s">
+      <c r="A23" s="129" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="127"/>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="128"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="131"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
@@ -9898,16 +11323,16 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="126" t="s">
+      <c r="A28" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="127"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="127"/>
-      <c r="E28" s="127"/>
-      <c r="F28" s="127"/>
-      <c r="G28" s="127"/>
-      <c r="H28" s="128"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="131"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
@@ -10027,7 +11452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
@@ -11153,7 +12578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>

</xml_diff>

<commit_message>
new risk rating estimate (final validation pending), started explanation for it
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
-    <sheet name="Vector risk assessment 2" sheetId="14" r:id="rId2"/>
-    <sheet name="Vector risk assessment" sheetId="5" r:id="rId3"/>
+    <sheet name="Vector risk assessment v4" sheetId="14" r:id="rId2"/>
+    <sheet name="(old) Vector risk assessment" sheetId="5" r:id="rId3"/>
     <sheet name="Risk assessment formula" sheetId="2" r:id="rId4"/>
     <sheet name="Vector Risk assessment OWASP" sheetId="11" r:id="rId5"/>
     <sheet name="Measure TempDump" sheetId="8" r:id="rId6"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="459">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -1538,6 +1538,9 @@
   </si>
   <si>
     <t>Vector risk assessment - Round 4</t>
+  </si>
+  <si>
+    <t>&lt;- two cases: cluster admin and/or namespace admin. Admin has higher risk</t>
   </si>
 </sst>
 </file>
@@ -1788,7 +1791,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -2201,13 +2204,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2470,6 +2503,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2903,7 +2957,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3193,7 +3247,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3213,6 +3267,8 @@
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="81.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
@@ -3299,14 +3355,14 @@
         <v>3</v>
       </c>
       <c r="E4" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="41">
         <v>2</v>
       </c>
       <c r="G4" s="50">
         <f>ROUND(((D4+C4+E4+F4)/4), 2)</f>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
@@ -3316,20 +3372,20 @@
         <v>3</v>
       </c>
       <c r="J4" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4" s="54">
         <v>3</v>
       </c>
       <c r="L4" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" s="41">
         <v>2</v>
       </c>
       <c r="N4" s="50">
         <f>ROUND(((K4+J4+L4+M4)/4), 2)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="O4" s="4">
         <v>1</v>
@@ -3342,9 +3398,6 @@
         <f t="shared" ref="Q4:Q23" si="0">I4-P4</f>
         <v>0</v>
       </c>
-      <c r="R4" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -3357,43 +3410,43 @@
         <v>3</v>
       </c>
       <c r="D5" s="41">
-        <v>2</v>
-      </c>
-      <c r="E5" s="38">
-        <v>2</v>
-      </c>
-      <c r="F5" s="38">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
       </c>
       <c r="G5" s="23">
         <f>ROUND(((D5+C5+E5+F5)/4), 2)</f>
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="H5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" s="48">
         <f>MIN(10, ROUND(G5*H5, 0))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="41">
-        <v>2</v>
-      </c>
-      <c r="L5" s="38">
-        <v>2</v>
-      </c>
-      <c r="M5" s="38">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L5" s="4">
+        <v>3</v>
+      </c>
+      <c r="M5" s="4">
+        <v>3</v>
       </c>
       <c r="N5" s="23">
         <f>ROUND(((K5+J5+L5+M5)/4), 2)</f>
-        <v>2.25</v>
+        <v>3.25</v>
       </c>
       <c r="O5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P5" s="48">
         <f t="shared" ref="P5:P23" si="1">MIN(10, ROUND(N5*O5, 0))</f>
@@ -3401,10 +3454,7 @@
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>56</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -3418,7 +3468,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="41">
         <v>3</v>
@@ -3428,7 +3478,7 @@
       </c>
       <c r="G6" s="23">
         <f t="shared" ref="G6:G22" si="2">ROUND(((D6+C6+E6+F6)/4), 2)</f>
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="H6" s="4">
         <v>3</v>
@@ -3438,7 +3488,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" s="41">
         <v>1</v>
@@ -3451,7 +3501,7 @@
       </c>
       <c r="N6" s="23">
         <f t="shared" ref="N6:N22" si="4">ROUND(((K6+J6+L6+M6)/4), 2)</f>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="O6" s="4">
         <v>3</v>
@@ -3465,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>56</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -3479,7 +3529,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4">
         <v>3</v>
@@ -3489,20 +3539,20 @@
       </c>
       <c r="G7" s="23">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="H7" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" s="48">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J7" s="38">
         <v>4</v>
       </c>
       <c r="K7" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L7" s="38">
         <v>3</v>
@@ -3512,22 +3562,19 @@
       </c>
       <c r="N7" s="23">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="O7" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P7" s="48">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="R7" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
@@ -3587,7 +3634,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>56</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3621,7 +3668,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K9" s="41">
         <v>1</v>
@@ -3634,21 +3681,18 @@
       </c>
       <c r="N9" s="23">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="O9" s="4">
         <v>3</v>
       </c>
       <c r="P9" s="48">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>56</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3668,11 +3712,11 @@
         <v>3</v>
       </c>
       <c r="F10" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="23">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="H10" s="4">
         <v>2</v>
@@ -3691,11 +3735,11 @@
         <v>3</v>
       </c>
       <c r="M10" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N10" s="23">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="O10" s="38">
         <v>2</v>
@@ -3766,9 +3810,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R11" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
@@ -3784,48 +3825,48 @@
         <v>2</v>
       </c>
       <c r="E12" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="41">
         <v>2</v>
       </c>
       <c r="G12" s="23">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="H12" s="4">
         <v>3</v>
       </c>
       <c r="I12" s="48">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="J12" s="41">
+        <v>7</v>
+      </c>
+      <c r="J12" s="10">
         <v>2</v>
       </c>
       <c r="K12" s="38">
         <v>2</v>
       </c>
       <c r="L12" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12" s="41">
         <v>2</v>
       </c>
       <c r="N12" s="23">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="O12" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P12" s="48">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -3839,30 +3880,30 @@
         <v>2</v>
       </c>
       <c r="D13" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="38">
         <v>3</v>
       </c>
       <c r="F13" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="23">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H13" s="4">
         <v>3</v>
       </c>
       <c r="I13" s="48">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="J13" s="38">
+        <v>6</v>
+      </c>
+      <c r="J13" s="23">
         <v>2</v>
       </c>
       <c r="K13" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L13" s="38">
         <v>3</v>
@@ -3872,21 +3913,18 @@
       </c>
       <c r="N13" s="23">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="O13" s="38">
         <v>3</v>
       </c>
       <c r="P13" s="48">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R13" t="s">
-        <v>56</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -3900,13 +3938,13 @@
         <v>1</v>
       </c>
       <c r="D14" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="41">
         <v>2</v>
       </c>
       <c r="F14" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="23">
         <f t="shared" si="2"/>
@@ -3919,17 +3957,17 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="10">
         <v>1</v>
       </c>
       <c r="K14" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="41">
         <v>2</v>
       </c>
       <c r="M14" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="23">
         <f t="shared" si="4"/>
@@ -4013,7 +4051,7 @@
         <v>441</v>
       </c>
       <c r="C16" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="41">
         <v>2</v>
@@ -4026,7 +4064,7 @@
       </c>
       <c r="G16" s="23">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="H16" s="4">
         <v>1</v>
@@ -4063,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
         <v>86</v>
       </c>
@@ -4071,43 +4109,43 @@
         <v>442</v>
       </c>
       <c r="C17" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="38">
         <v>3</v>
       </c>
       <c r="F17" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17" s="23">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="H17" s="4">
         <v>3</v>
       </c>
       <c r="I17" s="48">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J17" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K17" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="38">
         <v>3</v>
       </c>
       <c r="M17" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N17" s="23">
         <f t="shared" si="4"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="O17" s="38">
         <v>2</v>
@@ -4118,13 +4156,10 @@
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
         <v>87</v>
       </c>
@@ -4132,10 +4167,10 @@
         <v>443</v>
       </c>
       <c r="C18" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="38">
         <v>3</v>
@@ -4145,20 +4180,20 @@
       </c>
       <c r="G18" s="23">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="H18" s="4">
         <v>2</v>
       </c>
       <c r="I18" s="48">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J18" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="38">
         <v>3</v>
@@ -4168,21 +4203,21 @@
       </c>
       <c r="N18" s="23">
         <f t="shared" si="4"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="O18" s="38">
         <v>3</v>
       </c>
       <c r="P18" s="48">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
         <v>88</v>
       </c>
@@ -4190,7 +4225,7 @@
         <v>444</v>
       </c>
       <c r="C19" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="41">
         <v>2</v>
@@ -4199,11 +4234,11 @@
         <v>3</v>
       </c>
       <c r="F19" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="23">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="H19" s="4">
         <v>2</v>
@@ -4213,7 +4248,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K19" s="41">
         <v>2</v>
@@ -4222,25 +4257,25 @@
         <v>3</v>
       </c>
       <c r="M19" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19" s="23">
         <f t="shared" si="4"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="O19" s="38">
         <v>2</v>
       </c>
       <c r="P19" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
         <v>89</v>
       </c>
@@ -4248,7 +4283,7 @@
         <v>445</v>
       </c>
       <c r="C20" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" s="41">
         <v>1</v>
@@ -4261,47 +4296,44 @@
       </c>
       <c r="G20" s="23">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H20" s="4">
         <v>3</v>
       </c>
       <c r="I20" s="48">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J20" s="38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K20" s="41">
         <v>1</v>
       </c>
       <c r="L20" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" s="23">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="O20" s="38">
         <v>3</v>
       </c>
       <c r="P20" s="48">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
         <v>90</v>
       </c>
@@ -4309,13 +4341,13 @@
         <v>53</v>
       </c>
       <c r="C21" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" s="41">
         <v>4</v>
       </c>
       <c r="E21" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="38">
         <v>2</v>
@@ -4325,11 +4357,11 @@
         <v>2.75</v>
       </c>
       <c r="H21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I21" s="48">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J21" s="38">
         <v>4</v>
@@ -4338,31 +4370,28 @@
         <v>4</v>
       </c>
       <c r="L21" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" s="38">
         <v>2</v>
       </c>
       <c r="N21" s="23">
         <f t="shared" si="4"/>
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="O21" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P21" s="48">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>91</v>
       </c>
@@ -4420,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>92</v>
       </c>
@@ -4477,72 +4506,244 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="43"/>
       <c r="J25" s="37"/>
       <c r="K25" s="37"/>
       <c r="L25" s="37"/>
       <c r="M25" s="37"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="43"/>
       <c r="J26" s="37"/>
       <c r="K26" s="37"/>
       <c r="L26" s="37"/>
       <c r="M26" s="37"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="43"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="44"/>
       <c r="G28" s="41"/>
       <c r="N28" s="41"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K30"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K31"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K32"/>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33"/>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34"/>
-    </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35"/>
-    </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36"/>
-    </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="117"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="117"/>
+      <c r="J29" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="117"/>
+      <c r="L29" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" s="117"/>
+      <c r="N29" s="116" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="113" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="113"/>
+      <c r="L31" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="113"/>
+      <c r="N31" s="113"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="113"/>
+      <c r="D32" s="113"/>
+      <c r="E32" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="113"/>
+      <c r="G32" s="113"/>
+      <c r="H32" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="113"/>
+      <c r="J32" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="113"/>
+      <c r="L32" s="113" t="s">
+        <v>13</v>
+      </c>
+      <c r="M32" s="113"/>
+      <c r="N32" s="113"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="113" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="113"/>
+      <c r="D33" s="113"/>
+      <c r="E33" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="113"/>
+      <c r="G33" s="113"/>
+      <c r="H33" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="113"/>
+      <c r="J33" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="113"/>
+      <c r="L33" s="113" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" s="113"/>
+      <c r="N33" s="113"/>
+    </row>
+    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="119" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="120"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="120"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="120"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="120"/>
+      <c r="L35" s="121" t="s">
+        <v>37</v>
+      </c>
+      <c r="M35" s="120"/>
+      <c r="N35" s="119" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="115" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="113"/>
+      <c r="D36" s="113"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="113"/>
+      <c r="G36" s="113"/>
+      <c r="H36" s="113"/>
+      <c r="I36" s="113"/>
+      <c r="J36" s="113"/>
+      <c r="K36" s="113"/>
+      <c r="L36" s="114"/>
+      <c r="M36" s="113"/>
+      <c r="N36" s="115" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K37"/>
-    </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K38"/>
-    </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K39"/>
-    </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K40"/>
-    </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K41"/>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K42"/>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K43"/>
     </row>
   </sheetData>
@@ -4602,8 +4803,8 @@
   </sheetPr>
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6825,7 +7026,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A3" sqref="A3:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7088,30 +7289,30 @@
       <c r="A4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="130" t="s">
         <v>286</v>
       </c>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="121" t="s">
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="132"/>
+      <c r="N4" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="122"/>
-      <c r="W4" s="123"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="131"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="132"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -8561,30 +8762,30 @@
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="121" t="s">
+      <c r="D28" s="130" t="s">
         <v>286</v>
       </c>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="122"/>
-      <c r="I28" s="122"/>
-      <c r="J28" s="122"/>
-      <c r="K28" s="122"/>
-      <c r="L28" s="122"/>
-      <c r="M28" s="123"/>
-      <c r="N28" s="121" t="s">
+      <c r="E28" s="131"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="131"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="132"/>
+      <c r="N28" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="O28" s="122"/>
-      <c r="P28" s="122"/>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="122"/>
-      <c r="S28" s="122"/>
-      <c r="T28" s="122"/>
-      <c r="U28" s="122"/>
-      <c r="V28" s="122"/>
-      <c r="W28" s="123"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="131"/>
+      <c r="Q28" s="131"/>
+      <c r="R28" s="131"/>
+      <c r="S28" s="131"/>
+      <c r="T28" s="131"/>
+      <c r="U28" s="131"/>
+      <c r="V28" s="131"/>
+      <c r="W28" s="132"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -10027,26 +10228,26 @@
       </c>
     </row>
     <row r="53" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="124" t="s">
+      <c r="C53" s="133" t="s">
         <v>378</v>
       </c>
-      <c r="D53" s="125"/>
-      <c r="E53" s="126"/>
-      <c r="F53" s="126"/>
-      <c r="G53" s="127"/>
-      <c r="I53" s="128" t="s">
+      <c r="D53" s="134"/>
+      <c r="E53" s="135"/>
+      <c r="F53" s="135"/>
+      <c r="G53" s="136"/>
+      <c r="I53" s="137" t="s">
         <v>379</v>
       </c>
-      <c r="J53" s="127"/>
+      <c r="J53" s="136"/>
     </row>
     <row r="54" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="113"/>
-      <c r="D54" s="114"/>
-      <c r="E54" s="117" t="s">
+      <c r="C54" s="122"/>
+      <c r="D54" s="123"/>
+      <c r="E54" s="126" t="s">
         <v>286</v>
       </c>
-      <c r="F54" s="117"/>
-      <c r="G54" s="118"/>
+      <c r="F54" s="126"/>
+      <c r="G54" s="127"/>
       <c r="I54" s="78" t="s">
         <v>388</v>
       </c>
@@ -10055,8 +10256,8 @@
       </c>
     </row>
     <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="115"/>
-      <c r="D55" s="116"/>
+      <c r="C55" s="124"/>
+      <c r="D55" s="125"/>
       <c r="E55" s="89" t="s">
         <v>385</v>
       </c>
@@ -10074,7 +10275,7 @@
       </c>
     </row>
     <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="119" t="s">
+      <c r="C56" s="128" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="78" t="s">
@@ -10097,7 +10298,7 @@
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C57" s="119"/>
+      <c r="C57" s="128"/>
       <c r="D57" s="78" t="s">
         <v>386</v>
       </c>
@@ -10112,7 +10313,7 @@
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C58" s="120"/>
+      <c r="C58" s="129"/>
       <c r="D58" s="88" t="s">
         <v>380</v>
       </c>
@@ -10985,16 +11186,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="138" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="131"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="140"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -11127,16 +11328,16 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="130"/>
-      <c r="C13" s="130"/>
-      <c r="D13" s="130"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="131"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="140"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
@@ -11193,16 +11394,16 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="129" t="s">
+      <c r="A18" s="138" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="130"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="131"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="140"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
@@ -11257,16 +11458,16 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="130"/>
-      <c r="C23" s="130"/>
-      <c r="D23" s="130"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="131"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="140"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
@@ -11323,16 +11524,16 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="129" t="s">
+      <c r="A28" s="138" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="131"/>
+      <c r="B28" s="139"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="140"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">

</xml_diff>

<commit_message>
finished rating explanation, final check-over pending
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="458">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -1538,9 +1538,6 @@
   </si>
   <si>
     <t>Vector risk assessment - Round 4</t>
-  </si>
-  <si>
-    <t>&lt;- two cases: cluster admin and/or namespace admin. Admin has higher risk</t>
   </si>
 </sst>
 </file>
@@ -2957,7 +2954,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,10 +3241,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,12 +3268,12 @@
     <col min="19" max="19" width="81.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
@@ -3288,7 +3285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>110</v>
       </c>
@@ -3341,7 +3338,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>73</v>
       </c>
@@ -3399,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>74</v>
       </c>
@@ -3457,7 +3454,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
         <v>75</v>
       </c>
@@ -3474,18 +3471,18 @@
         <v>3</v>
       </c>
       <c r="F6" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="23">
         <f t="shared" ref="G6:G22" si="2">ROUND(((D6+C6+E6+F6)/4), 2)</f>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="H6" s="4">
         <v>3</v>
       </c>
       <c r="I6" s="48">
         <f t="shared" ref="I6:I23" si="3">MIN(10, ROUND(G6*H6, 0))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J6" s="41">
         <v>4</v>
@@ -3497,11 +3494,11 @@
         <v>3</v>
       </c>
       <c r="M6" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6" s="23">
         <f t="shared" ref="N6:N22" si="4">ROUND(((K6+J6+L6+M6)/4), 2)</f>
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="O6" s="4">
         <v>3</v>
@@ -3512,13 +3509,10 @@
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
         <v>76</v>
       </c>
@@ -3576,7 +3570,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
         <v>77</v>
       </c>
@@ -3593,18 +3587,18 @@
         <v>3</v>
       </c>
       <c r="F8" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="23">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="H8" s="4">
         <v>3</v>
       </c>
       <c r="I8" s="48">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="38">
         <v>4</v>
@@ -3616,11 +3610,11 @@
         <v>3</v>
       </c>
       <c r="M8" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N8" s="23">
         <f t="shared" si="4"/>
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="O8" s="4">
         <v>3</v>
@@ -3631,13 +3625,10 @@
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R8" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
         <v>78</v>
       </c>
@@ -3651,21 +3642,21 @@
         <v>1</v>
       </c>
       <c r="E9" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="41">
         <v>0</v>
       </c>
       <c r="G9" s="23">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="H9" s="4">
         <v>3</v>
       </c>
       <c r="I9" s="48">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J9" s="41">
         <v>4</v>
@@ -3674,28 +3665,28 @@
         <v>1</v>
       </c>
       <c r="L9" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M9" s="41">
         <v>0</v>
       </c>
       <c r="N9" s="23">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="O9" s="4">
         <v>3</v>
       </c>
       <c r="P9" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
         <v>79</v>
       </c>
@@ -3753,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>80</v>
       </c>
@@ -3811,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>81</v>
       </c>
@@ -3869,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
         <v>82</v>
       </c>
@@ -3927,7 +3918,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>83</v>
       </c>
@@ -3985,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
         <v>84</v>
       </c>
@@ -4002,11 +3993,11 @@
         <v>3</v>
       </c>
       <c r="F15" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="23">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="H15" s="4">
         <v>2</v>
@@ -4025,11 +4016,11 @@
         <v>3</v>
       </c>
       <c r="M15" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N15" s="23">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="O15" s="38">
         <v>2</v>
@@ -4043,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
         <v>85</v>
       </c>
@@ -4080,25 +4071,25 @@
         <v>2</v>
       </c>
       <c r="L16" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" s="38">
         <v>3</v>
       </c>
       <c r="N16" s="23">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="O16" s="38">
         <v>1</v>
       </c>
       <c r="P16" s="48">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -4176,18 +4167,18 @@
         <v>3</v>
       </c>
       <c r="F18" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" s="23">
         <f t="shared" si="2"/>
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="H18" s="4">
         <v>2</v>
       </c>
       <c r="I18" s="48">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J18" s="38">
         <v>3</v>
@@ -4199,11 +4190,11 @@
         <v>3</v>
       </c>
       <c r="M18" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N18" s="23">
         <f t="shared" si="4"/>
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="O18" s="38">
         <v>3</v>
@@ -4214,7 +4205,7 @@
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -4315,22 +4306,22 @@
         <v>1</v>
       </c>
       <c r="M20" s="38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N20" s="23">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="O20" s="38">
         <v>3</v>
       </c>
       <c r="P20" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -4431,22 +4422,22 @@
         <v>2</v>
       </c>
       <c r="M22" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N22" s="23">
         <f t="shared" si="4"/>
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="O22" s="38">
         <v>3</v>
       </c>
       <c r="P22" s="48">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -4466,11 +4457,11 @@
         <v>3</v>
       </c>
       <c r="F23" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" s="39">
         <f>ROUND(((D23+C23+E23+F23)/4), 2)</f>
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="H23" s="6">
         <v>3</v>
@@ -4489,11 +4480,11 @@
         <v>3</v>
       </c>
       <c r="M23" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N23" s="39">
         <f>ROUND(((K23+J23+L23+M23)/4), 2)</f>
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="O23" s="40">
         <v>3</v>
@@ -7026,7 +7017,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H14"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
moved explanation into chapters.tex (not typeset yet)
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -2483,6 +2483,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2539,12 +2545,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2920,8 +2920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6809,7 +6809,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -6977,48 +6977,48 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="34"/>
-      <c r="E11" s="133" t="s">
+      <c r="E11" s="114" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
-      <c r="E12" s="132" t="s">
+      <c r="E12" s="113" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
-      <c r="E13" s="132" t="s">
+      <c r="E13" s="113" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
-      <c r="E14" s="132" t="s">
+      <c r="E14" s="113" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="132" t="s">
+      <c r="D15" s="113" t="s">
         <v>454</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="132" t="s">
+      <c r="D16" s="113" t="s">
         <v>455</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="132" t="s">
+      <c r="D17" s="113" t="s">
         <v>456</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="132" t="s">
+      <c r="D18" s="113" t="s">
         <v>457</v>
       </c>
       <c r="E18" s="3"/>
@@ -7101,30 +7101,30 @@
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="123" t="s">
         <v>282</v>
       </c>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="121" t="s">
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="125"/>
+      <c r="N4" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="122"/>
-      <c r="W4" s="123"/>
+      <c r="O4" s="124"/>
+      <c r="P4" s="124"/>
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
+      <c r="T4" s="124"/>
+      <c r="U4" s="124"/>
+      <c r="V4" s="124"/>
+      <c r="W4" s="125"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -8574,30 +8574,30 @@
       <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="121" t="s">
+      <c r="D28" s="123" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="122"/>
-      <c r="I28" s="122"/>
-      <c r="J28" s="122"/>
-      <c r="K28" s="122"/>
-      <c r="L28" s="122"/>
-      <c r="M28" s="123"/>
-      <c r="N28" s="121" t="s">
+      <c r="E28" s="124"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="124"/>
+      <c r="I28" s="124"/>
+      <c r="J28" s="124"/>
+      <c r="K28" s="124"/>
+      <c r="L28" s="124"/>
+      <c r="M28" s="125"/>
+      <c r="N28" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="O28" s="122"/>
-      <c r="P28" s="122"/>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="122"/>
-      <c r="S28" s="122"/>
-      <c r="T28" s="122"/>
-      <c r="U28" s="122"/>
-      <c r="V28" s="122"/>
-      <c r="W28" s="123"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="124"/>
+      <c r="T28" s="124"/>
+      <c r="U28" s="124"/>
+      <c r="V28" s="124"/>
+      <c r="W28" s="125"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -10040,26 +10040,26 @@
       </c>
     </row>
     <row r="53" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="124" t="s">
+      <c r="C53" s="126" t="s">
         <v>374</v>
       </c>
-      <c r="D53" s="125"/>
-      <c r="E53" s="126"/>
-      <c r="F53" s="126"/>
-      <c r="G53" s="127"/>
-      <c r="I53" s="128" t="s">
+      <c r="D53" s="127"/>
+      <c r="E53" s="128"/>
+      <c r="F53" s="128"/>
+      <c r="G53" s="129"/>
+      <c r="I53" s="130" t="s">
         <v>375</v>
       </c>
-      <c r="J53" s="127"/>
+      <c r="J53" s="129"/>
     </row>
     <row r="54" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="113"/>
-      <c r="D54" s="114"/>
-      <c r="E54" s="117" t="s">
+      <c r="C54" s="115"/>
+      <c r="D54" s="116"/>
+      <c r="E54" s="119" t="s">
         <v>282</v>
       </c>
-      <c r="F54" s="117"/>
-      <c r="G54" s="118"/>
+      <c r="F54" s="119"/>
+      <c r="G54" s="120"/>
       <c r="I54" s="78" t="s">
         <v>384</v>
       </c>
@@ -10068,8 +10068,8 @@
       </c>
     </row>
     <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="115"/>
-      <c r="D55" s="116"/>
+      <c r="C55" s="117"/>
+      <c r="D55" s="118"/>
       <c r="E55" s="89" t="s">
         <v>381</v>
       </c>
@@ -10087,7 +10087,7 @@
       </c>
     </row>
     <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="119" t="s">
+      <c r="C56" s="121" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="78" t="s">
@@ -10110,7 +10110,7 @@
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C57" s="119"/>
+      <c r="C57" s="121"/>
       <c r="D57" s="78" t="s">
         <v>382</v>
       </c>
@@ -10125,7 +10125,7 @@
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C58" s="120"/>
+      <c r="C58" s="122"/>
       <c r="D58" s="88" t="s">
         <v>376</v>
       </c>
@@ -10998,16 +10998,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="131" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="131"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="133"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -11140,16 +11140,16 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="130"/>
-      <c r="C13" s="130"/>
-      <c r="D13" s="130"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="131"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="132"/>
+      <c r="H13" s="133"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
@@ -11206,16 +11206,16 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="129" t="s">
+      <c r="A18" s="131" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="130"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="131"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="132"/>
+      <c r="H18" s="133"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
@@ -11270,16 +11270,16 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="131" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="130"/>
-      <c r="C23" s="130"/>
-      <c r="D23" s="130"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="131"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="133"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
@@ -11336,16 +11336,16 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="129" t="s">
+      <c r="A28" s="131" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="131"/>
+      <c r="B28" s="132"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="132"/>
+      <c r="G28" s="132"/>
+      <c r="H28" s="133"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">

</xml_diff>

<commit_message>
fleshed out fundamentals, mainly the theory chapter up until orchestration
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -2920,7 +2920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -4587,8 +4587,8 @@
   </sheetPr>
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
propagated vector merge through to thesis chapters
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -2492,6 +2492,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2539,15 +2548,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2923,8 +2923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,7 +3177,7 @@
   </sheetPr>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -5352,16 +5352,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="115" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="117"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -5494,16 +5494,16 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="131" t="s">
+      <c r="A13" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="132"/>
-      <c r="H13" s="133"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="117"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
@@ -5560,16 +5560,16 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="131" t="s">
+      <c r="A18" s="115" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="132"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="132"/>
-      <c r="H18" s="133"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="117"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
@@ -5624,16 +5624,16 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="131" t="s">
+      <c r="A23" s="115" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="132"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="132"/>
-      <c r="H23" s="133"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="117"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
@@ -5690,16 +5690,16 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="131" t="s">
+      <c r="A28" s="115" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="132"/>
-      <c r="C28" s="132"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="132"/>
-      <c r="F28" s="132"/>
-      <c r="G28" s="132"/>
-      <c r="H28" s="133"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="117"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
@@ -8092,30 +8092,30 @@
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="126" t="s">
         <v>279</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="123" t="s">
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="128"/>
+      <c r="N4" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="125"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="127"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="127"/>
+      <c r="W4" s="128"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -9565,30 +9565,30 @@
       <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="123" t="s">
+      <c r="D28" s="126" t="s">
         <v>279</v>
       </c>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="124"/>
-      <c r="I28" s="124"/>
-      <c r="J28" s="124"/>
-      <c r="K28" s="124"/>
-      <c r="L28" s="124"/>
-      <c r="M28" s="125"/>
-      <c r="N28" s="123" t="s">
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="127"/>
+      <c r="J28" s="127"/>
+      <c r="K28" s="127"/>
+      <c r="L28" s="127"/>
+      <c r="M28" s="128"/>
+      <c r="N28" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="O28" s="124"/>
-      <c r="P28" s="124"/>
-      <c r="Q28" s="124"/>
-      <c r="R28" s="124"/>
-      <c r="S28" s="124"/>
-      <c r="T28" s="124"/>
-      <c r="U28" s="124"/>
-      <c r="V28" s="124"/>
-      <c r="W28" s="125"/>
+      <c r="O28" s="127"/>
+      <c r="P28" s="127"/>
+      <c r="Q28" s="127"/>
+      <c r="R28" s="127"/>
+      <c r="S28" s="127"/>
+      <c r="T28" s="127"/>
+      <c r="U28" s="127"/>
+      <c r="V28" s="127"/>
+      <c r="W28" s="128"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -11031,26 +11031,26 @@
       </c>
     </row>
     <row r="53" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="126" t="s">
+      <c r="C53" s="129" t="s">
         <v>371</v>
       </c>
-      <c r="D53" s="127"/>
-      <c r="E53" s="128"/>
-      <c r="F53" s="128"/>
-      <c r="G53" s="129"/>
-      <c r="I53" s="130" t="s">
+      <c r="D53" s="130"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="132"/>
+      <c r="I53" s="133" t="s">
         <v>372</v>
       </c>
-      <c r="J53" s="129"/>
+      <c r="J53" s="132"/>
     </row>
     <row r="54" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="115"/>
-      <c r="D54" s="116"/>
-      <c r="E54" s="119" t="s">
+      <c r="C54" s="118"/>
+      <c r="D54" s="119"/>
+      <c r="E54" s="122" t="s">
         <v>279</v>
       </c>
-      <c r="F54" s="119"/>
-      <c r="G54" s="120"/>
+      <c r="F54" s="122"/>
+      <c r="G54" s="123"/>
       <c r="I54" s="78" t="s">
         <v>381</v>
       </c>
@@ -11059,8 +11059,8 @@
       </c>
     </row>
     <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="117"/>
-      <c r="D55" s="118"/>
+      <c r="C55" s="120"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="89" t="s">
         <v>378</v>
       </c>
@@ -11078,7 +11078,7 @@
       </c>
     </row>
     <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="121" t="s">
+      <c r="C56" s="124" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="78" t="s">
@@ -11101,7 +11101,7 @@
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C57" s="121"/>
+      <c r="C57" s="124"/>
       <c r="D57" s="78" t="s">
         <v>379</v>
       </c>
@@ -11116,7 +11116,7 @@
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C58" s="122"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="88" t="s">
         <v>373</v>
       </c>

</xml_diff>

<commit_message>
slight rewordings on multiple chapters, scetched out conclusion, versioning info on ocp + aks
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="468">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -1553,6 +1553,21 @@
   </si>
   <si>
     <t>The provided resources may be misconfigured or misused for financial gains (mining cryptocurrencies)</t>
+  </si>
+  <si>
+    <t>AKS only</t>
+  </si>
+  <si>
+    <t>Results only</t>
+  </si>
+  <si>
+    <t>Risk OCP</t>
+  </si>
+  <si>
+    <t>Risk AKS</t>
+  </si>
+  <si>
+    <t>Vector ID</t>
   </si>
 </sst>
 </file>
@@ -2222,7 +2237,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2490,6 +2505,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2923,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,17 +3196,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -3221,7 +3242,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>105</v>
+        <v>467</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>9</v>
@@ -4272,56 +4293,858 @@
       <c r="L23" s="37"/>
       <c r="M23" s="37"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="43"/>
+    <row r="24" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B24" s="1" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="K25"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>467</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="47" t="s">
+        <v>37</v>
+      </c>
       <c r="K26"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="C27" s="41">
+        <v>4</v>
+      </c>
+      <c r="D27" s="54">
+        <v>3</v>
+      </c>
+      <c r="E27" s="41">
+        <v>3</v>
+      </c>
+      <c r="F27" s="41">
+        <v>2</v>
+      </c>
+      <c r="G27" s="50">
+        <f>ROUND(((D27+C27+E27+F27)/4), 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="48">
+        <f>MIN(10, ROUND(G27*H27, 0))</f>
+        <v>3</v>
+      </c>
       <c r="K27"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="C28" s="41">
+        <v>4</v>
+      </c>
+      <c r="D28" s="41">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="23">
+        <f>ROUND(((D28+C28+E28+F28)/4), 2)</f>
+        <v>3.25</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2</v>
+      </c>
+      <c r="I28" s="48">
+        <f t="shared" ref="I28:I43" si="5">MIN(10, ROUND(G28*H28, 0))</f>
+        <v>7</v>
+      </c>
       <c r="K28"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C29" s="41">
+        <v>4</v>
+      </c>
+      <c r="D29" s="41">
+        <v>1</v>
+      </c>
+      <c r="E29" s="41">
+        <v>3</v>
+      </c>
+      <c r="F29" s="41">
+        <v>2</v>
+      </c>
+      <c r="G29" s="23">
+        <f t="shared" ref="G29:G42" si="6">ROUND(((D29+C29+E29+F29)/4), 2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="H29" s="4">
+        <v>3</v>
+      </c>
+      <c r="I29" s="48">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="K29"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C30" s="41">
+        <v>4</v>
+      </c>
+      <c r="D30" s="41">
+        <v>1</v>
+      </c>
+      <c r="E30" s="41">
+        <v>3</v>
+      </c>
+      <c r="F30" s="41">
+        <v>0</v>
+      </c>
+      <c r="G30" s="23">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H30" s="4">
+        <v>3</v>
+      </c>
+      <c r="I30" s="48">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
       <c r="K30"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C31" s="41">
+        <v>4</v>
+      </c>
+      <c r="D31" s="41">
+        <v>4</v>
+      </c>
+      <c r="E31" s="41">
+        <v>3</v>
+      </c>
+      <c r="F31" s="41">
+        <v>2</v>
+      </c>
+      <c r="G31" s="23">
+        <f t="shared" si="6"/>
+        <v>3.25</v>
+      </c>
+      <c r="H31" s="38">
+        <v>2</v>
+      </c>
+      <c r="I31" s="48">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="K31"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C32" s="41">
+        <v>4</v>
+      </c>
+      <c r="D32" s="41">
+        <v>4</v>
+      </c>
+      <c r="E32" s="41">
+        <v>3</v>
+      </c>
+      <c r="F32" s="41">
+        <v>2</v>
+      </c>
+      <c r="G32" s="23">
+        <f t="shared" si="6"/>
+        <v>3.25</v>
+      </c>
+      <c r="H32" s="38">
+        <v>3</v>
+      </c>
+      <c r="I32" s="48">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="K32"/>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>442</v>
+      </c>
+      <c r="C33" s="10">
+        <v>2</v>
+      </c>
+      <c r="D33" s="38">
+        <v>2</v>
+      </c>
+      <c r="E33" s="41">
+        <v>3</v>
+      </c>
+      <c r="F33" s="41">
+        <v>2</v>
+      </c>
+      <c r="G33" s="23">
+        <f t="shared" si="6"/>
+        <v>2.25</v>
+      </c>
+      <c r="H33" s="38">
+        <v>3</v>
+      </c>
+      <c r="I33" s="48">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="K33"/>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="51" t="s">
+        <v>430</v>
+      </c>
+      <c r="C34" s="23">
+        <v>2</v>
+      </c>
+      <c r="D34" s="41">
+        <v>2</v>
+      </c>
+      <c r="E34" s="38">
+        <v>3</v>
+      </c>
+      <c r="F34" s="38">
+        <v>2</v>
+      </c>
+      <c r="G34" s="23">
+        <f t="shared" si="6"/>
+        <v>2.25</v>
+      </c>
+      <c r="H34" s="38">
+        <v>3</v>
+      </c>
+      <c r="I34" s="48">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="K34"/>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>431</v>
+      </c>
+      <c r="C35" s="10">
+        <v>1</v>
+      </c>
+      <c r="D35" s="41">
+        <v>1</v>
+      </c>
+      <c r="E35" s="41">
+        <v>2</v>
+      </c>
+      <c r="F35" s="41">
+        <v>2</v>
+      </c>
+      <c r="G35" s="23">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="H35" s="38">
+        <v>2</v>
+      </c>
+      <c r="I35" s="48">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
       <c r="K35"/>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>432</v>
+      </c>
+      <c r="C36" s="38">
+        <v>2</v>
+      </c>
+      <c r="D36" s="41">
+        <v>2</v>
+      </c>
+      <c r="E36" s="38">
+        <v>3</v>
+      </c>
+      <c r="F36" s="38">
+        <v>2</v>
+      </c>
+      <c r="G36" s="23">
+        <f t="shared" si="6"/>
+        <v>2.25</v>
+      </c>
+      <c r="H36" s="38">
+        <v>2</v>
+      </c>
+      <c r="I36" s="48">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="K36"/>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="C37" s="38">
+        <v>3</v>
+      </c>
+      <c r="D37" s="41">
+        <v>2</v>
+      </c>
+      <c r="E37" s="38">
+        <v>3</v>
+      </c>
+      <c r="F37" s="38">
+        <v>2</v>
+      </c>
+      <c r="G37" s="23">
+        <f t="shared" si="6"/>
+        <v>2.5</v>
+      </c>
+      <c r="H37" s="38">
+        <v>2</v>
+      </c>
+      <c r="I37" s="48">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="K37"/>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="C38" s="38">
+        <v>3</v>
+      </c>
+      <c r="D38" s="41">
+        <v>2</v>
+      </c>
+      <c r="E38" s="38">
+        <v>3</v>
+      </c>
+      <c r="F38" s="38">
+        <v>2</v>
+      </c>
+      <c r="G38" s="23">
+        <f t="shared" si="6"/>
+        <v>2.5</v>
+      </c>
+      <c r="H38" s="38">
+        <v>3</v>
+      </c>
+      <c r="I38" s="48">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="K38"/>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>436</v>
+      </c>
+      <c r="C39" s="38">
+        <v>4</v>
+      </c>
+      <c r="D39" s="41">
+        <v>2</v>
+      </c>
+      <c r="E39" s="38">
+        <v>3</v>
+      </c>
+      <c r="F39" s="38">
+        <v>2</v>
+      </c>
+      <c r="G39" s="23">
+        <f t="shared" si="6"/>
+        <v>2.75</v>
+      </c>
+      <c r="H39" s="38">
+        <v>2</v>
+      </c>
+      <c r="I39" s="48">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
       <c r="K39"/>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="51" t="s">
+        <v>437</v>
+      </c>
+      <c r="C40" s="38">
+        <v>4</v>
+      </c>
+      <c r="D40" s="41">
+        <v>1</v>
+      </c>
+      <c r="E40" s="38">
+        <v>1</v>
+      </c>
+      <c r="F40" s="38">
+        <v>2</v>
+      </c>
+      <c r="G40" s="23">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H40" s="38">
+        <v>3</v>
+      </c>
+      <c r="I40" s="48">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
       <c r="K40"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="38">
+        <v>4</v>
+      </c>
+      <c r="D41" s="41">
+        <v>4</v>
+      </c>
+      <c r="E41" s="38">
+        <v>2</v>
+      </c>
+      <c r="F41" s="38">
+        <v>2</v>
+      </c>
+      <c r="G41" s="23">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="H41" s="38">
+        <v>2</v>
+      </c>
+      <c r="I41" s="48">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="38">
+        <v>4</v>
+      </c>
+      <c r="D42" s="41">
+        <v>4</v>
+      </c>
+      <c r="E42" s="38">
+        <v>2</v>
+      </c>
+      <c r="F42" s="38">
+        <v>2</v>
+      </c>
+      <c r="G42" s="23">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="H42" s="38">
+        <v>3</v>
+      </c>
+      <c r="I42" s="48">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="53" t="s">
+        <v>438</v>
+      </c>
+      <c r="C43" s="40">
+        <v>4</v>
+      </c>
+      <c r="D43" s="6">
+        <v>4</v>
+      </c>
+      <c r="E43" s="40">
+        <v>3</v>
+      </c>
+      <c r="F43" s="40">
+        <v>2</v>
+      </c>
+      <c r="G43" s="39">
+        <f>ROUND(((D43+C43+E43+F43)/4), 2)</f>
+        <v>3.25</v>
+      </c>
+      <c r="H43" s="40">
+        <v>3</v>
+      </c>
+      <c r="I43" s="49">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="K43"/>
+    </row>
+    <row r="46" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B46" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="32"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>467</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>465</v>
+      </c>
+      <c r="D48" s="47" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="C49" s="48">
+        <v>3</v>
+      </c>
+      <c r="D49" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="C50" s="48">
+        <v>6</v>
+      </c>
+      <c r="D50" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C51" s="48">
+        <v>7</v>
+      </c>
+      <c r="D51" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C52" s="48">
+        <v>5</v>
+      </c>
+      <c r="D52" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C53" s="48">
+        <v>7</v>
+      </c>
+      <c r="D53" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C54" s="48">
+        <v>10</v>
+      </c>
+      <c r="D54" s="48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
+        <v>442</v>
+      </c>
+      <c r="C55" s="48">
+        <v>7</v>
+      </c>
+      <c r="D55" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="51" t="s">
+        <v>430</v>
+      </c>
+      <c r="C56" s="48">
+        <v>5</v>
+      </c>
+      <c r="D56" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="51" t="s">
+        <v>431</v>
+      </c>
+      <c r="C57" s="48">
+        <v>3</v>
+      </c>
+      <c r="D57" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="52" t="s">
+        <v>432</v>
+      </c>
+      <c r="C58" s="48">
+        <v>5</v>
+      </c>
+      <c r="D58" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="51" t="s">
+        <v>459</v>
+      </c>
+      <c r="C59" s="48">
+        <v>8</v>
+      </c>
+      <c r="D59" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="51" t="s">
+        <v>460</v>
+      </c>
+      <c r="C60" s="48">
+        <v>5</v>
+      </c>
+      <c r="D60" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="51" t="s">
+        <v>436</v>
+      </c>
+      <c r="C61" s="48">
+        <v>5</v>
+      </c>
+      <c r="D61" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="51" t="s">
+        <v>437</v>
+      </c>
+      <c r="C62" s="48">
+        <v>6</v>
+      </c>
+      <c r="D62" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" s="48">
+        <v>6</v>
+      </c>
+      <c r="D63" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="48">
+        <v>9</v>
+      </c>
+      <c r="D64" s="48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="53" t="s">
+        <v>438</v>
+      </c>
+      <c r="C65" s="49">
+        <v>10</v>
+      </c>
+      <c r="D65" s="49">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4330,7 +5153,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="47" id="{CE3E1A35-17C1-4254-BDAA-DB91301DFA4F}">
+          <x14:cfRule type="iconSet" priority="52" id="{CE3E1A35-17C1-4254-BDAA-DB91301DFA4F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4349,7 +5172,7 @@
           <xm:sqref>P4:P20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="49" id="{709B235F-63E3-4660-B256-0309169812CD}">
+          <x14:cfRule type="iconSet" priority="54" id="{709B235F-63E3-4660-B256-0309169812CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4366,6 +5189,63 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I4:I20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{2E41C5A3-54AC-4DDF-AD70-4007B999D186}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I27:I43</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{0BDE4070-C01A-41C0-AE11-96AE556C45B4}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>C49:C65</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{4B991457-1835-4C57-8A66-EB9771A32F32}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>7</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D49:D65</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4625,8 +5505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5352,16 +6232,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="117"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="119"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
@@ -5494,16 +6374,16 @@
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="115" t="s">
+      <c r="A13" s="117" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="117"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="119"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
@@ -5560,16 +6440,16 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="115" t="s">
+      <c r="A18" s="117" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="117"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="119"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
@@ -5624,16 +6504,16 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="115" t="s">
+      <c r="A23" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="117"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="119"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
@@ -5690,16 +6570,16 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="116"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="116"/>
-      <c r="H28" s="117"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="119"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
@@ -8092,30 +8972,30 @@
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="D4" s="128" t="s">
         <v>279</v>
       </c>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="126" t="s">
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="127"/>
-      <c r="P4" s="127"/>
-      <c r="Q4" s="127"/>
-      <c r="R4" s="127"/>
-      <c r="S4" s="127"/>
-      <c r="T4" s="127"/>
-      <c r="U4" s="127"/>
-      <c r="V4" s="127"/>
-      <c r="W4" s="128"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="129"/>
+      <c r="Q4" s="129"/>
+      <c r="R4" s="129"/>
+      <c r="S4" s="129"/>
+      <c r="T4" s="129"/>
+      <c r="U4" s="129"/>
+      <c r="V4" s="129"/>
+      <c r="W4" s="130"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -9565,30 +10445,30 @@
       <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="126" t="s">
+      <c r="D28" s="128" t="s">
         <v>279</v>
       </c>
-      <c r="E28" s="127"/>
-      <c r="F28" s="127"/>
-      <c r="G28" s="127"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="127"/>
-      <c r="J28" s="127"/>
-      <c r="K28" s="127"/>
-      <c r="L28" s="127"/>
-      <c r="M28" s="128"/>
-      <c r="N28" s="126" t="s">
+      <c r="E28" s="129"/>
+      <c r="F28" s="129"/>
+      <c r="G28" s="129"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
+      <c r="J28" s="129"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="129"/>
+      <c r="M28" s="130"/>
+      <c r="N28" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="O28" s="127"/>
-      <c r="P28" s="127"/>
-      <c r="Q28" s="127"/>
-      <c r="R28" s="127"/>
-      <c r="S28" s="127"/>
-      <c r="T28" s="127"/>
-      <c r="U28" s="127"/>
-      <c r="V28" s="127"/>
-      <c r="W28" s="128"/>
+      <c r="O28" s="129"/>
+      <c r="P28" s="129"/>
+      <c r="Q28" s="129"/>
+      <c r="R28" s="129"/>
+      <c r="S28" s="129"/>
+      <c r="T28" s="129"/>
+      <c r="U28" s="129"/>
+      <c r="V28" s="129"/>
+      <c r="W28" s="130"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -11031,26 +11911,26 @@
       </c>
     </row>
     <row r="53" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="129" t="s">
+      <c r="C53" s="131" t="s">
         <v>371</v>
       </c>
-      <c r="D53" s="130"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="131"/>
-      <c r="G53" s="132"/>
-      <c r="I53" s="133" t="s">
+      <c r="D53" s="132"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="133"/>
+      <c r="G53" s="134"/>
+      <c r="I53" s="135" t="s">
         <v>372</v>
       </c>
-      <c r="J53" s="132"/>
+      <c r="J53" s="134"/>
     </row>
     <row r="54" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="118"/>
-      <c r="D54" s="119"/>
-      <c r="E54" s="122" t="s">
+      <c r="C54" s="120"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="124" t="s">
         <v>279</v>
       </c>
-      <c r="F54" s="122"/>
-      <c r="G54" s="123"/>
+      <c r="F54" s="124"/>
+      <c r="G54" s="125"/>
       <c r="I54" s="78" t="s">
         <v>381</v>
       </c>
@@ -11059,8 +11939,8 @@
       </c>
     </row>
     <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="120"/>
-      <c r="D55" s="121"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="123"/>
       <c r="E55" s="89" t="s">
         <v>378</v>
       </c>
@@ -11078,7 +11958,7 @@
       </c>
     </row>
     <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="124" t="s">
+      <c r="C56" s="126" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="78" t="s">
@@ -11101,7 +11981,7 @@
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C57" s="124"/>
+      <c r="C57" s="126"/>
       <c r="D57" s="78" t="s">
         <v>379</v>
       </c>
@@ -11116,7 +11996,7 @@
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C58" s="125"/>
+      <c r="C58" s="127"/>
       <c r="D58" s="88" t="s">
         <v>373</v>
       </c>

</xml_diff>

<commit_message>
added pictures of demos, dumped raw commands and outputs into demo section
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -964,9 +964,6 @@
     <t>cluster isolation</t>
   </si>
   <si>
-    <t>follow additional tips by supplied</t>
-  </si>
-  <si>
     <t>same as V02</t>
   </si>
   <si>
@@ -1568,6 +1565,9 @@
   </si>
   <si>
     <t>Vector ID</t>
+  </si>
+  <si>
+    <t>follow additional tips by supplier</t>
   </si>
 </sst>
 </file>
@@ -2985,13 +2985,13 @@
         <v>68</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>108</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2999,11 +2999,11 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3011,11 +3011,11 @@
         <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3023,11 +3023,11 @@
         <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,7 +3035,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -3047,7 +3047,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
@@ -3059,7 +3059,7 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
@@ -3071,7 +3071,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
@@ -3083,11 +3083,11 @@
         <v>76</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
@@ -3107,11 +3107,11 @@
         <v>78</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3119,11 +3119,11 @@
         <v>79</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
@@ -3143,7 +3143,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3179,7 +3179,7 @@
         <v>84</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="35" t="s">
@@ -3198,7 +3198,7 @@
   </sheetPr>
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
@@ -3225,7 +3225,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>9</v>
@@ -3298,7 +3298,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C4" s="110">
         <v>3</v>
@@ -3356,7 +3356,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -3414,7 +3414,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C6" s="10">
         <v>3</v>
@@ -3472,7 +3472,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C7" s="10">
         <v>3</v>
@@ -3530,7 +3530,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C8" s="10">
         <v>4</v>
@@ -3588,7 +3588,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C9" s="10">
         <v>4</v>
@@ -3646,7 +3646,7 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C10" s="10">
         <v>2</v>
@@ -3704,7 +3704,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C11" s="23">
         <v>2</v>
@@ -3762,7 +3762,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C12" s="10">
         <v>1</v>
@@ -3820,7 +3820,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C13" s="23">
         <v>2</v>
@@ -3878,7 +3878,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C14" s="23">
         <v>3</v>
@@ -3936,7 +3936,7 @@
         <v>79</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C15" s="23">
         <v>3</v>
@@ -3994,7 +3994,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C16" s="23">
         <v>3</v>
@@ -4052,7 +4052,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C17" s="23">
         <v>3</v>
@@ -4226,7 +4226,7 @@
         <v>84</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C20" s="39">
         <v>4</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="24" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -4310,7 +4310,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B26" s="33" t="s">
         <v>9</v>
@@ -4343,7 +4343,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C27" s="41">
         <v>4</v>
@@ -4375,7 +4375,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C28" s="41">
         <v>4</v>
@@ -4407,7 +4407,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C29" s="41">
         <v>4</v>
@@ -4439,7 +4439,7 @@
         <v>71</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C30" s="41">
         <v>4</v>
@@ -4471,7 +4471,7 @@
         <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C31" s="41">
         <v>4</v>
@@ -4503,7 +4503,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C32" s="41">
         <v>4</v>
@@ -4535,7 +4535,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
@@ -4567,7 +4567,7 @@
         <v>75</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C34" s="23">
         <v>2</v>
@@ -4599,7 +4599,7 @@
         <v>76</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C35" s="10">
         <v>1</v>
@@ -4631,7 +4631,7 @@
         <v>77</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C36" s="38">
         <v>2</v>
@@ -4663,7 +4663,7 @@
         <v>78</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C37" s="38">
         <v>3</v>
@@ -4695,7 +4695,7 @@
         <v>79</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C38" s="38">
         <v>3</v>
@@ -4727,7 +4727,7 @@
         <v>80</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C39" s="38">
         <v>4</v>
@@ -4759,7 +4759,7 @@
         <v>81</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C40" s="38">
         <v>4</v>
@@ -4855,7 +4855,7 @@
         <v>84</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C43" s="40">
         <v>4</v>
@@ -4884,7 +4884,7 @@
     </row>
     <row r="46" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B46" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4896,16 +4896,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B48" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="47" t="s">
+        <v>464</v>
+      </c>
+      <c r="D48" s="47" t="s">
         <v>465</v>
-      </c>
-      <c r="D48" s="47" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4913,7 +4913,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C49" s="48">
         <v>3</v>
@@ -4927,7 +4927,7 @@
         <v>69</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C50" s="48">
         <v>6</v>
@@ -4941,7 +4941,7 @@
         <v>70</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C51" s="48">
         <v>7</v>
@@ -4955,7 +4955,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C52" s="48">
         <v>5</v>
@@ -4969,7 +4969,7 @@
         <v>72</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C53" s="48">
         <v>7</v>
@@ -4983,7 +4983,7 @@
         <v>73</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C54" s="48">
         <v>10</v>
@@ -4997,7 +4997,7 @@
         <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C55" s="48">
         <v>7</v>
@@ -5011,7 +5011,7 @@
         <v>75</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C56" s="48">
         <v>5</v>
@@ -5025,7 +5025,7 @@
         <v>76</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C57" s="48">
         <v>3</v>
@@ -5039,7 +5039,7 @@
         <v>77</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C58" s="48">
         <v>5</v>
@@ -5053,7 +5053,7 @@
         <v>78</v>
       </c>
       <c r="B59" s="51" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C59" s="48">
         <v>8</v>
@@ -5067,7 +5067,7 @@
         <v>79</v>
       </c>
       <c r="B60" s="51" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C60" s="48">
         <v>5</v>
@@ -5081,7 +5081,7 @@
         <v>80</v>
       </c>
       <c r="B61" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C61" s="48">
         <v>5</v>
@@ -5095,7 +5095,7 @@
         <v>81</v>
       </c>
       <c r="B62" s="51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C62" s="48">
         <v>6</v>
@@ -5137,7 +5137,7 @@
         <v>84</v>
       </c>
       <c r="B65" s="53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C65" s="49">
         <v>10</v>
@@ -5429,48 +5429,48 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="34"/>
       <c r="E11" s="114" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
       <c r="E12" s="113" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
       <c r="E13" s="113" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
       <c r="E14" s="113" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="113" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="113" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D17" s="113" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" s="113" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -5505,8 +5505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,7 +5730,7 @@
         <v>228</v>
       </c>
       <c r="C42" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -5846,7 +5846,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -6109,7 +6109,7 @@
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="61"/>
       <c r="B111" t="s">
-        <v>266</v>
+        <v>467</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -6120,7 +6120,7 @@
         <v>68</v>
       </c>
       <c r="B113" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -6131,10 +6131,10 @@
         <v>78</v>
       </c>
       <c r="B115" t="s">
+        <v>267</v>
+      </c>
+      <c r="C115" t="s">
         <v>268</v>
-      </c>
-      <c r="C115" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -6145,7 +6145,7 @@
         <v>80</v>
       </c>
       <c r="B117" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -6707,7 +6707,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6804,7 +6804,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C4" s="42">
         <v>3</v>
@@ -6865,7 +6865,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -6926,7 +6926,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C6" s="10">
         <v>3</v>
@@ -6987,7 +6987,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C7" s="10">
         <v>3</v>
@@ -7048,7 +7048,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C8" s="10">
         <v>3</v>
@@ -7109,7 +7109,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C9" s="10">
         <v>3</v>
@@ -7170,7 +7170,7 @@
         <v>74</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C10" s="10">
         <v>4</v>
@@ -7228,7 +7228,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C11" s="10">
         <v>4</v>
@@ -7289,7 +7289,7 @@
         <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C12" s="10">
         <v>2</v>
@@ -7347,7 +7347,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C13" s="23">
         <v>2</v>
@@ -7408,7 +7408,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C14" s="10">
         <v>1</v>
@@ -7466,7 +7466,7 @@
         <v>79</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C15" s="23">
         <v>2</v>
@@ -7524,7 +7524,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C16" s="23">
         <v>2</v>
@@ -7582,7 +7582,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C17" s="23">
         <v>2</v>
@@ -7643,7 +7643,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C18" s="23">
         <v>2</v>
@@ -7701,7 +7701,7 @@
         <v>83</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C19" s="23">
         <v>1</v>
@@ -7759,7 +7759,7 @@
         <v>84</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C20" s="23">
         <v>1</v>
@@ -7939,7 +7939,7 @@
         <v>87</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C23" s="39">
         <v>4</v>
@@ -8973,7 +8973,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="128" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4" s="129"/>
       <c r="F4" s="129"/>
@@ -9005,67 +9005,67 @@
         <v>9</v>
       </c>
       <c r="C5" s="94" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D5" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" s="90" t="s">
         <v>271</v>
       </c>
-      <c r="E5" s="90" t="s">
+      <c r="F5" s="90" t="s">
         <v>272</v>
       </c>
-      <c r="F5" s="90" t="s">
+      <c r="G5" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="H5" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="H5" s="91" t="s">
+      <c r="I5" s="91" t="s">
         <v>275</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="J5" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="J5" s="91" t="s">
+      <c r="K5" s="91" t="s">
         <v>277</v>
       </c>
-      <c r="K5" s="91" t="s">
-        <v>278</v>
-      </c>
       <c r="L5" s="96" t="s">
+        <v>279</v>
+      </c>
+      <c r="M5" s="97" t="s">
+        <v>279</v>
+      </c>
+      <c r="N5" s="93" t="s">
+        <v>281</v>
+      </c>
+      <c r="O5" s="90" t="s">
+        <v>282</v>
+      </c>
+      <c r="P5" s="90" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q5" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="R5" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="S5" s="91" t="s">
+        <v>286</v>
+      </c>
+      <c r="T5" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="U5" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="V5" s="96" t="s">
         <v>280</v>
       </c>
-      <c r="M5" s="97" t="s">
+      <c r="W5" s="97" t="s">
         <v>280</v>
-      </c>
-      <c r="N5" s="93" t="s">
-        <v>282</v>
-      </c>
-      <c r="O5" s="90" t="s">
-        <v>283</v>
-      </c>
-      <c r="P5" s="90" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q5" s="91" t="s">
-        <v>285</v>
-      </c>
-      <c r="R5" s="91" t="s">
-        <v>286</v>
-      </c>
-      <c r="S5" s="91" t="s">
-        <v>287</v>
-      </c>
-      <c r="T5" s="91" t="s">
-        <v>288</v>
-      </c>
-      <c r="U5" s="91" t="s">
-        <v>289</v>
-      </c>
-      <c r="V5" s="96" t="s">
-        <v>281</v>
-      </c>
-      <c r="W5" s="97" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="23.25" x14ac:dyDescent="0.25">
@@ -9073,35 +9073,35 @@
         <v>68</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C6" s="95" t="str">
         <f>INDEX($E$56:$G$58, MATCH(M6,$E$55:$G$55,0),MATCH(W6,$D$56:$D$58,0))</f>
         <v>Medium</v>
       </c>
       <c r="D6" s="106" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E6" s="107" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F6" s="107" t="s">
+        <v>389</v>
+      </c>
+      <c r="G6" s="107" t="s">
         <v>390</v>
       </c>
-      <c r="G6" s="107" t="s">
-        <v>391</v>
-      </c>
       <c r="H6" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I6" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J6" s="107" t="s">
+        <v>363</v>
+      </c>
+      <c r="K6" s="108" t="s">
         <v>364</v>
-      </c>
-      <c r="K6" s="108" t="s">
-        <v>365</v>
       </c>
       <c r="L6" s="100">
         <f t="shared" ref="L6:L25" si="0">(VALUE(LEFT(D6,1))+VALUE(LEFT(E6,1))+VALUE(LEFT(F6,1))+VALUE(LEFT(G6,1))+VALUE(LEFT(H6,1))+VALUE(LEFT(I6,1))+VALUE(LEFT(J6,1))+VALUE(LEFT(K6,1)))/8</f>
@@ -9112,16 +9112,16 @@
         <v>HIGH</v>
       </c>
       <c r="N6" s="106" t="s">
+        <v>365</v>
+      </c>
+      <c r="O6" s="107" t="s">
         <v>366</v>
       </c>
-      <c r="O6" s="107" t="s">
+      <c r="P6" s="107" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q6" s="107" t="s">
         <v>367</v>
-      </c>
-      <c r="P6" s="107" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q6" s="107" t="s">
-        <v>368</v>
       </c>
       <c r="R6" s="92"/>
       <c r="S6" s="92"/>
@@ -9141,35 +9141,35 @@
         <v>69</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C7" s="95" t="str">
         <f t="shared" ref="C7:C25" si="4">INDEX($E$56:$G$58, MATCH(M7,$E$55:$G$55,0),MATCH(W7,$D$56:$D$58,0))</f>
         <v>High</v>
       </c>
       <c r="D7" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E7" s="107" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F7" s="107" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G7" s="107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H7" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I7" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J7" s="107" t="s">
+        <v>363</v>
+      </c>
+      <c r="K7" s="108" t="s">
         <v>364</v>
-      </c>
-      <c r="K7" s="108" t="s">
-        <v>365</v>
       </c>
       <c r="L7" s="100">
         <f t="shared" si="0"/>
@@ -9180,16 +9180,16 @@
         <v>HIGH</v>
       </c>
       <c r="N7" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O7" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P7" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q7" s="107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R7" s="92"/>
       <c r="S7" s="92"/>
@@ -9209,35 +9209,35 @@
         <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C8" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D8" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E8" s="107" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F8" s="107" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G8" s="107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H8" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I8" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J8" s="107" t="s">
+        <v>363</v>
+      </c>
+      <c r="K8" s="108" t="s">
         <v>364</v>
-      </c>
-      <c r="K8" s="108" t="s">
-        <v>365</v>
       </c>
       <c r="L8" s="100">
         <f t="shared" si="0"/>
@@ -9248,16 +9248,16 @@
         <v>HIGH</v>
       </c>
       <c r="N8" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O8" s="107" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P8" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q8" s="107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R8" s="92"/>
       <c r="S8" s="92"/>
@@ -9277,35 +9277,35 @@
         <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C9" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D9" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E9" s="107" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F9" s="107" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G9" s="107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H9" s="107" t="s">
+        <v>392</v>
+      </c>
+      <c r="I9" s="107" t="s">
         <v>393</v>
       </c>
-      <c r="I9" s="107" t="s">
+      <c r="J9" s="107" t="s">
         <v>394</v>
       </c>
-      <c r="J9" s="107" t="s">
-        <v>395</v>
-      </c>
       <c r="K9" s="108" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L9" s="100">
         <f t="shared" ref="L9" si="5">(VALUE(LEFT(D9,1))+VALUE(LEFT(E9,1))+VALUE(LEFT(F9,1))+VALUE(LEFT(G9,1))+VALUE(LEFT(H9,1))+VALUE(LEFT(I9,1))+VALUE(LEFT(J9,1))+VALUE(LEFT(K9,1)))/8</f>
@@ -9316,16 +9316,16 @@
         <v>HIGH</v>
       </c>
       <c r="N9" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O9" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P9" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q9" s="107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R9" s="92"/>
       <c r="S9" s="92"/>
@@ -9345,35 +9345,35 @@
         <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C10" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D10" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E10" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F10" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G10" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H10" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I10" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I10" s="102" t="s">
+      <c r="J10" s="102" t="s">
         <v>394</v>
       </c>
-      <c r="J10" s="102" t="s">
-        <v>395</v>
-      </c>
       <c r="K10" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L10" s="104">
         <f t="shared" si="0"/>
@@ -9384,16 +9384,16 @@
         <v>HIGH</v>
       </c>
       <c r="N10" s="101" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O10" s="102" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P10" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q10" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R10" s="92"/>
       <c r="S10" s="92"/>
@@ -9413,35 +9413,35 @@
         <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C11" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D11" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E11" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F11" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G11" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H11" s="102" t="s">
+        <v>395</v>
+      </c>
+      <c r="I11" s="102" t="s">
         <v>396</v>
       </c>
-      <c r="I11" s="102" t="s">
-        <v>397</v>
-      </c>
       <c r="J11" s="102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K11" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L11" s="104">
         <f t="shared" si="0"/>
@@ -9452,16 +9452,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N11" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O11" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P11" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q11" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R11" s="92"/>
       <c r="S11" s="92"/>
@@ -9481,35 +9481,35 @@
         <v>74</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C12" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D12" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E12" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F12" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G12" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H12" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I12" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I12" s="102" t="s">
-        <v>394</v>
-      </c>
       <c r="J12" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K12" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K12" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L12" s="104">
         <f t="shared" si="0"/>
@@ -9520,16 +9520,16 @@
         <v>HIGH</v>
       </c>
       <c r="N12" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O12" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P12" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q12" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q12" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R12" s="92"/>
       <c r="S12" s="92"/>
@@ -9549,35 +9549,35 @@
         <v>75</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C13" s="95" t="str">
         <f t="shared" si="4"/>
         <v>Critical</v>
       </c>
       <c r="D13" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E13" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F13" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G13" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H13" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I13" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I13" s="102" t="s">
-        <v>394</v>
-      </c>
       <c r="J13" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K13" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K13" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L13" s="104">
         <f t="shared" si="0"/>
@@ -9588,16 +9588,16 @@
         <v>HIGH</v>
       </c>
       <c r="N13" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O13" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P13" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q13" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q13" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R13" s="92"/>
       <c r="S13" s="92"/>
@@ -9617,35 +9617,35 @@
         <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C14" s="95" t="str">
         <f t="shared" si="4"/>
         <v>Medium</v>
       </c>
       <c r="D14" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E14" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F14" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G14" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H14" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I14" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J14" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K14" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L14" s="104">
         <f t="shared" si="0"/>
@@ -9656,16 +9656,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N14" s="101" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O14" s="102" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P14" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q14" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="92"/>
@@ -9685,35 +9685,35 @@
         <v>77</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C15" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D15" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E15" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F15" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G15" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H15" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I15" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J15" s="102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K15" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L15" s="104">
         <f t="shared" si="0"/>
@@ -9724,16 +9724,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N15" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O15" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P15" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q15" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="92"/>
@@ -9753,35 +9753,35 @@
         <v>78</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C16" s="95" t="str">
         <f t="shared" si="4"/>
         <v>Medium</v>
       </c>
       <c r="D16" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E16" s="102" t="s">
+        <v>356</v>
+      </c>
+      <c r="F16" s="102" t="s">
         <v>357</v>
       </c>
-      <c r="F16" s="102" t="s">
-        <v>358</v>
-      </c>
       <c r="G16" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H16" s="102" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I16" s="102" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J16" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K16" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L16" s="104">
         <f t="shared" si="0"/>
@@ -9792,16 +9792,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N16" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O16" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P16" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q16" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R16" s="92"/>
       <c r="S16" s="92"/>
@@ -9821,35 +9821,35 @@
         <v>79</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C17" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D17" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E17" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F17" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G17" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H17" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I17" s="102" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J17" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K17" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K17" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L17" s="104">
         <f t="shared" si="0"/>
@@ -9860,16 +9860,16 @@
         <v>HIGH</v>
       </c>
       <c r="N17" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O17" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P17" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q17" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R17" s="92"/>
       <c r="S17" s="92"/>
@@ -9889,35 +9889,35 @@
         <v>80</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C18" s="95" t="str">
         <f t="shared" si="4"/>
         <v>Medium</v>
       </c>
       <c r="D18" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E18" s="102" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F18" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G18" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H18" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I18" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J18" s="102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K18" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L18" s="104">
         <f t="shared" si="0"/>
@@ -9928,19 +9928,19 @@
         <v>HIGH</v>
       </c>
       <c r="N18" s="101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O18" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P18" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q18" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R18" s="102" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S18" s="92"/>
       <c r="T18" s="92"/>
@@ -9959,35 +9959,35 @@
         <v>81</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C19" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D19" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E19" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F19" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G19" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H19" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I19" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J19" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K19" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L19" s="104">
         <f t="shared" si="0"/>
@@ -9998,16 +9998,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N19" s="101" t="s">
+        <v>401</v>
+      </c>
+      <c r="O19" s="102" t="s">
+        <v>400</v>
+      </c>
+      <c r="P19" s="102" t="s">
         <v>402</v>
       </c>
-      <c r="O19" s="102" t="s">
-        <v>401</v>
-      </c>
-      <c r="P19" s="102" t="s">
-        <v>403</v>
-      </c>
       <c r="Q19" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R19" s="92"/>
       <c r="S19" s="92"/>
@@ -10027,35 +10027,35 @@
         <v>82</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C20" s="95" t="str">
         <f t="shared" si="4"/>
         <v>Medium</v>
       </c>
       <c r="D20" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E20" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F20" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G20" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H20" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I20" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I20" s="102" t="s">
-        <v>394</v>
-      </c>
       <c r="J20" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K20" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K20" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L20" s="104">
         <f t="shared" si="0"/>
@@ -10066,19 +10066,19 @@
         <v>HIGH</v>
       </c>
       <c r="N20" s="101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O20" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P20" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q20" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R20" s="102" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S20" s="92"/>
       <c r="T20" s="92"/>
@@ -10097,35 +10097,35 @@
         <v>83</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C21" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D21" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="E21" s="102" t="s">
+        <v>356</v>
+      </c>
+      <c r="F21" s="102" t="s">
+        <v>358</v>
+      </c>
+      <c r="G21" s="102" t="s">
         <v>387</v>
       </c>
-      <c r="E21" s="102" t="s">
-        <v>357</v>
-      </c>
-      <c r="F21" s="102" t="s">
-        <v>359</v>
-      </c>
-      <c r="G21" s="102" t="s">
-        <v>388</v>
-      </c>
       <c r="H21" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I21" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I21" s="102" t="s">
+      <c r="J21" s="102" t="s">
         <v>394</v>
       </c>
-      <c r="J21" s="102" t="s">
-        <v>395</v>
-      </c>
       <c r="K21" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L21" s="104">
         <f t="shared" si="0"/>
@@ -10136,16 +10136,16 @@
         <v>HIGH</v>
       </c>
       <c r="N21" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O21" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P21" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q21" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R21" s="92"/>
       <c r="S21" s="92"/>
@@ -10165,35 +10165,35 @@
         <v>84</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C22" s="95" t="str">
         <f t="shared" si="4"/>
         <v>High</v>
       </c>
       <c r="D22" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F22" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G22" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H22" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I22" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J22" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K22" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L22" s="104">
         <f t="shared" si="0"/>
@@ -10204,16 +10204,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N22" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O22" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P22" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q22" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R22" s="92"/>
       <c r="S22" s="92"/>
@@ -10240,28 +10240,28 @@
         <v>High</v>
       </c>
       <c r="D23" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E23" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F23" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G23" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H23" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I23" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J23" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K23" s="103" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L23" s="104">
         <f t="shared" si="0"/>
@@ -10272,16 +10272,16 @@
         <v>HIGH</v>
       </c>
       <c r="N23" s="101" t="s">
+        <v>397</v>
+      </c>
+      <c r="O23" s="102" t="s">
         <v>398</v>
       </c>
-      <c r="O23" s="102" t="s">
-        <v>399</v>
-      </c>
       <c r="P23" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q23" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q23" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R23" s="92"/>
       <c r="S23" s="92"/>
@@ -10308,28 +10308,28 @@
         <v>Critical</v>
       </c>
       <c r="D24" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E24" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F24" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G24" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H24" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I24" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J24" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K24" s="103" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L24" s="104">
         <f t="shared" si="0"/>
@@ -10340,16 +10340,16 @@
         <v>HIGH</v>
       </c>
       <c r="N24" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O24" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P24" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q24" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q24" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R24" s="92"/>
       <c r="S24" s="92"/>
@@ -10369,35 +10369,35 @@
         <v>87</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C25" s="95" t="str">
         <f t="shared" si="4"/>
         <v>Critical</v>
       </c>
       <c r="D25" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E25" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F25" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G25" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H25" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I25" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J25" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K25" s="103" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L25" s="104">
         <f t="shared" si="0"/>
@@ -10408,16 +10408,16 @@
         <v>HIGH</v>
       </c>
       <c r="N25" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O25" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P25" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q25" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q25" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R25" s="92"/>
       <c r="S25" s="92"/>
@@ -10446,7 +10446,7 @@
         <v>60</v>
       </c>
       <c r="D28" s="128" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E28" s="129"/>
       <c r="F28" s="129"/>
@@ -10478,67 +10478,67 @@
         <v>9</v>
       </c>
       <c r="C29" s="94" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D29" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="E29" s="90" t="s">
         <v>271</v>
       </c>
-      <c r="E29" s="90" t="s">
+      <c r="F29" s="90" t="s">
         <v>272</v>
       </c>
-      <c r="F29" s="90" t="s">
+      <c r="G29" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="G29" s="91" t="s">
+      <c r="H29" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="H29" s="91" t="s">
+      <c r="I29" s="91" t="s">
         <v>275</v>
       </c>
-      <c r="I29" s="91" t="s">
+      <c r="J29" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="J29" s="91" t="s">
+      <c r="K29" s="91" t="s">
         <v>277</v>
       </c>
-      <c r="K29" s="91" t="s">
-        <v>278</v>
-      </c>
       <c r="L29" s="96" t="s">
+        <v>279</v>
+      </c>
+      <c r="M29" s="97" t="s">
+        <v>279</v>
+      </c>
+      <c r="N29" s="93" t="s">
+        <v>281</v>
+      </c>
+      <c r="O29" s="90" t="s">
+        <v>282</v>
+      </c>
+      <c r="P29" s="90" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q29" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="R29" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="S29" s="91" t="s">
+        <v>286</v>
+      </c>
+      <c r="T29" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="U29" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="V29" s="96" t="s">
         <v>280</v>
       </c>
-      <c r="M29" s="97" t="s">
+      <c r="W29" s="97" t="s">
         <v>280</v>
-      </c>
-      <c r="N29" s="93" t="s">
-        <v>282</v>
-      </c>
-      <c r="O29" s="90" t="s">
-        <v>283</v>
-      </c>
-      <c r="P29" s="90" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q29" s="91" t="s">
-        <v>285</v>
-      </c>
-      <c r="R29" s="91" t="s">
-        <v>286</v>
-      </c>
-      <c r="S29" s="91" t="s">
-        <v>287</v>
-      </c>
-      <c r="T29" s="91" t="s">
-        <v>288</v>
-      </c>
-      <c r="U29" s="91" t="s">
-        <v>289</v>
-      </c>
-      <c r="V29" s="96" t="s">
-        <v>281</v>
-      </c>
-      <c r="W29" s="97" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="23.25" x14ac:dyDescent="0.25">
@@ -10546,35 +10546,35 @@
         <v>68</v>
       </c>
       <c r="B30" s="68" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C30" s="95" t="str">
         <f>INDEX($E$56:$G$58, MATCH(M30,$E$55:$G$55,0),MATCH(W30,$D$56:$D$58,0))</f>
         <v>Medium</v>
       </c>
       <c r="D30" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E30" s="107" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F30" s="107" t="s">
+        <v>358</v>
+      </c>
+      <c r="G30" s="107" t="s">
         <v>359</v>
       </c>
-      <c r="G30" s="107" t="s">
-        <v>360</v>
-      </c>
       <c r="H30" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I30" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J30" s="107" t="s">
+        <v>363</v>
+      </c>
+      <c r="K30" s="108" t="s">
         <v>364</v>
-      </c>
-      <c r="K30" s="108" t="s">
-        <v>365</v>
       </c>
       <c r="L30" s="100">
         <f t="shared" ref="L30:L32" si="6">(VALUE(LEFT(D30,1))+VALUE(LEFT(E30,1))+VALUE(LEFT(F30,1))+VALUE(LEFT(G30,1))+VALUE(LEFT(H30,1))+VALUE(LEFT(I30,1))+VALUE(LEFT(J30,1))+VALUE(LEFT(K30,1)))/8</f>
@@ -10585,16 +10585,16 @@
         <v>HIGH</v>
       </c>
       <c r="N30" s="106" t="s">
+        <v>365</v>
+      </c>
+      <c r="O30" s="107" t="s">
         <v>366</v>
       </c>
-      <c r="O30" s="107" t="s">
+      <c r="P30" s="107" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q30" s="107" t="s">
         <v>367</v>
-      </c>
-      <c r="P30" s="107" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q30" s="107" t="s">
-        <v>368</v>
       </c>
       <c r="R30" s="92"/>
       <c r="S30" s="92"/>
@@ -10621,28 +10621,28 @@
         <v>High</v>
       </c>
       <c r="D31" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E31" s="107" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F31" s="107" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G31" s="107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H31" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I31" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J31" s="107" t="s">
+        <v>363</v>
+      </c>
+      <c r="K31" s="108" t="s">
         <v>364</v>
-      </c>
-      <c r="K31" s="108" t="s">
-        <v>365</v>
       </c>
       <c r="L31" s="100">
         <f t="shared" si="6"/>
@@ -10653,16 +10653,16 @@
         <v>HIGH</v>
       </c>
       <c r="N31" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O31" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P31" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q31" s="107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R31" s="92"/>
       <c r="S31" s="92"/>
@@ -10689,28 +10689,28 @@
         <v>High</v>
       </c>
       <c r="D32" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E32" s="107" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F32" s="107" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G32" s="107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H32" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I32" s="107" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J32" s="107" t="s">
+        <v>363</v>
+      </c>
+      <c r="K32" s="108" t="s">
         <v>364</v>
-      </c>
-      <c r="K32" s="108" t="s">
-        <v>365</v>
       </c>
       <c r="L32" s="100">
         <f t="shared" si="6"/>
@@ -10721,16 +10721,16 @@
         <v>HIGH</v>
       </c>
       <c r="N32" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O32" s="107" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P32" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q32" s="107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R32" s="92"/>
       <c r="S32" s="92"/>
@@ -10757,28 +10757,28 @@
         <v>High</v>
       </c>
       <c r="D33" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E33" s="107" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F33" s="107" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G33" s="107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H33" s="107" t="s">
+        <v>392</v>
+      </c>
+      <c r="I33" s="107" t="s">
         <v>393</v>
       </c>
-      <c r="I33" s="107" t="s">
+      <c r="J33" s="107" t="s">
         <v>394</v>
       </c>
-      <c r="J33" s="107" t="s">
-        <v>395</v>
-      </c>
       <c r="K33" s="108" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L33" s="100">
         <f t="shared" ref="L33:L49" si="11">(VALUE(LEFT(D33,1))+VALUE(LEFT(E33,1))+VALUE(LEFT(F33,1))+VALUE(LEFT(G33,1))+VALUE(LEFT(H33,1))+VALUE(LEFT(I33,1))+VALUE(LEFT(J33,1))+VALUE(LEFT(K33,1)))/8</f>
@@ -10789,16 +10789,16 @@
         <v>HIGH</v>
       </c>
       <c r="N33" s="106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O33" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P33" s="107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q33" s="107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="92"/>
@@ -10825,28 +10825,28 @@
         <v>High</v>
       </c>
       <c r="D34" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="E34" s="102" t="s">
+        <v>385</v>
+      </c>
+      <c r="F34" s="102" t="s">
+        <v>358</v>
+      </c>
+      <c r="G34" s="102" t="s">
         <v>387</v>
       </c>
-      <c r="E34" s="102" t="s">
-        <v>386</v>
-      </c>
-      <c r="F34" s="102" t="s">
-        <v>359</v>
-      </c>
-      <c r="G34" s="102" t="s">
-        <v>388</v>
-      </c>
       <c r="H34" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I34" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I34" s="102" t="s">
+      <c r="J34" s="102" t="s">
         <v>394</v>
       </c>
-      <c r="J34" s="102" t="s">
-        <v>395</v>
-      </c>
       <c r="K34" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L34" s="104">
         <f t="shared" si="11"/>
@@ -10857,16 +10857,16 @@
         <v>HIGH</v>
       </c>
       <c r="N34" s="101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O34" s="102" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P34" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q34" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R34" s="92"/>
       <c r="S34" s="92"/>
@@ -10893,28 +10893,28 @@
         <v>Medium</v>
       </c>
       <c r="D35" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E35" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F35" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G35" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H35" s="102" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I35" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J35" s="102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K35" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L35" s="104">
         <f t="shared" si="11"/>
@@ -10925,16 +10925,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N35" s="101" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O35" s="102" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P35" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q35" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R35" s="92"/>
       <c r="S35" s="92"/>
@@ -10961,28 +10961,28 @@
         <v>High</v>
       </c>
       <c r="D36" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E36" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F36" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G36" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H36" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I36" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I36" s="102" t="s">
-        <v>394</v>
-      </c>
       <c r="J36" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K36" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K36" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L36" s="104">
         <f t="shared" si="11"/>
@@ -10993,16 +10993,16 @@
         <v>HIGH</v>
       </c>
       <c r="N36" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O36" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P36" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q36" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q36" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R36" s="92"/>
       <c r="S36" s="92"/>
@@ -11029,28 +11029,28 @@
         <v>Critical</v>
       </c>
       <c r="D37" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E37" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F37" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G37" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H37" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I37" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I37" s="102" t="s">
-        <v>394</v>
-      </c>
       <c r="J37" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K37" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K37" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L37" s="104">
         <f t="shared" si="11"/>
@@ -11061,16 +11061,16 @@
         <v>HIGH</v>
       </c>
       <c r="N37" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O37" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P37" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q37" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q37" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R37" s="92"/>
       <c r="S37" s="92"/>
@@ -11097,28 +11097,28 @@
         <v>Medium</v>
       </c>
       <c r="D38" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E38" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F38" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G38" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H38" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I38" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J38" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K38" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L38" s="104">
         <f t="shared" si="11"/>
@@ -11129,16 +11129,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N38" s="101" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="O38" s="102" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P38" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q38" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R38" s="92"/>
       <c r="S38" s="92"/>
@@ -11165,28 +11165,28 @@
         <v>High</v>
       </c>
       <c r="D39" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E39" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F39" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G39" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H39" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I39" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J39" s="102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K39" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L39" s="104">
         <f t="shared" si="11"/>
@@ -11197,16 +11197,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N39" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O39" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P39" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q39" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R39" s="92"/>
       <c r="S39" s="92"/>
@@ -11233,28 +11233,28 @@
         <v>Medium</v>
       </c>
       <c r="D40" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E40" s="102" t="s">
+        <v>356</v>
+      </c>
+      <c r="F40" s="102" t="s">
         <v>357</v>
       </c>
-      <c r="F40" s="102" t="s">
-        <v>358</v>
-      </c>
       <c r="G40" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H40" s="102" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I40" s="102" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J40" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K40" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L40" s="104">
         <f t="shared" si="11"/>
@@ -11265,16 +11265,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N40" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O40" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P40" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q40" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R40" s="92"/>
       <c r="S40" s="92"/>
@@ -11301,28 +11301,28 @@
         <v>High</v>
       </c>
       <c r="D41" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E41" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F41" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G41" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H41" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I41" s="102" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J41" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K41" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K41" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L41" s="104">
         <f t="shared" si="11"/>
@@ -11333,16 +11333,16 @@
         <v>HIGH</v>
       </c>
       <c r="N41" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O41" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P41" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q41" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="92"/>
@@ -11369,28 +11369,28 @@
         <v>Medium</v>
       </c>
       <c r="D42" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E42" s="102" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F42" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G42" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H42" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I42" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J42" s="102" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K42" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L42" s="104">
         <f t="shared" si="11"/>
@@ -11401,19 +11401,19 @@
         <v>HIGH</v>
       </c>
       <c r="N42" s="101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O42" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P42" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q42" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R42" s="102" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S42" s="92"/>
       <c r="T42" s="92"/>
@@ -11439,28 +11439,28 @@
         <v>High</v>
       </c>
       <c r="D43" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E43" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F43" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G43" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H43" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I43" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J43" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K43" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L43" s="104">
         <f t="shared" si="11"/>
@@ -11471,16 +11471,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N43" s="101" t="s">
+        <v>401</v>
+      </c>
+      <c r="O43" s="102" t="s">
+        <v>400</v>
+      </c>
+      <c r="P43" s="102" t="s">
         <v>402</v>
       </c>
-      <c r="O43" s="102" t="s">
-        <v>401</v>
-      </c>
-      <c r="P43" s="102" t="s">
-        <v>403</v>
-      </c>
       <c r="Q43" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R43" s="92"/>
       <c r="S43" s="92"/>
@@ -11507,28 +11507,28 @@
         <v>Medium</v>
       </c>
       <c r="D44" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E44" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F44" s="102" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G44" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H44" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I44" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I44" s="102" t="s">
-        <v>394</v>
-      </c>
       <c r="J44" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="K44" s="103" t="s">
         <v>364</v>
-      </c>
-      <c r="K44" s="103" t="s">
-        <v>365</v>
       </c>
       <c r="L44" s="104">
         <f t="shared" si="11"/>
@@ -11539,19 +11539,19 @@
         <v>HIGH</v>
       </c>
       <c r="N44" s="101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O44" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P44" s="102" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q44" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R44" s="102" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S44" s="92"/>
       <c r="T44" s="92"/>
@@ -11577,28 +11577,28 @@
         <v>High</v>
       </c>
       <c r="D45" s="101" t="s">
+        <v>386</v>
+      </c>
+      <c r="E45" s="102" t="s">
+        <v>356</v>
+      </c>
+      <c r="F45" s="102" t="s">
+        <v>358</v>
+      </c>
+      <c r="G45" s="102" t="s">
         <v>387</v>
       </c>
-      <c r="E45" s="102" t="s">
-        <v>357</v>
-      </c>
-      <c r="F45" s="102" t="s">
-        <v>359</v>
-      </c>
-      <c r="G45" s="102" t="s">
-        <v>388</v>
-      </c>
       <c r="H45" s="102" t="s">
+        <v>392</v>
+      </c>
+      <c r="I45" s="102" t="s">
         <v>393</v>
       </c>
-      <c r="I45" s="102" t="s">
+      <c r="J45" s="102" t="s">
         <v>394</v>
       </c>
-      <c r="J45" s="102" t="s">
-        <v>395</v>
-      </c>
       <c r="K45" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L45" s="104">
         <f t="shared" si="11"/>
@@ -11609,16 +11609,16 @@
         <v>HIGH</v>
       </c>
       <c r="N45" s="101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="O45" s="102" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P45" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q45" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R45" s="92"/>
       <c r="S45" s="92"/>
@@ -11645,28 +11645,28 @@
         <v>High</v>
       </c>
       <c r="D46" s="101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E46" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F46" s="102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G46" s="102" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H46" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I46" s="102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J46" s="102" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K46" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L46" s="104">
         <f t="shared" si="11"/>
@@ -11677,16 +11677,16 @@
         <v>MEDIUM</v>
       </c>
       <c r="N46" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O46" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P46" s="102" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Q46" s="102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R46" s="92"/>
       <c r="S46" s="92"/>
@@ -11713,28 +11713,28 @@
         <v>High</v>
       </c>
       <c r="D47" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E47" s="102" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F47" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G47" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H47" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I47" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J47" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K47" s="103" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L47" s="104">
         <f t="shared" si="11"/>
@@ -11745,16 +11745,16 @@
         <v>HIGH</v>
       </c>
       <c r="N47" s="101" t="s">
+        <v>397</v>
+      </c>
+      <c r="O47" s="102" t="s">
         <v>398</v>
       </c>
-      <c r="O47" s="102" t="s">
-        <v>399</v>
-      </c>
       <c r="P47" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q47" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q47" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R47" s="92"/>
       <c r="S47" s="92"/>
@@ -11781,28 +11781,28 @@
         <v>Critical</v>
       </c>
       <c r="D48" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E48" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F48" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G48" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H48" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I48" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J48" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K48" s="103" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L48" s="104">
         <f t="shared" si="11"/>
@@ -11813,16 +11813,16 @@
         <v>HIGH</v>
       </c>
       <c r="N48" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O48" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P48" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q48" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q48" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R48" s="92"/>
       <c r="S48" s="92"/>
@@ -11849,28 +11849,28 @@
         <v>Critical</v>
       </c>
       <c r="D49" s="101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E49" s="102" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F49" s="102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G49" s="102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H49" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I49" s="102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J49" s="102" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K49" s="103" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L49" s="104">
         <f t="shared" si="11"/>
@@ -11881,16 +11881,16 @@
         <v>HIGH</v>
       </c>
       <c r="N49" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="O49" s="102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P49" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q49" s="102" t="s">
         <v>367</v>
-      </c>
-      <c r="Q49" s="102" t="s">
-        <v>368</v>
       </c>
       <c r="R49" s="92"/>
       <c r="S49" s="92"/>
@@ -11907,19 +11907,19 @@
     </row>
     <row r="52" spans="1:23" ht="21" x14ac:dyDescent="0.35">
       <c r="C52" s="69" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="53" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="131" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D53" s="132"/>
       <c r="E53" s="133"/>
       <c r="F53" s="133"/>
       <c r="G53" s="134"/>
       <c r="I53" s="135" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J53" s="134"/>
     </row>
@@ -11927,34 +11927,34 @@
       <c r="C54" s="120"/>
       <c r="D54" s="121"/>
       <c r="E54" s="124" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F54" s="124"/>
       <c r="G54" s="125"/>
       <c r="I54" s="78" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J54" s="83" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="122"/>
       <c r="D55" s="123"/>
       <c r="E55" s="89" t="s">
+        <v>377</v>
+      </c>
+      <c r="F55" s="88" t="s">
         <v>378</v>
       </c>
-      <c r="F55" s="88" t="s">
-        <v>379</v>
-      </c>
       <c r="G55" s="78" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I55" s="78" t="s">
+        <v>376</v>
+      </c>
+      <c r="J55" s="82" t="s">
         <v>377</v>
-      </c>
-      <c r="J55" s="82" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11962,57 +11962,57 @@
         <v>4</v>
       </c>
       <c r="D56" s="78" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E56" s="85" t="s">
+        <v>381</v>
+      </c>
+      <c r="F56" s="86" t="s">
+        <v>379</v>
+      </c>
+      <c r="G56" s="87" t="s">
+        <v>373</v>
+      </c>
+      <c r="I56" s="78" t="s">
         <v>382</v>
       </c>
-      <c r="F56" s="86" t="s">
-        <v>380</v>
-      </c>
-      <c r="G56" s="87" t="s">
-        <v>374</v>
-      </c>
-      <c r="I56" s="78" t="s">
-        <v>383</v>
-      </c>
       <c r="J56" s="80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C57" s="126"/>
       <c r="D57" s="78" t="s">
+        <v>378</v>
+      </c>
+      <c r="E57" s="83" t="s">
         <v>379</v>
       </c>
-      <c r="E57" s="83" t="s">
-        <v>380</v>
-      </c>
       <c r="F57" s="84" t="s">
+        <v>373</v>
+      </c>
+      <c r="G57" s="80" t="s">
         <v>374</v>
-      </c>
-      <c r="G57" s="80" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C58" s="127"/>
       <c r="D58" s="88" t="s">
+        <v>372</v>
+      </c>
+      <c r="E58" s="79" t="s">
         <v>373</v>
       </c>
-      <c r="E58" s="79" t="s">
+      <c r="F58" s="80" t="s">
         <v>374</v>
       </c>
-      <c r="F58" s="80" t="s">
+      <c r="G58" s="81" t="s">
         <v>375</v>
-      </c>
-      <c r="G58" s="81" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -12161,52 +12161,52 @@
     <row r="1" spans="1:17" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70"/>
       <c r="B1" s="70" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C1" s="70" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="70" t="s">
         <v>272</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="E1" s="70" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="F1" s="70" t="s">
         <v>274</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="G1" s="70" t="s">
         <v>275</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="H1" s="70" t="s">
         <v>276</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="I1" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="I1" s="70" t="s">
-        <v>278</v>
-      </c>
       <c r="J1" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" s="70" t="s">
         <v>282</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="L1" s="70" t="s">
         <v>283</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="M1" s="70" t="s">
         <v>284</v>
       </c>
-      <c r="M1" s="70" t="s">
+      <c r="N1" s="70" t="s">
         <v>285</v>
       </c>
-      <c r="N1" s="70" t="s">
+      <c r="O1" s="70" t="s">
         <v>286</v>
       </c>
-      <c r="O1" s="70" t="s">
+      <c r="P1" s="70" t="s">
         <v>287</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="Q1" s="70" t="s">
         <v>288</v>
-      </c>
-      <c r="Q1" s="70" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="74" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
@@ -12216,7 +12216,7 @@
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
       <c r="D2" s="73" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E2" s="73"/>
       <c r="F2" s="73"/>
@@ -12238,40 +12238,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="73" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="73" t="s">
         <v>294</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>295</v>
       </c>
       <c r="D3" s="73"/>
       <c r="E3" s="73"/>
       <c r="F3" s="73" t="s">
+        <v>295</v>
+      </c>
+      <c r="G3" s="73" t="s">
         <v>296</v>
       </c>
-      <c r="G3" s="73" t="s">
+      <c r="H3" s="73" t="s">
         <v>297</v>
       </c>
-      <c r="H3" s="73" t="s">
+      <c r="I3" s="73" t="s">
         <v>298</v>
-      </c>
-      <c r="I3" s="73" t="s">
-        <v>299</v>
       </c>
       <c r="J3" s="73"/>
       <c r="K3" s="73" t="s">
+        <v>299</v>
+      </c>
+      <c r="L3" s="73" t="s">
         <v>300</v>
       </c>
-      <c r="L3" s="73" t="s">
+      <c r="M3" s="73" t="s">
         <v>301</v>
       </c>
-      <c r="M3" s="73" t="s">
+      <c r="N3" s="73" t="s">
         <v>302</v>
       </c>
-      <c r="N3" s="73" t="s">
+      <c r="O3" s="73" t="s">
         <v>303</v>
-      </c>
-      <c r="O3" s="73" t="s">
-        <v>304</v>
       </c>
       <c r="P3" s="73"/>
       <c r="Q3" s="73"/>
@@ -12285,14 +12285,14 @@
       <c r="C4" s="73"/>
       <c r="D4" s="73"/>
       <c r="E4" s="73" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F4" s="73"/>
       <c r="G4" s="73"/>
       <c r="H4" s="73"/>
       <c r="I4" s="73"/>
       <c r="J4" s="73" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
@@ -12300,7 +12300,7 @@
       <c r="N4" s="73"/>
       <c r="O4" s="73"/>
       <c r="P4" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q4" s="73"/>
     </row>
@@ -12310,34 +12310,34 @@
         <v>3</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C5" s="73"/>
       <c r="D5" s="73"/>
       <c r="E5" s="73"/>
       <c r="F5" s="73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G5" s="73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H5" s="73"/>
       <c r="I5" s="73" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J5" s="73"/>
       <c r="K5" s="73" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L5" s="73"/>
       <c r="M5" s="73"/>
       <c r="N5" s="73" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O5" s="73"/>
       <c r="P5" s="73"/>
       <c r="Q5" s="73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="74" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
@@ -12347,29 +12347,29 @@
       </c>
       <c r="B6" s="73"/>
       <c r="C6" s="73" t="s">
+        <v>313</v>
+      </c>
+      <c r="D6" s="73" t="s">
         <v>314</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="E6" s="73" t="s">
         <v>315</v>
-      </c>
-      <c r="E6" s="73" t="s">
-        <v>316</v>
       </c>
       <c r="F6" s="73"/>
       <c r="G6" s="73"/>
       <c r="H6" s="73" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I6" s="73"/>
       <c r="J6" s="73" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
       <c r="M6" s="73"/>
       <c r="N6" s="73"/>
       <c r="O6" s="73" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P6" s="73"/>
       <c r="Q6" s="73"/>
@@ -12380,38 +12380,38 @@
         <v>5</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C7" s="73"/>
       <c r="D7" s="73"/>
       <c r="E7" s="73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F7" s="73"/>
       <c r="G7" s="73" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H7" s="73"/>
       <c r="I7" s="73"/>
       <c r="J7" s="73" t="s">
+        <v>322</v>
+      </c>
+      <c r="K7" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="K7" s="73" t="s">
+      <c r="L7" s="73" t="s">
         <v>324</v>
-      </c>
-      <c r="L7" s="73" t="s">
-        <v>325</v>
       </c>
       <c r="M7" s="73"/>
       <c r="N7" s="73"/>
       <c r="O7" s="73" t="s">
+        <v>325</v>
+      </c>
+      <c r="P7" s="73" t="s">
         <v>326</v>
       </c>
-      <c r="P7" s="73" t="s">
+      <c r="Q7" s="73" t="s">
         <v>327</v>
-      </c>
-      <c r="Q7" s="73" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="74" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
@@ -12420,17 +12420,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="73" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8" s="73"/>
       <c r="D8" s="73"/>
       <c r="E8" s="73" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="73"/>
       <c r="H8" s="73" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I8" s="73"/>
       <c r="J8" s="73"/>
@@ -12450,34 +12450,34 @@
       <c r="B9" s="73"/>
       <c r="C9" s="73"/>
       <c r="D9" s="73" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E9" s="73"/>
       <c r="F9" s="73" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G9" s="73"/>
       <c r="H9" s="73"/>
       <c r="I9" s="73"/>
       <c r="J9" s="73"/>
       <c r="K9" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="L9" s="73" t="s">
         <v>333</v>
       </c>
-      <c r="L9" s="73" t="s">
+      <c r="M9" s="73" t="s">
         <v>334</v>
       </c>
-      <c r="M9" s="73" t="s">
+      <c r="N9" s="73" t="s">
         <v>335</v>
-      </c>
-      <c r="N9" s="73" t="s">
-        <v>336</v>
       </c>
       <c r="O9" s="73"/>
       <c r="P9" s="73" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q9" s="73" t="s">
         <v>337</v>
-      </c>
-      <c r="Q9" s="73" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="74" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
@@ -12493,7 +12493,7 @@
       <c r="G10" s="73"/>
       <c r="H10" s="73"/>
       <c r="I10" s="73" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
@@ -12510,50 +12510,50 @@
         <v>9</v>
       </c>
       <c r="B11" s="73" t="s">
+        <v>339</v>
+      </c>
+      <c r="C11" s="73" t="s">
         <v>340</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="D11" s="73" t="s">
         <v>341</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="E11" s="73" t="s">
         <v>342</v>
       </c>
-      <c r="E11" s="73" t="s">
+      <c r="F11" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="G11" s="73" t="s">
+        <v>343</v>
+      </c>
+      <c r="H11" s="73" t="s">
         <v>344</v>
       </c>
-      <c r="G11" s="73" t="s">
-        <v>344</v>
-      </c>
-      <c r="H11" s="73" t="s">
+      <c r="I11" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="I11" s="73" t="s">
+      <c r="J11" s="73" t="s">
         <v>346</v>
       </c>
-      <c r="J11" s="73" t="s">
+      <c r="K11" s="73" t="s">
         <v>347</v>
       </c>
-      <c r="K11" s="73" t="s">
+      <c r="L11" s="73" t="s">
         <v>348</v>
       </c>
-      <c r="L11" s="73" t="s">
+      <c r="M11" s="73" t="s">
         <v>349</v>
       </c>
-      <c r="M11" s="73" t="s">
+      <c r="N11" s="73" t="s">
         <v>350</v>
       </c>
-      <c r="N11" s="73" t="s">
+      <c r="O11" s="73" t="s">
         <v>351</v>
-      </c>
-      <c r="O11" s="73" t="s">
-        <v>352</v>
       </c>
       <c r="P11" s="73"/>
       <c r="Q11" s="73" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="74" customFormat="1" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12587,7 +12587,7 @@
     </row>
     <row r="14" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B14" s="74"/>
       <c r="C14" s="74"/>
@@ -13276,72 +13276,72 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed vectors and propagated change everywhere, tried formatting tables
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="481">
   <si>
     <t>supply compromised container (base) image</t>
   </si>
@@ -1528,24 +1528,12 @@
     <t>Only when the stars align just right = Theoretical</t>
   </si>
   <si>
-    <t>Read confidentials through Kubernetes &amp; platform control plane interfaces</t>
-  </si>
-  <si>
     <t>Gather confidential information through the Kubernetes dashboard &amp; apiserver as well as potential platform webinterfaces &amp; apiserver(s)</t>
   </si>
   <si>
-    <t>Change configuration through Kubernetes &amp; platform control plane interfaces</t>
-  </si>
-  <si>
     <t>Change the existing configuration through the Kubernetes dashboard &amp; apiserver as well as potential platform webinterfaces &amp; apiserver(s)</t>
   </si>
   <si>
-    <t>Hoard resources (sabotage)</t>
-  </si>
-  <si>
-    <t>Misuse resources (cryptojacking)</t>
-  </si>
-  <si>
     <t>The provided resources may be misconfigured or misused to disrupt service availability (i.e. through fork bombing or misconfiguration)</t>
   </si>
   <si>
@@ -1568,6 +1556,57 @@
   </si>
   <si>
     <t>follow additional tips by supplier</t>
+  </si>
+  <si>
+    <t>Reconaissance through interface components</t>
+  </si>
+  <si>
+    <t>Reading confidentials through interface components</t>
+  </si>
+  <si>
+    <t>Configuration manipulation through interface components</t>
+  </si>
+  <si>
+    <t>Compromise internal master components</t>
+  </si>
+  <si>
+    <t>Image poisoning and baiting</t>
+  </si>
+  <si>
+    <t>Configuration poisoning and baiting</t>
+  </si>
+  <si>
+    <t>Lateral movement through cluster</t>
+  </si>
+  <si>
+    <t>Container breakout</t>
+  </si>
+  <si>
+    <t>Image cache compromise</t>
+  </si>
+  <si>
+    <t>Container modification at runtime</t>
+  </si>
+  <si>
+    <t>Resource hoarding (sabotage)</t>
+  </si>
+  <si>
+    <t>Resource misuse (cryptojacking)</t>
+  </si>
+  <si>
+    <t>Adding rogue containers</t>
+  </si>
+  <si>
+    <t>Adding rogue nodes</t>
+  </si>
+  <si>
+    <t>Leveraging bad user practice</t>
+  </si>
+  <si>
+    <t>Leveraging bad infrastructure</t>
+  </si>
+  <si>
+    <t>Leveraging bad patch management</t>
   </si>
 </sst>
 </file>
@@ -2944,8 +2983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,7 +3024,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>440</v>
+        <v>464</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>108</v>
@@ -2999,11 +3038,11 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3011,11 +3050,11 @@
         <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3023,7 +3062,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>425</v>
+        <v>467</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
@@ -3035,7 +3074,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>427</v>
+        <v>468</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -3047,7 +3086,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
@@ -3059,7 +3098,7 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
@@ -3071,7 +3110,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>429</v>
+        <v>471</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
@@ -3083,7 +3122,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>430</v>
+        <v>472</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
@@ -3095,7 +3134,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>431</v>
+        <v>473</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
@@ -3107,11 +3146,11 @@
         <v>78</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3119,11 +3158,11 @@
         <v>79</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,7 +3170,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>435</v>
+        <v>476</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
@@ -3143,7 +3182,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>436</v>
+        <v>477</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
@@ -3155,7 +3194,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>51</v>
+        <v>478</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
@@ -3167,7 +3206,7 @@
         <v>83</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>50</v>
+        <v>479</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
@@ -3179,7 +3218,7 @@
         <v>84</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="35" t="s">
@@ -3188,6 +3227,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3198,8 +3238,8 @@
   </sheetPr>
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,7 +3282,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>9</v>
@@ -3298,7 +3338,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>440</v>
+        <v>464</v>
       </c>
       <c r="C4" s="110">
         <v>3</v>
@@ -3356,7 +3396,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -3414,7 +3454,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="C6" s="10">
         <v>3</v>
@@ -3472,7 +3512,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>425</v>
+        <v>467</v>
       </c>
       <c r="C7" s="10">
         <v>3</v>
@@ -3530,7 +3570,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>427</v>
+        <v>468</v>
       </c>
       <c r="C8" s="10">
         <v>4</v>
@@ -3588,7 +3628,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
       <c r="C9" s="10">
         <v>4</v>
@@ -3646,7 +3686,7 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="C10" s="10">
         <v>2</v>
@@ -3704,7 +3744,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>429</v>
+        <v>471</v>
       </c>
       <c r="C11" s="23">
         <v>2</v>
@@ -3762,7 +3802,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>430</v>
+        <v>472</v>
       </c>
       <c r="C12" s="10">
         <v>1</v>
@@ -3820,7 +3860,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>431</v>
+        <v>473</v>
       </c>
       <c r="C13" s="23">
         <v>2</v>
@@ -3878,7 +3918,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="C14" s="23">
         <v>3</v>
@@ -3936,7 +3976,7 @@
         <v>79</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="C15" s="23">
         <v>3</v>
@@ -3994,7 +4034,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>435</v>
+        <v>476</v>
       </c>
       <c r="C16" s="23">
         <v>3</v>
@@ -4052,7 +4092,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>436</v>
+        <v>477</v>
       </c>
       <c r="C17" s="23">
         <v>3</v>
@@ -4110,7 +4150,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>51</v>
+        <v>478</v>
       </c>
       <c r="C18" s="23">
         <v>3</v>
@@ -4168,7 +4208,7 @@
         <v>83</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>50</v>
+        <v>479</v>
       </c>
       <c r="C19" s="23">
         <v>4</v>
@@ -4226,7 +4266,7 @@
         <v>84</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="C20" s="39">
         <v>4</v>
@@ -4295,7 +4335,7 @@
     </row>
     <row r="24" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -4310,7 +4350,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B26" s="33" t="s">
         <v>9</v>
@@ -4343,7 +4383,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>440</v>
+        <v>464</v>
       </c>
       <c r="C27" s="41">
         <v>4</v>
@@ -4375,7 +4415,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C28" s="41">
         <v>4</v>
@@ -4407,7 +4447,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="C29" s="41">
         <v>4</v>
@@ -4439,7 +4479,7 @@
         <v>71</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>425</v>
+        <v>467</v>
       </c>
       <c r="C30" s="41">
         <v>4</v>
@@ -4471,7 +4511,7 @@
         <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>427</v>
+        <v>468</v>
       </c>
       <c r="C31" s="41">
         <v>4</v>
@@ -4503,7 +4543,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
       <c r="C32" s="41">
         <v>4</v>
@@ -4535,7 +4575,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
@@ -4567,7 +4607,7 @@
         <v>75</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>429</v>
+        <v>471</v>
       </c>
       <c r="C34" s="23">
         <v>2</v>
@@ -4599,7 +4639,7 @@
         <v>76</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>430</v>
+        <v>472</v>
       </c>
       <c r="C35" s="10">
         <v>1</v>
@@ -4631,7 +4671,7 @@
         <v>77</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>431</v>
+        <v>473</v>
       </c>
       <c r="C36" s="38">
         <v>2</v>
@@ -4663,7 +4703,7 @@
         <v>78</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="C37" s="38">
         <v>3</v>
@@ -4695,7 +4735,7 @@
         <v>79</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="C38" s="38">
         <v>3</v>
@@ -4727,7 +4767,7 @@
         <v>80</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>435</v>
+        <v>476</v>
       </c>
       <c r="C39" s="38">
         <v>4</v>
@@ -4759,7 +4799,7 @@
         <v>81</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>436</v>
+        <v>477</v>
       </c>
       <c r="C40" s="38">
         <v>4</v>
@@ -4791,7 +4831,7 @@
         <v>82</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>51</v>
+        <v>478</v>
       </c>
       <c r="C41" s="38">
         <v>4</v>
@@ -4823,7 +4863,7 @@
         <v>83</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>50</v>
+        <v>479</v>
       </c>
       <c r="C42" s="38">
         <v>4</v>
@@ -4855,7 +4895,7 @@
         <v>84</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="C43" s="40">
         <v>4</v>
@@ -4884,7 +4924,7 @@
     </row>
     <row r="46" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B46" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4896,16 +4936,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B48" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D48" s="47" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4913,7 +4953,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>440</v>
+        <v>464</v>
       </c>
       <c r="C49" s="48">
         <v>3</v>
@@ -4927,7 +4967,7 @@
         <v>69</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C50" s="48">
         <v>6</v>
@@ -4941,7 +4981,7 @@
         <v>70</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="C51" s="48">
         <v>7</v>
@@ -4955,7 +4995,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>425</v>
+        <v>467</v>
       </c>
       <c r="C52" s="48">
         <v>5</v>
@@ -4969,7 +5009,7 @@
         <v>72</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>427</v>
+        <v>468</v>
       </c>
       <c r="C53" s="48">
         <v>7</v>
@@ -4983,7 +5023,7 @@
         <v>73</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
       <c r="C54" s="48">
         <v>10</v>
@@ -4997,7 +5037,7 @@
         <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="C55" s="48">
         <v>7</v>
@@ -5011,7 +5051,7 @@
         <v>75</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>429</v>
+        <v>471</v>
       </c>
       <c r="C56" s="48">
         <v>5</v>
@@ -5025,7 +5065,7 @@
         <v>76</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>430</v>
+        <v>472</v>
       </c>
       <c r="C57" s="48">
         <v>3</v>
@@ -5039,7 +5079,7 @@
         <v>77</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>431</v>
+        <v>473</v>
       </c>
       <c r="C58" s="48">
         <v>5</v>
@@ -5053,7 +5093,7 @@
         <v>78</v>
       </c>
       <c r="B59" s="51" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="C59" s="48">
         <v>8</v>
@@ -5067,7 +5107,7 @@
         <v>79</v>
       </c>
       <c r="B60" s="51" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="C60" s="48">
         <v>5</v>
@@ -5081,7 +5121,7 @@
         <v>80</v>
       </c>
       <c r="B61" s="51" t="s">
-        <v>435</v>
+        <v>476</v>
       </c>
       <c r="C61" s="48">
         <v>5</v>
@@ -5095,7 +5135,7 @@
         <v>81</v>
       </c>
       <c r="B62" s="51" t="s">
-        <v>436</v>
+        <v>477</v>
       </c>
       <c r="C62" s="48">
         <v>6</v>
@@ -5109,7 +5149,7 @@
         <v>82</v>
       </c>
       <c r="B63" s="51" t="s">
-        <v>51</v>
+        <v>478</v>
       </c>
       <c r="C63" s="48">
         <v>6</v>
@@ -5123,7 +5163,7 @@
         <v>83</v>
       </c>
       <c r="B64" s="51" t="s">
-        <v>50</v>
+        <v>479</v>
       </c>
       <c r="C64" s="48">
         <v>9</v>
@@ -5137,7 +5177,7 @@
         <v>84</v>
       </c>
       <c r="B65" s="53" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="C65" s="49">
         <v>10</v>
@@ -5505,7 +5545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
@@ -6109,7 +6149,7 @@
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="61"/>
       <c r="B111" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
wrote out vectors until v10
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -63,7 +63,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0">
@@ -76,7 +76,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -2611,9 +2611,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -2719,7 +2719,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2983,11 +2983,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" customWidth="1"/>
@@ -3242,7 +3242,7 @@
       <selection activeCell="B49" sqref="B49:B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -5304,7 +5304,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
@@ -5545,11 +5545,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
@@ -6224,7 +6224,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
@@ -6750,7 +6750,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -8969,7 +8969,7 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" customWidth="1"/>
@@ -12189,7 +12189,7 @@
       <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="77"/>
     <col min="2" max="4" width="17.28515625" style="77" customWidth="1"/>
@@ -13312,7 +13312,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
started write-out of estimation procedure and approach, end of day commit
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -63,7 +63,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0">
@@ -76,7 +76,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -2611,9 +2611,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -2719,7 +2719,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2987,7 +2987,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" customWidth="1"/>
@@ -3238,11 +3238,11 @@
   </sheetPr>
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:B65"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -5304,7 +5304,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
@@ -5545,11 +5545,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
@@ -6224,7 +6224,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
@@ -6746,11 +6746,11 @@
   </sheetPr>
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -8965,11 +8965,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" customWidth="1"/>
@@ -12189,7 +12189,7 @@
       <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="77"/>
     <col min="2" max="4" width="17.28515625" style="77" customWidth="1"/>
@@ -13312,7 +13312,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
indermediate commit, switching workstation
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -3247,8 +3247,8 @@
   </sheetPr>
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3930,7 +3930,7 @@
         <v>473</v>
       </c>
       <c r="C14" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="41">
         <v>2</v>
@@ -3943,17 +3943,17 @@
       </c>
       <c r="G14" s="23">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="H14" s="4">
         <v>3</v>
       </c>
       <c r="I14" s="48">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J14" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K14" s="41">
         <v>2</v>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="N14" s="23">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="O14" s="38">
         <v>2</v>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -5309,8 +5309,8 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
wrote out vector assess up to v12
</commit_message>
<xml_diff>
--- a/Attack_Vector_2.xlsx
+++ b/Attack_Vector_2.xlsx
@@ -63,7 +63,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0">
@@ -76,7 +76,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -2620,9 +2620,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -2728,7 +2728,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2996,7 +2996,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" customWidth="1"/>
@@ -3248,10 +3248,10 @@
   <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -3930,7 +3930,7 @@
         <v>473</v>
       </c>
       <c r="C14" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="41">
         <v>2</v>
@@ -3943,17 +3943,17 @@
       </c>
       <c r="G14" s="23">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="H14" s="4">
         <v>3</v>
       </c>
       <c r="I14" s="48">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J14" s="38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K14" s="41">
         <v>2</v>
@@ -3966,14 +3966,14 @@
       </c>
       <c r="N14" s="23">
         <f t="shared" si="4"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="O14" s="38">
         <v>2</v>
       </c>
       <c r="P14" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
@@ -4011,7 +4011,7 @@
         <v>5</v>
       </c>
       <c r="J15" s="38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15" s="41">
         <v>2</v>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="N15" s="23">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="O15" s="38">
         <v>3</v>
@@ -5313,7 +5313,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
@@ -5558,7 +5558,7 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
@@ -6233,7 +6233,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
@@ -6759,7 +6759,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -8978,7 +8978,7 @@
       <selection activeCell="N5" sqref="N5:Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" customWidth="1"/>
@@ -12198,7 +12198,7 @@
       <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="77"/>
     <col min="2" max="4" width="17.28515625" style="77" customWidth="1"/>
@@ -13321,7 +13321,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">

</xml_diff>